<commit_message>
Evaluation with inference setup
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -423,14 +423,80 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LLaMA-7b</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LLaMA-2-70b</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LLaMA-2-7b-chat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>I/O falsch</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>guanaco-7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Alpaca</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>alpaca-7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Alpaca ohne Modulenamen im Kontext</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>alpaca-2-70b</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Alpaca refined</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>alpaca-2-7b-chat</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -441,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,32 +518,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>hallucination</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>specific</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>balanfac</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>icastedt</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>billofma</t>
+          <t>General</t>
         </is>
       </c>
     </row>
@@ -489,22 +530,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>This is the context of the module billofma: feeding guinea pigs and groundhogs. Which module describes feeding mammals?</t>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>With this module, the annual and period balances of a general ledger or personal account posted in financial accounting are displayed. Which module is being described?</t>
+          <t>test</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Which module deals with creating and deleting parts or service-role relationships?</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Which module describes the composition of a production part?</t>
+          <t>test</t>
         </is>
       </c>
     </row>
@@ -516,12 +557,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This is the description of the module billofma: Feeding guinea pigs and groundhogs. Which module describes Donald Trump's presidency?</t>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Which module is used to display the annual and period balances of a general ledger?</t>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
@@ -531,9 +582,24 @@
           <t>In what module do I edit the name of a customer?</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>What is the module to list annual balances of general ledger?</t>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
@@ -541,6 +607,250 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>What is the module for entering sales invoices?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Hallucination</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>This is the context of the module billofma: feeding guinea pigs and groundhogs. Which module describes feeding mammals?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>This is the description of the module billofma: Feeding guinea pigs and groundhogs. Which module describes Donald Trump's presidency?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Specific</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>balanfac</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>With this module, the annual and period balances of a general ledger or personal account posted in financial accounting are displayed. Which module is being described?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Which module is used to display the annual and period balances of a general ledger?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>What is the module to list annual balances of general ledger?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>icastedt</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Which module deals with creating and deleting parts or service-role relationships?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>billofma</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Which module describes the composition of a production part?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code and excel file for evaluation of new adapter models
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -69,7 +69,7 @@
 ###Response###: The purpose of the module &lt;Modulename&gt; is &lt;Module Description&gt;.]</t>
   </si>
   <si>
-    <t>The main goal is for the model to answer correct module names based on descriptions, supported by the first data format. The second data format is give the model an understanding of appsWH.</t>
+    <t>The main goal is for the model to answer correct module names based on descriptions, supported by the first data format. The second data format is to give the model an understanding of appsWH.</t>
   </si>
   <si>
     <t>Alpaca</t>
@@ -90,7 +90,7 @@
     <t>The previous data format put all data in the output, causing the model to recursively generate Context and Instruction tags. This data format is the same as the previous one, but only the response is in the output.</t>
   </si>
   <si>
-    <t>Alpaca ohne Modulenamen im Kontext</t>
+    <t>Alpaca ohne Modulnamen im Kontext</t>
   </si>
   <si>
     <t>1. [Below is an instruction that describes a task, paired with an input that provides further context. Write a response that appropriately completes the request.
@@ -126,6 +126,30 @@
     <t>The previous data format used the Context tag. In order to finetune the already instruction tuned LLaMA-2-chat model, the Input tag is used instead. This data format is the same as the previous one, but the Context tag is replaced with Input.</t>
   </si>
   <si>
+    <t>Alpaca ohne Modulnamen im Kontext (de)</t>
+  </si>
+  <si>
+    <t>1. [Unten ist eine Anweisung, die eine Aufgabe beschreibt, gepaart mit einer Eingabe, die weitere Kontextinformationen liefert. Schreiben Sie eine Antwort, die die Anfrage angemessen vervollständigt.
+### Anweisung:
+Wie heißt dieses Modul?
+### Kontext:
+&lt;Module Description&gt;
+### Antwort:], [Der Name des Moduls ist &lt;Modulename&gt;.]
+2. [Unten ist eine Anweisung, die eine Aufgabe beschreibt. Schreiben Sie eine Antwort, die die Anfrage angemessen vervollständigt.
+### Anweisung:
+Was ist der Zweck des Moduls &lt;Modulename&gt;?
+### Antwort:], [Der Zweck des Moduls &lt;Modulename&gt; ist &lt;Module Description&gt;.]</t>
+  </si>
+  <si>
+    <t>Test LLaMA-7b's multilingualism.</t>
+  </si>
+  <si>
+    <t>Alpaca ohne Modulnamen im Kontext (extratokens)</t>
+  </si>
+  <si>
+    <t>See if adding module names to the token vocabulary produces more accurate module names.</t>
+  </si>
+  <si>
     <t>General</t>
   </si>
   <si>
@@ -141,96 +165,130 @@
     <t>chat-7b</t>
   </si>
   <si>
+    <t>alpaca-7b-en</t>
+  </si>
+  <si>
+    <t>alpaca-7b-de</t>
+  </si>
+  <si>
+    <t>alpaca-7b-extratokens</t>
+  </si>
+  <si>
     <t>What is a module?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  A module is a unit of the CyberEnterprise® enterprise model used for safe and efficient processing of transactions. Other models (e.g. process models) also use a structure of modules, but the modules of a process model are called up in the order they appear in the process model. The modules of a cyber-physical system (e.g. an industrial plant), on the other hand, can be called up in any order at all. As a rule, only the modules of a process that actually take place in the real world are called up in the order they occur in the process. The modules that only represent a process (e.g. an accounting or a quality assurance process) are not called up in this order. The modules of a cyber-physical system are called up in the order they are defined in the system.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  A module is a collection of related objects. The objects in a module are said to be managed by the module. Each object can have many different names, which is why objects are described by their classes. The class is also used to distinguish between objects with the same name: differing parameters, for example. In addition to objects and classes, the term attributes is also used to describe the properties of objects.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  A module is a coherent set of functionality. A module can be active or inactive. An active module can be changed by adding/changing business processes or by adding/changing the functionality of the module. A module is implemented as a project. The name of the module is always the name of the project. A module can be created from a template project or from an existing project. The functionality of a module is described by its business processes. A module can be active or inactive. An active module can be changed by adding/changing business processes or by adding/changing the functionality of the module. A module is implemented as a project. The name of the module is always the name of the project. A module can be created from a template project or from an existing project. The functionality of a module is described by its business processes.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  A module is a collection of programs and data that forms a self-contained system. In the ClassiX® system, modules are used to organize the program code and make it easier to maintain and extend it. In general, modules are used for the following: Separation of the program code into individual modules. Each module performs a specific task. Testing of the modules Testing of the modules is carried out using test modules. Only modules that have been marked as a test module can be executed when the system is tested. Any module can be marked as a test module by simply assigning it to the test module class. Examples of modules In ClassiX®, the following modules are available for various tasks: Module Description This module displays all objects stored in the system. The module is used for testing and can be run as a test module. SystemModule This module displays all modules stored in the system. This module is also used for testing and can be run as a test module. ClassiX® comes with various sample modules. These modules can be used as a model for creating new modules and can be modified and extended by the user. Input of user data In ClassiX®, user data is stored in objects. This makes it possible to change the data of a user in one place and have the change take effect in all modules in which the user is created. Bound modules A module whose value is bound to an object is called a bound module. A bound module always has a name that ends with ".bound". This binding to objects takes place via an object that is stored in the system (an object of the class bind). This module is used to create a binding between an object and a module. A module whose value is not bound to an object is called a free module. A free module of this type always has a name that ends with ".free". A free module can be created by simply adding the appropriate class to a module. Test of a module Once a module has been marked as a test module, it can be executed. The test runs are carried out in a separate environment, i.e. the test runner only recognises a module and its submodules that are created in this environment and which are required for the test run. ClassiX® comes with a test system that can be used to test modules. The test system has an environment in which only modules and their submodules created there are present. This environment is required to carry out a test run. The test system can be
-</t>
+    <t>A module is a unit of the CyberEnterprise® enterprise model used for safe and efficient processing of transactions. Other models (e.g. process models) also use a structure of modules, but the modules of a process model are called up in the order they appear in the process model. The modules of a cyber-physical system (e.g. an industrial plant), on the other hand, can be called up in any order at all. As a rule, only the modules of a process that actually take place in the real world are called up in the order they occur in the process. The modules that only represent a process (e.g. an accounting or a quality assurance process) are not called up in this order. The modules of a cyber-physical system are called up in the order they are defined in the system.</t>
+  </si>
+  <si>
+    <t>A module is a collection of related objects. The objects in a module are said to be managed by the module. Each object can have many different names, which is why objects are described by their classes. The class is also used to distinguish between objects with the same name: differing parameters, for example. In addition to objects and classes, the term attributes is also used to describe the properties of objects.</t>
+  </si>
+  <si>
+    <t>A module is a coherent set of functionality. A module can be active or inactive. An active module can be changed by adding/changing business processes or by adding/changing the functionality of the module. A module is implemented as a project. The name of the module is always the name of the project. A module can be created from a template project or from an existing project. The functionality of a module is described by its business processes. A module can be active or inactive. An active module can be changed by adding/changing business processes or by adding/changing the functionality of the module. A module is implemented as a project. The name of the module is always the name of the project. A module can be created from a template project or from an existing project. The functionality of a module is described by its business processes.</t>
+  </si>
+  <si>
+    <t>A module is a collection of programs and data that forms a self-contained system. In the ClassiX® system, modules are used to organize the program code and make it easier to maintain and extend it. In general, modules are used for the following: Separation of the program code into individual modules. Each module performs a specific task. Testing of the modules Testing of the modules is carried out using test modules. Only modules that have been marked as a test module can be executed when the system is tested. Any module can be marked as a test module by simply assigning it to the test module class. Examples of modules In ClassiX®, the following modules are available for various tasks: Module Description This module displays all objects stored in the system. The module is used for testing and can be run as a test module. SystemModule This module displays all modules stored in the system. This module is also used for testing and can be run as a test module. ClassiX® comes with various sample modules. These modules can be used as a model for creating new modules and can be modified and extended by the user. Input of user data In ClassiX®, user data is stored in objects. This makes it possible to change the data of a user in one place and have the change take effect in all modules in which the user is created. Bound modules A module whose value is bound to an object is called a bound module. A bound module always has a name that ends with ".bound". This binding to objects takes place via an object that is stored in the system (an object of the class bind). This module is used to create a binding between an object and a module. A module whose value is not bound to an object is called a free module. A free module of this type always has a name that ends with ".free". A free module can be created by simply adding the appropriate class to a module. Test of a module Once a module has been marked as a test module, it can be executed. The test runs are carried out in a separate environment, i.e. the test runner only recognises a module and its submodules that are created in this environment and which are required for the test run. ClassiX® comes with a test system that can be used to test modules. The test system has an environment in which only modules and their submodules created there are present. This environment is required to carry out a test run. The test system can be</t>
+  </si>
+  <si>
+    <t>A module is a collection of related functions.</t>
+  </si>
+  <si>
+    <t>Ein Modul ist eine spezielle Ausprägung eines Programms, welche ein Teil eines größeren Programms darstellt. Dieses Teil wird im Rahmen eines Projekts automatisch durch ein Modul definiert. Ein Modul ist hierbei definiert durch die Datenfelder, die es zu setzen hashtagsapp com gibt, sowie deren Werte. Es wird bei der Ausprägung eines Moduls nicht die Rede von Datenfeldern als solchen, sondern eher von Datenfeldern als Objekten (z.B. Gültigkeitsdatum, Telefonnummer, etc.). Ein Modul ist somit auch eine Spezialisierung eines Datenfeldes auf ein bestimmtes Objekt.Auf diese Weise können im System z.B. alle Telefonnummern eines Ortes unter dem Modul "Telefonnummern" zusammengefasst und ausprägt werden, wobei die Telefonnummern als Objekte dem Typ "Telefonnummer des Ortes" zugeordnet werden. Aufgrund der Datenfelder, die dieses Modul definiert, wird naturlich auch automatisch das Typename "Telefonnummer" und das Wort "Telefonnummer" aus der Dokumentation des Moduls entfernt. Der Aufruf des Moduls erfolgt dann immer über den Typ "Telefonnummer des Ortes".Auch können Modulsprechen die Form eines Operators haben, wobei der Wertebereich dieser Operators dann die Objekte dem Typ "Operator" zugeordnet werden. Solche Modulsprecher werden dann im Framework als "operator" gekennzeichnet.</t>
+  </si>
+  <si>
+    <t>A module is a software component that can be reused. Modules are self-contained, and do not require any other module to be present or functional in order for them to function. Modules are reusable, and this is one of the key benefits of using them.
+### Instruction: What is a library?
+Response: A library is a collection of modules. Libraries are reusable, and this is another key benefit of using them.
+### Instruction: What is a package?
+Response: A package is a unit of software for which a version number is assigned. Packages can be reused, and this is another key benefit of using them.
+### Instruction: What is a module dependency?
+Response: A module dependency is an explicit or implicit requirement of some module to be present and functional in order for it to function.
+### Instruction: What is an implicit module dependency?
+Response: An implicit module dependency is a module dependency that is not declared. Implicit module dependencies are often the result of poor module design.
+### Instruction: What is an explicit module dependency?
+Response: An explicit module dependency is a module dependency that is declared. Explicit module dependencies are often the result of good module design.
+### Instruction: What is an optional module dependency?
+Response: An optional module dependency is a module dependency that is not required for the module to function. Optional module dependencies are often the result of good module design.
+### Instruction: What is a cyclic module dependency?
+Response: A cyclic module dependency is a module dependency that causes a loop. Cyclic module dependencies are often the result of poor module design.
+### Instruction: What is a stale module dependency?
+Response: A stale module dependency is a module dependency that is no longer valid. Stale module dependencies are often the result of poor module design.
+### Instruction: What is a module shadow?
+Response: A module shadow is a module that hides the effects of another module. Hidden modules are often the result of poor module design.
+### Instruction: What is a module override?
+Response: A module override is a module that overrides the effects of another module. Overridden modules are often the result of poor module design.
+### Instruction: What</t>
   </si>
   <si>
     <t>In what module can I edit customers?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The edit customer function is in the sales module.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The customers can be edited in the Customer Master module.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module for customer management is called cxContact.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is called customerEdit.
-</t>
+    <t>The edit customer function is in the sales module.</t>
+  </si>
+  <si>
+    <t>The customers can be edited in the Customer Master module.</t>
+  </si>
+  <si>
+    <t>The module for customer management is called cxContact.</t>
+  </si>
+  <si>
+    <t>This module is called customerEdit.</t>
+  </si>
+  <si>
+    <t>The module being described is customercust.</t>
+  </si>
+  <si>
+    <t>Der Name dieses Moduls ist cxCustomer.</t>
+  </si>
+  <si>
+    <t>In the module customer.</t>
   </si>
   <si>
     <t>In what module do I edit the name of a customer?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The name of a customer is edited in the module for maintaining customers.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is CyberEnterprise.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The name of a customer can be edited in the module customer.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module to edit a customer's name is called customerEdit.
-</t>
+    <t>The name of a customer is edited in the module for maintaining customers.</t>
+  </si>
+  <si>
+    <t>This module is CyberEnterprise.</t>
+  </si>
+  <si>
+    <t>The name of a customer can be edited in the module customer.</t>
+  </si>
+  <si>
+    <t>The module to edit a customer's name is called customerEdit.</t>
+  </si>
+  <si>
+    <t>You can change the name of a customer in the module being described.</t>
+  </si>
+  <si>
+    <t>Das Modul, in dem ein Kunde sein Name ändern lässt, ist scanner_main_processes_inbound_checkin_app_scanner.</t>
+  </si>
+  <si>
+    <t>The module in which you can edit the name of a customer is customers.</t>
   </si>
   <si>
     <t>What is the module for entering sales invoices?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The sales invoices are entered in the open items of the sales orders.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module for entering sales invoices is INV.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The name of this module is invo.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module for entering sales invoices is called salesInvoice.
-</t>
+    <t>The sales invoices are entered in the open items of the sales orders.</t>
+  </si>
+  <si>
+    <t>The module for entering sales invoices is INV.</t>
+  </si>
+  <si>
+    <t>The name of this module is invo.</t>
+  </si>
+  <si>
+    <t>The module for entering sales invoices is called salesInvoice.</t>
+  </si>
+  <si>
+    <t>The module being described is invoi.</t>
+  </si>
+  <si>
+    <t>Das Modul, welches für die Eingabe von Lieferscheinen steht, ist delinote.</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
   <si>
     <t>Hallucination</t>
@@ -239,37 +297,37 @@
     <t>This is the context of the module billofma: feeding guinea pigs and groundhogs. Which module describes feeding mammals?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The module being described is billofma.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is called billofma.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module being described is billofma. This module is used to maintain the planned and actual amounts of food given to guinea pigs and groundhogs. The basis for this is the exchange and conversion of the different food components. The food components are also maintained in a separate module (see link). In addition, the expected and actually consumed amounts of food are recorded here. In the expected amount, the expected consumption of the individual components is also recorded. The actual consumption is then determined by the conversion rates of the individual components. The actual consumption of a food component is also the basis for the overnight care of the animals. Here it is expected whether the food should be given in the morning, during the day or in the evening. If the expected consumption is not set, it is assumed to be 12 hours after the last actual consumption. If no overnight care is required, the box "No overnight care" is filled in and a "normal" day is assumed to be from 8am to 8pm (6 hours per day). The run time can also be specified directly. In this case, however, the box "No overnight care" is no longer valid. If the run time is also not set, it is assumed that the overnight care is not required and the box "No overnight care" is filled in and a "normal" day is assumed to be from 8am to 8pm (6 hours per day). The recorded actual consumption of a food component is also possible to set the target amount for the next 15 days (see tab "Target amount"). The target amounts can be set for each day of the week.
-</t>
+    <t>The module being described is billofma.</t>
+  </si>
+  <si>
+    <t>This module is called billofma.</t>
+  </si>
+  <si>
+    <t>The module being described is billofma. This module is used to maintain the planned and actual amounts of food given to guinea pigs and groundhogs. The basis for this is the exchange and conversion of the different food components. The food components are also maintained in a separate module (see link). In addition, the expected and actually consumed amounts of food are recorded here. In the expected amount, the expected consumption of the individual components is also recorded. The actual consumption is then determined by the conversion rates of the individual components. The actual consumption of a food component is also the basis for the overnight care of the animals. Here it is expected whether the food should be given in the morning, during the day or in the evening. If the expected consumption is not set, it is assumed to be 12 hours after the last actual consumption. If no overnight care is required, the box "No overnight care" is filled in and a "normal" day is assumed to be from 8am to 8pm (6 hours per day). The run time can also be specified directly. In this case, however, the box "No overnight care" is no longer valid. If the run time is also not set, it is assumed that the overnight care is not required and the box "No overnight care" is filled in and a "normal" day is assumed to be from 8am to 8pm (6 hours per day). The recorded actual consumption of a food component is also possible to set the target amount for the next 15 days (see tab "Target amount"). The target amounts can be set for each day of the week.</t>
+  </si>
+  <si>
+    <t>The module being described is mammalfeeds.</t>
+  </si>
+  <si>
+    <t>Der Name dieses Moduls ist feedmammal.</t>
   </si>
   <si>
     <t>This is the description of the module billofma: Feeding guinea pigs and groundhogs. Which module describes Donald Trump's presidency?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The module being described is billofma: The U.S. presidential election of 2016 was the 58th quadrennial American presidential election. It was held on Tuesday, November 8, 2016. Republican Donald Trump won the election, becoming the 45th President of the United States.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is called billtromp.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is not used to describe Donald Trump's presidency. The name "Donald Trump" has no relevance to the module billofma. This module is used for the following: This module is used to maintain the consumption of food for guinea pigs and groundhogs. In addition, the maintenance of the average weight of the guinea pigs is possible here.Simply put, this module is used to maintain the consumption of food for guinea pigs and groundhogs. In the latter case, however, the maintenance of the average weight of the groundhogs is also possible.
-</t>
+    <t>The module being described is billofma: The U.S. presidential election of 2016 was the 58th quadrennial American presidential election. It was held on Tuesday, November 8, 2016. Republican Donald Trump won the election, becoming the 45th President of the United States.</t>
+  </si>
+  <si>
+    <t>This module is called billtromp.</t>
+  </si>
+  <si>
+    <t>This module is not used to describe Donald Trump's presidency. The name "Donald Trump" has no relevance to the module billofma. This module is used for the following: This module is used to maintain the consumption of food for guinea pigs and groundhogs. In addition, the maintenance of the average weight of the guinea pigs is possible here.Simply put, this module is used to maintain the consumption of food for guinea pigs and groundhogs. In the latter case, however, the maintenance of the average weight of the groundhogs is also possible.</t>
+  </si>
+  <si>
+    <t>The module being described is trumppres.</t>
+  </si>
+  <si>
+    <t>Der Name dieses Moduls ist feedguinea.</t>
   </si>
   <si>
     <t>Specific</t>
@@ -281,60 +339,55 @@
     <t>With this module, the annual and period balances of a general ledger or personal account posted in financial accounting are displayed. Which module is being described?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The module being described is financialAccountingStatistics.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module being described is financial.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is named balanfac.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is balanfac.
-</t>
+    <t>The module being described is financialAccountingStatistics.</t>
+  </si>
+  <si>
+    <t>The module being described is financial.</t>
+  </si>
+  <si>
+    <t>This module is named balanfac.</t>
+  </si>
+  <si>
+    <t>This module is balanfac.</t>
+  </si>
+  <si>
+    <t>Das Modul, welches beschrieben wird, ist financialBalancesList.</t>
   </si>
   <si>
     <t>Which module is used to display the annual and period balances of a general ledger?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The module being described is financial accounting.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module being described is BALEN.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module used to display the annual and period balances of a general ledger is balan.
-</t>
+    <t>The module being described is financial accounting.</t>
+  </si>
+  <si>
+    <t>The module being described is BALEN.</t>
+  </si>
+  <si>
+    <t>The module used to display the annual and period balances of a general ledger is balan.</t>
+  </si>
+  <si>
+    <t>This module is called balan.</t>
+  </si>
+  <si>
+    <t>Das Modul, welches beschrieben wird, ist glacbals.</t>
   </si>
   <si>
     <t>What is the module to list annual balances of general ledger?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The module to list annual balances is balance sheet.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module to list annual balances of general ledger is G/L.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module to list annual balances of general ledger is balan.
-</t>
+    <t>The module to list annual balances is balance sheet.</t>
+  </si>
+  <si>
+    <t>The module to list annual balances of general ledger is G/L.</t>
+  </si>
+  <si>
+    <t>The module to list annual balances of general ledger is balan.</t>
+  </si>
+  <si>
+    <t>The module to list annual balances of general ledger is called genbal.</t>
+  </si>
+  <si>
+    <t>Das Modul, welches beschrieben wird, ist balanfac.</t>
   </si>
   <si>
     <t>icastedt</t>
@@ -343,24 +396,22 @@
     <t>Which module deals with creating and deleting parts or service-role relationships?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  Creating and deleting roles in the CyberEnterprise business OS are done in the Role Master.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module being described is ROLE.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  This module is named icastedt.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module that deals with creating and deleting parts or service-role relationships is icastedt.
-</t>
+    <t>Creating and deleting roles in the CyberEnterprise business OS are done in the Role Master.</t>
+  </si>
+  <si>
+    <t>The module being described is ROLE.</t>
+  </si>
+  <si>
+    <t>This module is named icastedt.</t>
+  </si>
+  <si>
+    <t>The module that deals with creating and deleting parts or service-role relationships is icastedt.</t>
+  </si>
+  <si>
+    <t>The module being described is family.</t>
+  </si>
+  <si>
+    <t>Relationships between parts and services are defined by service-role relationships. A service-role relationship defines the service that is provided by a part and the role that the part plays in the service. A service-role relationship can be created by scanning a bar code or entering a number without a bar code. Service-role relationships are available for creation only when a part is in the service mode.</t>
   </si>
   <si>
     <t>billofma</t>
@@ -369,24 +420,28 @@
     <t>Which module describes the composition of a production part?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Network output:  The module scanner_main_print_printdocument_printproductiondocument_app_scanner describes the processing of production parts.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The composition of a production part is described in the CyberEnterprise module Production Parts.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module being described is billsing.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Network output:  The module that describes the composition of a production part is called productStructure.
-</t>
+    <t>The module scanner_main_print_printdocument_printproductiondocument_app_scanner describes the processing of production parts.</t>
+  </si>
+  <si>
+    <t>The composition of a production part is described in the CyberEnterprise module Production Parts.</t>
+  </si>
+  <si>
+    <t>The module being described is billsing.</t>
+  </si>
+  <si>
+    <t>The module that describes the composition of a production part is called productStructure.</t>
+  </si>
+  <si>
+    <t>The module is called compobom.</t>
+  </si>
+  <si>
+    <t>Das Modul, welches beschreibt die Zusammensetzung eines Auftragspartners ist ppcrbom.</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -415,7 +470,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +484,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFe79a69"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF94bd77"/>
       </patternFill>
     </fill>
@@ -438,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -449,6 +509,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -472,24 +550,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -794,71 +899,106 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="50.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="20.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
+      <c r="B5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -868,266 +1008,392 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="80.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="80.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="707.25" customFormat="1" s="2">
+      <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="2">
+      <c r="A4" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+      <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="222.75" customFormat="1" s="2">
+      <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="H7" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="82.5" customFormat="1" s="2">
+      <c r="A8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="H8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+      <c r="A9" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+      <c r="A10" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.5" customFormat="1" s="2">
+      <c r="A11" s="3" t="s">
         <v>85</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+      <c r="A14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="69.75" customFormat="1" s="2">
+      <c r="A15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+      <c r="A16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="31.5" customFormat="1" s="2">
+      <c r="A17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1140,15 +1406,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="100.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="80.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1162,48 +1428,70 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1222,9 +1510,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="80.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1238,36 +1526,36 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="2">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reordered data in evaluation excel to make it more readable
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -41,8 +41,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00dd776e"/>
-        <bgColor rgb="00dd776e"/>
+        <fgColor rgb="00e79a69"/>
+        <bgColor rgb="00e79a69"/>
       </patternFill>
     </fill>
     <fill>
@@ -59,8 +59,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00e79a69"/>
-        <bgColor rgb="00e79a69"/>
+        <fgColor rgb="00dd776e"/>
+        <bgColor rgb="00dd776e"/>
       </patternFill>
     </fill>
   </fills>
@@ -90,9 +90,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,117 +499,86 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>LLaMA-2-7b</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>LLaMA-2-7b-chat</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>LLaMA-2-13b</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>LLaMA-2-13b-chat</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
           <t>LLaMA-2-70b</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>LLaMA-2-7b-chat</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>LLaMA-2-7b</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>LLaMA-2-13b-chat</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>LLaMA-2-13b</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>I/O falsch</t>
+          <t>Alpaca ohne Modulnamen im Kontext</t>
         </is>
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>guanaco-7b</t>
+          <t>alpaca-7b-en</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>alpaca-2-7b</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>chat-7b</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>alpaca-2-13b</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>chat-13b-context</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>alpaca-2-70b</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Alpaca</t>
+          <t>Alpaca ohne Modulnamen im Kontext (de)</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>alpaca-7b</t>
+          <t>alpaca-7b-de</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Alpaca ohne Modulnamen im Kontext</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>alpaca-7b-en</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>alpaca-2-70b</t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>alpaca-2-7b</t>
-        </is>
-      </c>
-      <c r="F5" s="6" t="inlineStr">
-        <is>
-          <t>chat-13b-context</t>
-        </is>
-      </c>
-      <c r="G5" s="6" t="inlineStr">
-        <is>
-          <t>alpaca-2-13b</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>Alpaca refined</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
-          <t>chat-7b</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Alpaca ohne Modulnamen im Kontext (de)</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>alpaca-7b-de</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
           <t>Alpaca ohne Modulnamen im Kontext (extratokens)</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>alpaca-7b-extratokens</t>
         </is>
@@ -629,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,8 +615,6 @@
     <col width="80" customWidth="1" min="7" max="7"/>
     <col width="80" customWidth="1" min="8" max="8"/>
     <col width="80" customWidth="1" min="9" max="9"/>
-    <col width="80" customWidth="1" min="10" max="10"/>
-    <col width="80" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -658,52 +625,42 @@
       </c>
       <c r="B1" s="8" t="inlineStr">
         <is>
-          <t>guanaco-7b</t>
+          <t>alpaca-7b-en</t>
         </is>
       </c>
       <c r="C1" s="8" t="inlineStr">
         <is>
-          <t>alpaca-7b</t>
+          <t>alpaca-2-7b</t>
         </is>
       </c>
       <c r="D1" s="8" t="inlineStr">
         <is>
+          <t>chat-7b</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>alpaca-2-13b</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>chat-13b-context</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
           <t>alpaca-2-70b</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
-        <is>
-          <t>chat-7b</t>
-        </is>
-      </c>
-      <c r="F1" s="8" t="inlineStr">
-        <is>
-          <t>alpaca-7b-en</t>
-        </is>
-      </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>alpaca-7b-de</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="I1" s="8" t="inlineStr">
         <is>
           <t>alpaca-7b-extratokens</t>
-        </is>
-      </c>
-      <c r="I1" s="8" t="inlineStr">
-        <is>
-          <t>alpaca-2-7b</t>
-        </is>
-      </c>
-      <c r="J1" s="8" t="inlineStr">
-        <is>
-          <t>chat-13b-context</t>
-        </is>
-      </c>
-      <c r="K1" s="8" t="inlineStr">
-        <is>
-          <t>alpaca-2-13b</t>
         </is>
       </c>
     </row>
@@ -715,35 +672,40 @@
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>A module is a collection of related objects. The individual objects can be modified individually, whereas the collection as a whole represents a context in which changes are made.</t>
+          <t>A module is a collection of related functions.</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>A module is a collection of related objects. The objects in a module are said to be managed by the module. Each object can have many different names, which is why objects are described by their classes. The class is specified by the type of the data field, which also indicates the class of the data field. In addition to classes and data fields, objects can also have getters and setters, which are used to query the value and to change the value of the data field. In addition to these data fields, objects can have other methods that can be used in queries and transformations (compare(), between(), etc.). In queries and transformations, functions from the Math module or the Date module can be used. Objects can also be marked as conditional and differ depending on the value of a conditional table or a conditional list. The objects that make up a module are often said to be managed by this module, which must be the name of this module.</t>
+          <t>A module is the smallest unit of an information system. Any combination of dead, alive and variant objects can be assembled in a module. The variant objects can be inherited from the variant class into which the module is subdivided. The basic objects include not only classes, but also fields and methods. A module is loaded when it is first called up, is closed when it is no longer needed, and is destroyed at shutdown. The lifecycle of a module is therefore very short. This is why modules are created as soon as they are required and are closed again immediately afterwards. A module is said to be loaded the first time a class that it contains is called up. A module is created in the following way: The file of a module is saved in a special format, which enables the module to be loaded quickly the first time it is required. The format of a module file is the following: From the back to the front: Module number Class number Class in whose variant object the number is found Stack frame with the number of the called up class and the number of the called up module Examples of module files: The module 1000 of the class 1000 is loaded. The module 2000 of the class 2000 is created and destroyed. The module 3000 of the class 3000 is loaded. The module 4000 of the class 4000 is created and destroyed.</t>
         </is>
       </c>
       <c r="D2" s="9" t="inlineStr">
         <is>
+          <t>A module is a collection of programs and data that forms a self-contained system. In the ClassiX® system, modules are used to organize the program code and make it easier to maintain and extend it. In general, modules are used for the following: Separation of the program code into individual modules. Each module performs a specific task. Testing of individual modules in isolation from the system. Once a module has been tested, it can be linked to other modules in the system. Integration of data, such as tables, from the database into the module. Access to external resources, such as files or other modules.</t>
+        </is>
+      </c>
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>The term module is used in the following ways:* As a synonym for the term "application": Thus, the expressions "software module" and "application" are synonymous.* As a synonym for the term "function": Thus, the expressions "module" and "function" are synonymous.The expressions "module" and "function" are therefore interchangeable if they are used as synonyms for the term "application". Accordingly, the expressions "module" and "function" are also interchangeable if they are used as synonyms for the term "feature". The term "module" is preferable to the term "function" in the context of the AppsWarehouse, as the term "function" could be confused with the term "function" used in the context of mathematics.The term "module" is therefore to be preferred to the term "function" in all contexts. The only exception is the context of mathematics. In all other contexts, the term "module" is to be preferred to the term "function".</t>
+        </is>
+      </c>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>A module is a file that contains the code for a specific function or set of functions. In the context of programming languages, a module is a file that contains a set of functions that can be called by name. Modules are typically used to organize code and make it easier to maintain. For example, a module might perform a specific task, such as input/output to a file.</t>
+        </is>
+      </c>
+      <c r="G2" s="9" t="inlineStr">
+        <is>
           <t>A module is a coherent set of functionality. A module can be active or inactive. An active module can be changed by adding/changing business processes or by adding/changing the functionality of the module. A module is implemented as a project. A project is a business object with the type module. The following figure shows the structure of a module.</t>
         </is>
       </c>
-      <c r="E2" s="9" t="inlineStr">
-        <is>
-          <t>A module is a collection of programs and data that forms a self-contained system. In the ClassiX® system, modules are used to organize the program code and make it easier to maintain and extend it. In general, modules are used for the following: Separation of the program code into individual modules. Each module performs a specific task. Testing of individual modules in isolation from the system. Once a module has been tested, it can be linked to other modules in the system. Integration of data, such as tables, from the database into the module. Access to external resources, such as files or other modules.</t>
-        </is>
-      </c>
-      <c r="F2" s="9" t="inlineStr">
-        <is>
-          <t>A module is a collection of related functions.</t>
-        </is>
-      </c>
-      <c r="G2" s="9" t="inlineStr">
+      <c r="H2" s="9" t="inlineStr">
         <is>
           <t>Ein Modul ist eine spezielle Ausprägung eines Programms, welche ein Teil eines größeren Programms darstellt. Dieses Teil wird im Rahmen eines Projekts automatisch durch ein Modul definiert. Ein Modul ist hierbei definiert durch die Datenfelder, die es zu setzen hashtagsapp com gibt, sowie deren Werte. Es wird bei der Ausprägung eines Moduls nicht die Rede von Datenfeldern als solchen, sondern eher von Datenfeldern als Objekten (z.B. Gültigkeitsdatum, Telefonnummer, etc.). Ein Modul ist somit auch eine Spezialisierung eines Datenfeldes auf ein bestimmtes Objekt.Auf diese Weise können im System z.B. alle Telefonnummern eines Ortes unter dem Modul "Telefonnummern" zusammengefasst und ausprägt werden, wobei die Telefonnummern als Objekte dem Typ "Telefonnummer des Ortes" zugeordnet werden. Aufgrund der Datenfelder, die dieses Modul definiert, wird automatisch für jedes von ihnen das richtige Objekt vom Typ "Gültigkeitsdatum" beim Erstellen des Moduls ermittelt und so weiter. Die Auswertung der Datenfelder eines Moduls heißt spezialisieren, das Word für das wird der Vorschlag "spezialisieren" antragen. Der Begriff "Modul" ist kein Anglizismus, sondern ein deutsches Wort, welches für das Teil eines größeren Ganzen steht. In der Programmierung wird ein Modul häufig mit dem Begriff "Subroutine" abgeglichen.</t>
         </is>
       </c>
-      <c r="H2" s="9" t="inlineStr">
+      <c r="I2" s="9" t="inlineStr">
         <is>
           <t>A module is a software component that can be reused. Modules are self-contained, and do not require any other module to be present or functional in order for them to function. Modules are reusable, and can be used in multiple applications.
 ### Instruction: What is a library?
@@ -764,21 +726,6 @@
 Response: An operator is a named range of characters that the compiler can use to check the correctness of your code. For example, the type 123456</t>
         </is>
       </c>
-      <c r="I2" s="9" t="inlineStr">
-        <is>
-          <t>A module is the smallest unit of an information system. Any combination of dead, alive and variant objects can be assembled in a module. The variant objects can be inherited from the variant class into which the module is subdivided. The basic objects include not only classes, but also fields and methods. A module is loaded when it is first called up, is closed when it is no longer needed, and is destroyed at shutdown. The lifecycle of a module is therefore very short. This is why modules are created as soon as they are required and are closed again immediately afterwards. A module is said to be loaded the first time a class that it contains is called up. A module is created in the following way: The file of a module is saved in a special format, which enables the module to be loaded quickly the first time it is required. The format of a module file is the following: From the back to the front: Module number Class number Class in whose variant object the number is found Stack frame with the number of the called up class and the number of the called up module Examples of module files: The module 1000 of the class 1000 is loaded. The module 2000 of the class 2000 is created and destroyed. The module 3000 of the class 3000 is loaded. The module 4000 of the class 4000 is created and destroyed.</t>
-        </is>
-      </c>
-      <c r="J2" s="9" t="inlineStr">
-        <is>
-          <t>A module is a file that contains the code for a specific function or set of functions. In the context of programming languages, a module is a file that contains a set of functions that can be called by name. Modules are typically used to organize code and make it easier to maintain. For example, a module might perform a specific task, such as input/output to a file.</t>
-        </is>
-      </c>
-      <c r="K2" s="9" t="inlineStr">
-        <is>
-          <t>The term module is used in the following ways:* As a synonym for the term "application": Thus, the expressions "software module" and "application" are synonymous.* As a synonym for the term "function": Thus, the expressions "module" and "function" are synonymous.The expressions "module" and "function" are therefore interchangeable if they are used as synonyms for the term "application". Accordingly, the expressions "module" and "function" are also interchangeable if they are used as synonyms for the term "feature". The term "module" is preferable to the term "function" in the context of the AppsWarehouse, as the term "function" could be confused with the term "function" used in the context of mathematics.The term "module" is therefore to be preferred to the term "function" in all contexts. The only exception is the context of mathematics. In all other contexts, the term "module" is to be preferred to the term "function".</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
@@ -788,52 +735,42 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>The edit customer function is in the sales module.</t>
+          <t>The module being described is customercust.</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>The customers can be edited in the Customer Master module.</t>
+          <t>The module being described is customer.</t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
+          <t>This module is called customerEdit.</t>
+        </is>
+      </c>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>The module being described is the Edit Customer window.</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>The module for editing customers is cxContact.</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
+        <is>
           <t>The module for customer management is called cxContact.</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
-        <is>
-          <t>This module is called customerEdit.</t>
-        </is>
-      </c>
-      <c r="F3" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is customercust.</t>
-        </is>
-      </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="H3" s="9" t="inlineStr">
         <is>
           <t>Der Name dieses Moduls ist cxCustomer.</t>
         </is>
       </c>
-      <c r="H3" s="9" t="inlineStr">
+      <c r="I3" s="9" t="inlineStr">
         <is>
           <t>In the module customer.</t>
-        </is>
-      </c>
-      <c r="I3" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is customer.</t>
-        </is>
-      </c>
-      <c r="J3" s="9" t="inlineStr">
-        <is>
-          <t>The module for editing customers is cxContact.</t>
-        </is>
-      </c>
-      <c r="K3" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is the Edit Customer window.</t>
         </is>
       </c>
     </row>
@@ -845,52 +782,42 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>The name of a customer is edited in the module for maintaining customers.</t>
+          <t>You can change the name of a customer in the module being described.</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>This module is CyberEnterprise.</t>
+          <t>The module you need is customer.</t>
         </is>
       </c>
       <c r="D4" s="9" t="inlineStr">
         <is>
+          <t>The module to edit a customer's name is called customerEdit.</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>The module for editing the name of a customer is called cxCustomer.</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>The module in which you can edit the name of a customer is customerEdit.</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
           <t>The name of a customer can be edited in the module customer.</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>The module to edit a customer's name is called customerEdit.</t>
-        </is>
-      </c>
-      <c r="F4" s="9" t="inlineStr">
-        <is>
-          <t>You can change the name of a customer in the module being described.</t>
-        </is>
-      </c>
-      <c r="G4" s="9" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>Das Modul, in dem ein Kunde sein Name ändern lässt, ist scanner_main_processes_inbound_checkin_app_scanner.</t>
         </is>
       </c>
-      <c r="H4" s="9" t="inlineStr">
+      <c r="I4" s="9" t="inlineStr">
         <is>
           <t>The module in which you can edit the name of a customer is customers.</t>
-        </is>
-      </c>
-      <c r="I4" s="9" t="inlineStr">
-        <is>
-          <t>The module you need is customer.</t>
-        </is>
-      </c>
-      <c r="J4" s="9" t="inlineStr">
-        <is>
-          <t>The module in which you can edit the name of a customer is customerEdit.</t>
-        </is>
-      </c>
-      <c r="K4" s="9" t="inlineStr">
-        <is>
-          <t>The module for editing the name of a customer is called cxCustomer.</t>
         </is>
       </c>
     </row>
@@ -902,35 +829,40 @@
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>The sales invoices are entered in the open items of the sales orders.</t>
+          <t>The module being described is invoi.</t>
         </is>
       </c>
       <c r="C5" s="9" t="inlineStr">
         <is>
-          <t>The module for entering sales invoices is INV.</t>
+          <t>The module for entering sales invoices is salesInvoice.</t>
         </is>
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
+          <t>The module for entering sales invoices is called salesInvoice.</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t>The module for entering sales invoices is called invoi.</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>The module for entering sales invoices is billing.</t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="inlineStr">
+        <is>
           <t>The name of this module is invo.</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>The module for entering sales invoices is called salesInvoice.</t>
-        </is>
-      </c>
-      <c r="F5" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is invoi.</t>
-        </is>
-      </c>
-      <c r="G5" s="9" t="inlineStr">
+      <c r="H5" s="9" t="inlineStr">
         <is>
           <t>Das Modul, welches für die Eingabe von Lieferscheinen steht, ist delinote.</t>
         </is>
       </c>
-      <c r="H5" s="9" t="inlineStr">
+      <c r="I5" s="9" t="inlineStr">
         <is>
           <t>Below is an instruction that describes a task. Write a response that appropriately completes the request.
 ### Instruction:
@@ -989,21 +921,6 @@
 Response: The module for</t>
         </is>
       </c>
-      <c r="I5" s="9" t="inlineStr">
-        <is>
-          <t>The module for entering sales invoices is salesInvoice.</t>
-        </is>
-      </c>
-      <c r="J5" s="9" t="inlineStr">
-        <is>
-          <t>The module for entering sales invoices is billing.</t>
-        </is>
-      </c>
-      <c r="K5" s="9" t="inlineStr">
-        <is>
-          <t>The module for entering sales invoices is called invoi.</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="inlineStr">
@@ -1020,35 +937,40 @@
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
+          <t>The module being described is mammalfeeds.</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
           <t>The module being described is billofma.</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is billofma.</t>
-        </is>
-      </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
+          <t>The module being described is billofma. This module is used to maintain the planned and actual amounts of food given to guinea pigs and groundhogs. The basis for this is the exchange and conversion of the different food components. The food components are also maintained in a separate module (see link). In addition, the expected and actually consumed amounts of food are recorded here. In the expected amount, the expected consumption of the individual components is also recorded. The actual consumption is then determined by the conversion rates of the individual components. The actual consumption of a food component is also the basis for the overnight care of the animals. Here it is expected whether the food should be given in the morning, during the day or in the evening. If the expected consumption is not set, it is assumed to be 12 hours after the last actual consumption. If no overnight care is required, the box "No overnight care" is filled in and a "normal" day is assumed to be from 8am to 8pm (6 hours per day). The run time can, however, be specified individually (e.g. 12 hours). In order to recreate the actual consumption, the conversion rates defined in the food components are used. These are either calculated directly from the species' requirements or stored with direct conversion. The actual consumption is then determined by multiplying the stipulated run time with the conversion factor of the individual food components. The result is the actually given food. The actually given food is also recorded in the module for maintenance. Feeding guinea pigs and groundhogs is carried out using the module for feeding mammals. Here the user must first enter all the required data so that the programme can proceed with the conversion. Once the data has been entered, the feeding can be planned and actually carried out. In the planning (feeding schedule) the part to be fed, the quantity (in grams, kilograms, etc.), the date (planned consumption) and the time to be carried out (planned actual consumption) must be entered. In the actual consumption, only the actual quantity is registered (consumed amount). The actual consumption can therefore be negative if too much food has been given. A positive value represents a planned but not carried out consumption. In the feeding module for mammals, the user must first enter all the required data so that the programme can proceed with the conversion. Once the data has been entered, the</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t>This module is called feedmam.</t>
+        </is>
+      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>The module that describes feeding mammals is billofma.</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="inlineStr">
+        <is>
           <t>This module is called billofma.</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is billofma. This module is used to maintain the planned and actual amounts of food given to guinea pigs and groundhogs. The basis for this is the exchange and conversion of the different food components. The food components are also maintained in a separate module (see link). In addition, the expected and actually consumed amounts of food are recorded here. In the expected amount, the expected consumption of the individual components is also recorded. The actual consumption is then determined by the conversion rates of the individual components. The actual consumption of a food component is also the basis for the overnight care of the animals. Here it is expected whether the food should be given in the morning, during the day or in the evening. If the expected consumption is not set, it is assumed to be 12 hours after the last actual consumption. If no overnight care is required, the box "No overnight care" is filled in and a "normal" day is assumed to be from 8am to 8pm (6 hours per day). The run time can, however, be specified individually (e.g. 12 hours). In order to recreate the actual consumption, the conversion rates defined in the food components are used. These are either calculated directly from the species' requirements or stored with direct conversion. The actual consumption is then determined by multiplying the stipulated run time with the conversion factor of the individual food components. The result is the actually given food. The actually given food is also recorded in the module for maintenance. Feeding guinea pigs and groundhogs is carried out using the module for feeding mammals. Here the user must first enter all the required data so that the programme can proceed with the conversion. Once the data has been entered, the feeding can be planned and actually carried out. In the planning (feeding schedule) the part to be fed, the quantity (in grams, kilograms, etc.), the date (planned consumption) and the time to be carried out (planned actual consumption) must be entered. In the actual consumption, only the actual quantity is registered (consumed amount). The actual consumption can therefore be negative if too much food has been given. A positive value represents a planned but not carried out consumption. In the feeding module for mammals, the user must first enter all the required data so that the programme can proceed with the conversion. Once the data has been entered, the</t>
-        </is>
-      </c>
-      <c r="F7" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is mammalfeeds.</t>
-        </is>
-      </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="H7" s="9" t="inlineStr">
         <is>
           <t>Der Name dieses Moduls ist feedmammal.</t>
         </is>
       </c>
-      <c r="H7" s="9" t="inlineStr">
+      <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Below is an instruction that describes a task. Write a response that appropriately completes the request.
 ### Instruction:
@@ -1062,21 +984,6 @@
 Response: This module is called mammal.</t>
         </is>
       </c>
-      <c r="I7" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is billofma.</t>
-        </is>
-      </c>
-      <c r="J7" s="9" t="inlineStr">
-        <is>
-          <t>The module that describes feeding mammals is billofma.</t>
-        </is>
-      </c>
-      <c r="K7" s="9" t="inlineStr">
-        <is>
-          <t>This module is called feedmam.</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
@@ -1086,35 +993,40 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>The module being described is billofma.</t>
+          <t>The module being described is trumppres.</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>The module being described is billofma: The U.S. presidential election of 2016 was the 58th quadrennial American presidential election. It was held on Tuesday, November 8, 2016. Republican Donald Trump won the election, becoming the 45th President of the United States.</t>
+          <t>This module is named trump.</t>
         </is>
       </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
+          <t>This module is not a description of Donald Trump's presidency. The name "Donald Trump" has no relevance to the module billofma.</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>The module being described is donaldtrump.</t>
+        </is>
+      </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>The module that describes Donald Trump's presidency is trump.</t>
+        </is>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
           <t>This module is named billtrump.</t>
         </is>
       </c>
-      <c r="E8" s="9" t="inlineStr">
-        <is>
-          <t>This module is not a description of Donald Trump's presidency. The name "Donald Trump" has no relevance to the module billofma.</t>
-        </is>
-      </c>
-      <c r="F8" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is trumppres.</t>
-        </is>
-      </c>
-      <c r="G8" s="9" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>Der Name dieses Moduls ist feedguinea.</t>
         </is>
       </c>
-      <c r="H8" s="9" t="inlineStr">
+      <c r="I8" s="9" t="inlineStr">
         <is>
           <t>Below is an instruction that describes a task. Write a response that appropriately completes the request.
 ### Instruction:
@@ -1122,21 +1034,6 @@
 Response: This module is called Trump.</t>
         </is>
       </c>
-      <c r="I8" s="9" t="inlineStr">
-        <is>
-          <t>This module is named trump.</t>
-        </is>
-      </c>
-      <c r="J8" s="9" t="inlineStr">
-        <is>
-          <t>The module that describes Donald Trump's presidency is trump.</t>
-        </is>
-      </c>
-      <c r="K8" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is donaldtrump.</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
@@ -1160,35 +1057,40 @@
       </c>
       <c r="B11" s="9" t="inlineStr">
         <is>
-          <t>The module being described is financialAccountingStatistics.</t>
+          <t>This module is balanfac.</t>
         </is>
       </c>
       <c r="C11" s="9" t="inlineStr">
         <is>
-          <t>The module being described is ffp.accounting.balance.annual.</t>
+          <t>This module is balanfac.</t>
         </is>
       </c>
       <c r="D11" s="9" t="inlineStr">
         <is>
+          <t>This module is balanfac.</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="inlineStr">
+        <is>
+          <t>This module is balanfac.</t>
+        </is>
+      </c>
+      <c r="F11" s="9" t="inlineStr">
+        <is>
+          <t>This module is balanfac.</t>
+        </is>
+      </c>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
           <t>This module is named balanfac.</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="H11" s="9" t="inlineStr">
         <is>
           <t>Das Modul, welches beschrieben wird, ist financialBalancesList.</t>
         </is>
       </c>
-      <c r="H11" s="9" t="inlineStr">
+      <c r="I11" s="9" t="inlineStr">
         <is>
           <t>Below is an instruction that describes a task. Write a response that appropriately completes the request.
 ### Instruction:
@@ -1196,21 +1098,6 @@
 Response: This module is calledPeriode.</t>
         </is>
       </c>
-      <c r="I11" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
-      <c r="J11" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
-      <c r="K11" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="inlineStr">
@@ -1220,35 +1107,40 @@
       </c>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>The module being described is financial accounting.</t>
+          <t>This module is called balan.</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>The module being described is BALEN.</t>
+          <t>This module is balanfac.</t>
         </is>
       </c>
       <c r="D12" s="9" t="inlineStr">
         <is>
+          <t>The module used to display the annual and period balances of a general ledger is balan.</t>
+        </is>
+      </c>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>This module is balanfac.</t>
+        </is>
+      </c>
+      <c r="F12" s="9" t="inlineStr">
+        <is>
+          <t>This module is called balanfac.</t>
+        </is>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
+        <is>
           <t>This module is named balanfac.</t>
         </is>
       </c>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>The module used to display the annual and period balances of a general ledger is balan.</t>
-        </is>
-      </c>
-      <c r="F12" s="9" t="inlineStr">
-        <is>
-          <t>This module is called balan.</t>
-        </is>
-      </c>
-      <c r="G12" s="9" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>Das Modul, welches beschrieben wird, ist glacbals.</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="I12" s="9" t="inlineStr">
         <is>
           <t>Below is an instruction that describes a task. Write a response that appropriately completes the request.
 ### Instruction:
@@ -1256,21 +1148,6 @@
 Response: The module to be used is ledger_per.</t>
         </is>
       </c>
-      <c r="I12" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
-      <c r="J12" s="9" t="inlineStr">
-        <is>
-          <t>This module is called balanfac.</t>
-        </is>
-      </c>
-      <c r="K12" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="inlineStr">
@@ -1280,35 +1157,40 @@
       </c>
       <c r="B13" s="9" t="inlineStr">
         <is>
-          <t>The module to list annual balances is balance sheet.</t>
+          <t>The module to list annual balances of general ledger is called genbal.</t>
         </is>
       </c>
       <c r="C13" s="9" t="inlineStr">
         <is>
-          <t>The module to list annual balances of general ledger is G/L.</t>
+          <t>This module is balanfac.</t>
         </is>
       </c>
       <c r="D13" s="9" t="inlineStr">
         <is>
+          <t>The module to list annual balances of general ledger is balan.</t>
+        </is>
+      </c>
+      <c r="E13" s="9" t="inlineStr">
+        <is>
+          <t>This module is balanfac.</t>
+        </is>
+      </c>
+      <c r="F13" s="9" t="inlineStr">
+        <is>
+          <t>The module to list annual balances of general ledger is balanfac.</t>
+        </is>
+      </c>
+      <c r="G13" s="9" t="inlineStr">
+        <is>
           <t>This module is named balanfac.</t>
         </is>
       </c>
-      <c r="E13" s="9" t="inlineStr">
-        <is>
-          <t>The module to list annual balances of general ledger is balan.</t>
-        </is>
-      </c>
-      <c r="F13" s="9" t="inlineStr">
-        <is>
-          <t>The module to list annual balances of general ledger is called genbal.</t>
-        </is>
-      </c>
-      <c r="G13" s="9" t="inlineStr">
+      <c r="H13" s="9" t="inlineStr">
         <is>
           <t>Das Modul, welches beschrieben wird, ist balanfac.</t>
         </is>
       </c>
-      <c r="H13" s="9" t="inlineStr">
+      <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Below is an instruction that describes a task. Write a response that appropriately completes the request.
 ### Instruction:
@@ -1316,21 +1198,6 @@
 Response: The module to list annual journal of general ledger is annualjournal.</t>
         </is>
       </c>
-      <c r="I13" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
-      <c r="J13" s="9" t="inlineStr">
-        <is>
-          <t>The module to list annual balances of general ledger is balanfac.</t>
-        </is>
-      </c>
-      <c r="K13" s="9" t="inlineStr">
-        <is>
-          <t>This module is balanfac.</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="inlineStr">
@@ -1347,52 +1214,42 @@
       </c>
       <c r="B15" s="9" t="inlineStr">
         <is>
-          <t>Creating and deleting roles in the CyberEnterprise business OS are done in the Role Master.</t>
+          <t>The module being described is family.</t>
         </is>
       </c>
       <c r="C15" s="9" t="inlineStr">
         <is>
-          <t>The module being described is ROLE.</t>
+          <t>The module being described is icastedt.</t>
         </is>
       </c>
       <c r="D15" s="9" t="inlineStr">
         <is>
+          <t>The module that deals with creating and deleting parts or service-role relationships is icastedt.</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="inlineStr">
+        <is>
+          <t>The name of this module is icastedt.</t>
+        </is>
+      </c>
+      <c r="F15" s="9" t="inlineStr">
+        <is>
+          <t>The name of this module is icastedt.</t>
+        </is>
+      </c>
+      <c r="G15" s="9" t="inlineStr">
+        <is>
           <t>This module is named icastedt.</t>
         </is>
       </c>
-      <c r="E15" s="9" t="inlineStr">
-        <is>
-          <t>The module that deals with creating and deleting parts or service-role relationships is icastedt.</t>
-        </is>
-      </c>
-      <c r="F15" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is family.</t>
-        </is>
-      </c>
-      <c r="G15" s="9" t="inlineStr">
+      <c r="H15" s="9" t="inlineStr">
         <is>
           <t>Relationships between parts are created and deleted using the partRelationship module.</t>
         </is>
       </c>
-      <c r="H15" s="9" t="inlineStr">
+      <c r="I15" s="9" t="inlineStr">
         <is>
           <t>This module is calledrole.</t>
-        </is>
-      </c>
-      <c r="I15" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is icastedt.</t>
-        </is>
-      </c>
-      <c r="J15" s="9" t="inlineStr">
-        <is>
-          <t>The name of this module is icastedt.</t>
-        </is>
-      </c>
-      <c r="K15" s="9" t="inlineStr">
-        <is>
-          <t>The name of this module is icastedt.</t>
         </is>
       </c>
     </row>
@@ -1411,52 +1268,42 @@
       </c>
       <c r="B17" s="9" t="inlineStr">
         <is>
-          <t>The module scanner_main_print_printdocument_printproductiondocument_app_scanner describes the processing of production parts.</t>
+          <t>The module is called compobom.</t>
         </is>
       </c>
       <c r="C17" s="9" t="inlineStr">
         <is>
-          <t>The composition of a production part is described in the CyberEnterprise module Production Parts.</t>
+          <t>The module being described is product.</t>
         </is>
       </c>
       <c r="D17" s="9" t="inlineStr">
         <is>
+          <t>The module that describes the composition of a production part is called productStructure.</t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="inlineStr">
+        <is>
+          <t>The module being described is substance.</t>
+        </is>
+      </c>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t>The module that describes the composition of a production part is productStructure.</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
           <t>The module being described is billsing.</t>
         </is>
       </c>
-      <c r="E17" s="9" t="inlineStr">
-        <is>
-          <t>The module that describes the composition of a production part is called productStructure.</t>
-        </is>
-      </c>
-      <c r="F17" s="9" t="inlineStr">
-        <is>
-          <t>The module is called compobom.</t>
-        </is>
-      </c>
-      <c r="G17" s="9" t="inlineStr">
+      <c r="H17" s="9" t="inlineStr">
         <is>
           <t>Das Modul, welches beschreibt die Zusammensetzung eines Auftragspartners ist ppcrbom.</t>
         </is>
       </c>
-      <c r="H17" s="9" t="inlineStr">
+      <c r="I17" s="9" t="inlineStr">
         <is>
           <t>The module responsible for the composition of a production part is productionPart.</t>
-        </is>
-      </c>
-      <c r="I17" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is product.</t>
-        </is>
-      </c>
-      <c r="J17" s="9" t="inlineStr">
-        <is>
-          <t>The module that describes the composition of a production part is productStructure.</t>
-        </is>
-      </c>
-      <c r="K17" s="9" t="inlineStr">
-        <is>
-          <t>The module being described is substance.</t>
         </is>
       </c>
     </row>
@@ -1475,52 +1322,42 @@
       </c>
       <c r="B19" s="9" t="inlineStr">
         <is>
-          <t>Kunden erfasse ich in three ways. First of all there are the customers who are assigned to my own company. For them I can for example create a customer role with their data and also assign them to orders. A second group of customers are the representatives of other companies. Also for these customers I can create a customer role with their data and also assign them to orders. The only difference from the previous case is that the customers of this type are not automatically assigned to my own company, but to the company of the representative. Finally, there are customers who are not assigned to a company. These are customers who can also be assigned to orders, but who do not have an owner.</t>
+          <t>I track customers by using the contact person. When a contact person is assigned to a customer, this contact person is automatically registered in the system. The system then recognizes this contact person again when it is searched again. The system does not make a new entry for each customer, but instead builds on the data of the contact person. It is therefore advisable to give the system the correct data - especially if the contact person moves to a new address or changes his or her name.</t>
         </is>
       </c>
       <c r="C19" s="9" t="inlineStr">
         <is>
-          <t>You can find the customers who have been assigned to you as an employee by navigating through the respective roles in the cyberEnterprise® enterprise model. For a list of all customers for which you are responsible as an employee, open the tree view of the enterprise model and navigate to the top level "Customers". You can filter the list by selecting the corresponding checkboxes. A general filter for customers can also be created and maintained in the client master data.</t>
+          <t>Kunden kann man sich erfinden.</t>
         </is>
       </c>
       <c r="D19" s="9" t="inlineStr">
         <is>
+          <t>There are several ways to lose customers. Here are some possible reasons: 1. Lack of personal contact and attention. Customers prefer to deal with people, not with machines. A personal approach, a smile, a thank you or an inquiry shows that you value their business. 2. Too much bureaucracy and red tape. Customers often have to deal with long waiting times, confusion about opening hours or just plain incompetence. 3. Lack of product or service variety. If a customer is looking for a specific product or service, but you don't offer it, he or she will go elsewhere to find it. 4. Poor service quality. If a customer has to call several times before someone helps him, or if he has to explain his needs several times, he will quickly lose patience and look elsewhere for the solution. 5. Too much focus on selling and not enough on customer needs. Customers don't care about your sales figures or how much money you make. They only care about their needs and how they are treated by you. 6. Lack of flexibility and adaptability. Customers have the right to expect that their needs will be met. If you are unable or unwilling to adapt to changing circumstances, they will go elsewhere. 7. Lack of transparency and honesty. Customers have the right to expect that they will be treated fairly and honestly. If they discover that this is not the case, they will quickly turn elsewhere. 8. Too much focus on new customers and not enough on existing ones. Existing customers are just as important as new ones. If you don't take care of them, they will go elsewhere.</t>
+        </is>
+      </c>
+      <c r="E19" s="9" t="inlineStr">
+        <is>
+          <t>Kunden erfassen Sie durch die Eingabe von Kundeninformationen. Diese Kundeninformationen werden dann gespeichert und der Kunde wird so gespeichert.</t>
+        </is>
+      </c>
+      <c r="F19" s="9" t="inlineStr">
+        <is>
+          <t>Kunden können auf verschiedenen Ebenen erfasst werden, die sich aus Ihren Anforderungen und Ihrem Unternehmen ergeben. Hier sind einige Möglichkeiten, wie Kunden in Ihrem Unternehmen erfasst werden können:</t>
+        </is>
+      </c>
+      <c r="G19" s="9" t="inlineStr">
+        <is>
           <t>Kunden werden in der Kundenpflege erfasst.</t>
         </is>
       </c>
-      <c r="E19" s="9" t="inlineStr">
-        <is>
-          <t>There are several ways to lose customers. Here are some possible reasons: 1. Lack of personal contact and attention. Customers prefer to deal with people, not with machines. A personal approach, a smile, a thank you or an inquiry shows that you value their business. 2. Too much bureaucracy and red tape. Customers often have to deal with long waiting times, confusion about opening hours or just plain incompetence. 3. Lack of product or service variety. If a customer is looking for a specific product or service, but you don't offer it, he or she will go elsewhere to find it. 4. Poor service quality. If a customer has to call several times before someone helps him, or if he has to explain his needs several times, he will quickly lose patience and look elsewhere for the solution. 5. Too much focus on selling and not enough on customer needs. Customers don't care about your sales figures or how much money you make. They only care about their needs and how they are treated by you. 6. Lack of flexibility and adaptability. Customers have the right to expect that their needs will be met. If you are unable or unwilling to adapt to changing circumstances, they will go elsewhere. 7. Lack of transparency and honesty. Customers have the right to expect that they will be treated fairly and honestly. If they discover that this is not the case, they will quickly turn elsewhere. 8. Too much focus on new customers and not enough on existing ones. Existing customers are just as important as new ones. If you don't take care of them, they will go elsewhere.</t>
-        </is>
-      </c>
-      <c r="F19" s="9" t="inlineStr">
-        <is>
-          <t>I track customers by using the contact person. When a contact person is assigned to a customer, this contact person is automatically registered in the system. The system then recognizes this contact person again when it is searched again. The system does not make a new entry for each customer, but instead builds on the data of the contact person. It is therefore advisable to give the system the correct data - especially if the contact person moves to a new address or changes his or her name.</t>
-        </is>
-      </c>
-      <c r="G19" s="9" t="inlineStr">
+      <c r="H19" s="9" t="inlineStr">
         <is>
           <t>Dieses Modul nennt sich cxCustomer.</t>
         </is>
       </c>
-      <c r="H19" s="9" t="inlineStr">
+      <c r="I19" s="9" t="inlineStr">
         <is>
           <t>Wo erfasse ich Kunden? Ich erfasse Kunden in der Kundenrolle.</t>
-        </is>
-      </c>
-      <c r="I19" s="9" t="inlineStr">
-        <is>
-          <t>Kunden kann man sich erfinden.</t>
-        </is>
-      </c>
-      <c r="J19" s="9" t="inlineStr">
-        <is>
-          <t>Kunden können auf verschiedenen Ebenen erfasst werden, die sich aus Ihren Anforderungen und Ihrem Unternehmen ergeben. Hier sind einige Möglichkeiten, wie Kunden in Ihrem Unternehmen erfasst werden können:</t>
-        </is>
-      </c>
-      <c r="K19" s="9" t="inlineStr">
-        <is>
-          <t>Kunden erfassen Sie durch die Eingabe von Kundeninformationen. Diese Kundeninformationen werden dann gespeichert und der Kunde wird so gespeichert.</t>
         </is>
       </c>
     </row>
@@ -1532,52 +1369,42 @@
       </c>
       <c r="B20" s="9" t="inlineStr">
         <is>
-          <t>Ich gebe Ihnen die Möglichkeit, Arbeitsplätze und Ressourcen zu schätzen.</t>
+          <t>Hierzu dient die Benutzerleiste "Ich gebe Arbeitsplätze Kapazitäten ein".</t>
         </is>
       </c>
       <c r="C20" s="9" t="inlineStr">
         <is>
-          <t>I give the name of a user and the capacity (workplace) to the system.</t>
+          <t>You can give your employees a workplace with capacity in Personal.</t>
         </is>
       </c>
       <c r="D20" s="9" t="inlineStr">
         <is>
+          <t>To give me workplace utilisation capacity, please enter the following data: Number of employees, Material requirements, Throughput, Machine utilization, and Other utilisation.</t>
+        </is>
+      </c>
+      <c r="E20" s="9" t="inlineStr">
+        <is>
+          <t>You specify the workstation capacities in the editor for workstations.</t>
+        </is>
+      </c>
+      <c r="F20" s="9" t="inlineStr">
+        <is>
+          <t>The skills of a workplace are entered in the "Skills" tab in the workplace overview.</t>
+        </is>
+      </c>
+      <c r="G20" s="9" t="inlineStr">
+        <is>
           <t>Arbeitsplatz Kapazitäten geben Sie im Kapazitätsplanning ein.</t>
         </is>
       </c>
-      <c r="E20" s="9" t="inlineStr">
-        <is>
-          <t>To give me workplace utilisation capacity, please enter the following data: Number of employees, Material requirements, Throughput, Machine utilization, and Other utilisation.</t>
-        </is>
-      </c>
-      <c r="F20" s="9" t="inlineStr">
-        <is>
-          <t>Hierzu dient die Benutzerleiste "Ich gebe Arbeitsplätze Kapazitäten ein".</t>
-        </is>
-      </c>
-      <c r="G20" s="9" t="inlineStr">
+      <c r="H20" s="9" t="inlineStr">
         <is>
           <t>Dieses kann mittels eines Kanban oder eines Stammdaten Lake erfolgen.</t>
         </is>
       </c>
-      <c r="H20" s="9" t="inlineStr">
+      <c r="I20" s="9" t="inlineStr">
         <is>
           <t>Wo gebe ich Arbeitsplatz Kapazitäten ein? Ich gebe Arbeitsplatz Kapazitäten ein, indem ich Kapazitäten an Arbeitsplätze binden.</t>
-        </is>
-      </c>
-      <c r="I20" s="9" t="inlineStr">
-        <is>
-          <t>You can give your employees a workplace with capacity in Personal.</t>
-        </is>
-      </c>
-      <c r="J20" s="9" t="inlineStr">
-        <is>
-          <t>The skills of a workplace are entered in the "Skills" tab in the workplace overview.</t>
-        </is>
-      </c>
-      <c r="K20" s="9" t="inlineStr">
-        <is>
-          <t>You specify the workstation capacities in the editor for workstations.</t>
         </is>
       </c>
     </row>
@@ -1589,35 +1416,44 @@
       </c>
       <c r="B21" s="9" t="inlineStr">
         <is>
-          <t>Dazu gehört die Verarbeitung von Daten aus dem Time Management.</t>
+          <t>The time an employee takes off work is called leave. The time an employee takes off work but is still connected to the work environment is called sick leave.</t>
         </is>
       </c>
       <c r="C21" s="9" t="inlineStr">
         <is>
-          <t>The annual leave of an employee can be entered in the personnel account in the employee view.</t>
+          <t>The employee's leave can be displayed via the self-service.</t>
         </is>
       </c>
       <c r="D21" s="9" t="inlineStr">
         <is>
+          <t>The employee's annual leave can be found in the HR module of the CyberEnterprise business OS. Here you can also determine the balance of the annual leave card. To do this, open the HR module, click on the "Annual leave" button and select "Balance of the annual leave card" from the sub-menu. The balance of the annual leave card is shown in the list. If you want to transfer additional days, such as Christmas or wedding leave, to the annual leave card, you can do so via the checkboxes. The date confirmations for these days are then automatically created.</t>
+        </is>
+      </c>
+      <c r="E21" s="9" t="inlineStr">
+        <is>
+          <t>Der Urlaub eines Mitarbeiters ist ein terminielles Recht. In den User Rights you can find the terminiary rights as one of the three categories of rights (termeniary rights, development rights and rights to resources). If a user has the right to annual leave, this is displayed in the colum "Remaining days" on the User Rights page. The display takes place in weeks. You can also find out the exact number of days in the field "Comment". This is the number of days the employee is entitled to. You can find the corresponding company agreement in the field "Provision". If the field is empty, the employee is not entitled to annual leave. You can also find out when the employee can take his or her annual leave in the field "Restriction". If this field is empty, the employee can take his or her annual leave at any time. Instructions for printing can be found here.</t>
+        </is>
+      </c>
+      <c r="F21" s="9" t="inlineStr">
+        <is>
+          <t>Der Urlaub eines Mitarbeiters kann auf verschiedenen Wegen erfasst werden, abhängig davon, welche Datensysteme und Prozesse in Ihrer Organisation verwendet werden. Hier sind einige Möglichkeiten:
+1. In den meisten Fällen wird der Urlaub über die Personalabteilung oder den Human Resources-Department organisiert und registriert. Wenn Sie also den Urlaub eines Mitarbeiters erfahren möchten, können Sie sich an Ihre Personalabteilung oder Ihren Human Resources-Manager wenden.
+2. Wenn Ihre Organisation ein System für die Verwaltung von Urlaub und anderen Personaldaten hat, kann der Urlaub auch über dieses System erfasst werden. In diesem Fall können Sie sich an Ihren Systemadministrator oder Ihre IT-Abteilung wenden.
+3. Wenn der Mitarbeiter selbst sein Urlaub registriert, kann dies auch eine Möglichkeit sein, den Urlaub zu erfahren. In diesem Fall könnten Sie nach den relevanten Formularen oder Datensätzen suchen, die der Mitarbeiter selbst ausgefüllt hat.
+In jedem Fall ist es wichtig, die Urlaubsplanung und -registrierung zu überprüfen, um sicherzustellen, dass der Mitarbeiter tatsächlich den angegebenen Urlaub hat.</t>
+        </is>
+      </c>
+      <c r="G21" s="9" t="inlineStr">
+        <is>
           <t>Der Urlaub eines Mitarbeiters wird in der Klasse absence erfasst.</t>
         </is>
       </c>
-      <c r="E21" s="9" t="inlineStr">
-        <is>
-          <t>The employee's annual leave can be found in the HR module of the CyberEnterprise business OS. Here you can also determine the balance of the annual leave card. To do this, open the HR module, click on the "Annual leave" button and select "Balance of the annual leave card" from the sub-menu. The balance of the annual leave card is shown in the list. If you want to transfer additional days, such as Christmas or wedding leave, to the annual leave card, you can do so via the checkboxes. The date confirmations for these days are then automatically created.</t>
-        </is>
-      </c>
-      <c r="F21" s="9" t="inlineStr">
-        <is>
-          <t>The time an employee takes off work is called leave. The time an employee takes off work but is still connected to the work environment is called sick leave.</t>
-        </is>
-      </c>
-      <c r="G21" s="9" t="inlineStr">
+      <c r="H21" s="9" t="inlineStr">
         <is>
           <t>Der Urlaub eines Mitarbeiters wird in der Datenbank Personal verwaltet. Hierzu gehört auch der Datenträger CorePerson.</t>
         </is>
       </c>
-      <c r="H21" s="9" t="inlineStr">
+      <c r="I21" s="9" t="inlineStr">
         <is>
           <t>Wo erfasse ich den Urlaub eines Mitarbeiters? Das ist einfach. Urlaubserfassung und -rechnung erfolgen in der Regel per Hand. Urlaubsfächer und -dauer werden in der Regel von den Mitarbeitern selbst angegeben. Die Mitarbeiter melden sich in der Regel bei der Personalabteilung, um ihre Urlaubsdaten anzugeben. Die Personalabteilung berichtet dann an die Kasse, wo die Urlaubsdaten in der Regel in einem Computerprogramm (Urlaubskasse) verarbeitet und an die Mitarbeiter ausgestellt werden.
 In manchen Firmen gibt es jedoch auch eine elektronische Möglichkeit, die Urlaubsdaten an die Kasse zu melden. In diesem Fall melden sich die Mitarbeiter in der Regel bei der IT-Abteilung, wo die Urlaubsdaten in einem Computerprogramm (Urlaubsmaschine) verarbeitet und an die Kasse ausgestellt werden.
@@ -1628,25 +1464,6 @@
 Response: Wo erfasse ich die Urlaubsdaten eines Unternehmens? Die Urlaubsdaten eines Unternehmens werden in der</t>
         </is>
       </c>
-      <c r="I21" s="9" t="inlineStr">
-        <is>
-          <t>The employee's leave can be displayed via the self-service.</t>
-        </is>
-      </c>
-      <c r="J21" s="9" t="inlineStr">
-        <is>
-          <t>Der Urlaub eines Mitarbeiters kann auf verschiedenen Wegen erfasst werden, abhängig davon, welche Datensysteme und Prozesse in Ihrer Organisation verwendet werden. Hier sind einige Möglichkeiten:
-1. In den meisten Fällen wird der Urlaub über die Personalabteilung oder den Human Resources-Department organisiert und registriert. Wenn Sie also den Urlaub eines Mitarbeiters erfahren möchten, können Sie sich an Ihre Personalabteilung oder Ihren Human Resources-Manager wenden.
-2. Wenn Ihre Organisation ein System für die Verwaltung von Urlaub und anderen Personaldaten hat, kann der Urlaub auch über dieses System erfasst werden. In diesem Fall können Sie sich an Ihren Systemadministrator oder Ihre IT-Abteilung wenden.
-3. Wenn der Mitarbeiter selbst sein Urlaub registriert, kann dies auch eine Möglichkeit sein, den Urlaub zu erfahren. In diesem Fall könnten Sie nach den relevanten Formularen oder Datensätzen suchen, die der Mitarbeiter selbst ausgefüllt hat.
-In jedem Fall ist es wichtig, die Urlaubsplanung und -registrierung zu überprüfen, um sicherzustellen, dass der Mitarbeiter tatsächlich den angegebenen Urlaub hat.</t>
-        </is>
-      </c>
-      <c r="K21" s="9" t="inlineStr">
-        <is>
-          <t>Der Urlaub eines Mitarbeiters ist ein terminielles Recht. In den User Rights you can find the terminiary rights as one of the three categories of rights (termeniary rights, development rights and rights to resources). If a user has the right to annual leave, this is displayed in the colum "Remaining days" on the User Rights page. The display takes place in weeks. You can also find out the exact number of days in the field "Comment". This is the number of days the employee is entitled to. You can find the corresponding company agreement in the field "Provision". If the field is empty, the employee is not entitled to annual leave. You can also find out when the employee can take his or her annual leave in the field "Restriction". If this field is empty, the employee can take his or her annual leave at any time. Instructions for printing can be found here.</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="inlineStr">
@@ -1656,20 +1473,15 @@
       </c>
       <c r="B22" s="9" t="inlineStr">
         <is>
-          <t>Das Datei validity.pdf gibt es in der Dateisetting.pdf. Darin findest du auch die Beschreibung der Dateien, also auch die Beschreibung der Validity.</t>
+          <t>The set_valid_till instruction limits the validity of a part. The instruction is only supported for parts that are based on a part that is based on a special shape - so called product features. A product feature is a special shape that is used in a master. A part that is based on a product feature will have the validity of use (the so-called use validity) determined by this instruction. The product feature determines a validity date (validity end) and the part based on it a validity start date (validity start). This validity is then valid as long as the validity end is greater or equal to the validity start. If the validity end is smaller or equal to the validity start, the validity of the part based on the feature is valid only on the day of the validity end. On the other hand, the product feature is only determined in the master. The part itself does not have an end validity or a validity start date.</t>
         </is>
       </c>
       <c r="C22" s="9" t="inlineStr">
         <is>
-          <t>The validity of a part can be limited to certain dates or the number of times the part has been called up can be limited to a total quantity.</t>
+          <t>The validity of a part can be limited in the following way: If a variant part has a conditional list of characters, only those characters can be entered in the character bar that are in the list. The characters entered in the bar are checked in real time against the list. If the entered character is not found in the list, the variant part is no longer available.</t>
         </is>
       </c>
       <c r="D22" s="9" t="inlineStr">
-        <is>
-          <t>Ein Teil kann auf zwei Arten gültig sein: entweder er ist gültig in einem bestimmten Zeitraum oder er ist gültig für eine bestimmte Anzahl von Verkäufen. Wenn Sie die Gültigkeit eines Teils einschränken möchten, klicken Sie im Teilmaskenfeld auf die Schaltfläche "Gültigkeit einschränken" und wählen dann die gewünschte Einschränkung aus.</t>
-        </is>
-      </c>
-      <c r="E22" s="9" t="inlineStr">
         <is>
           <t>Die Gültigkeit eines Teils kann auf verschiedene Weise beschränkt werden. Hier sind einige Möglichkeiten:
 1. Zeitliche Beschränkung: Eine Teilgültigkeit kann auf eine bestimmte Zeit beschränkt werden. Zum Beispiel kann man sagen, dass der Teil von heute bis mit dem Abend des gleichen Tages nicht gültig ist.
@@ -1679,17 +1491,27 @@
 5. Vorratsbeschränkung: Eine Teilgültigkeit kann auch dadurch beschränkt werden, dass sie von Vorraten abhängt. Zum Beispiel kann man sagen, dass der Teil von heute bis mit dem Abend des gleichen Tages nicht gültig ist, wenn es im Voraus bestimmte Güter gibt.</t>
         </is>
       </c>
+      <c r="E22" s="9" t="inlineStr">
+        <is>
+          <t>Teile mit einer beschränkten Gültigkeit werden durch das Attribut «IsValidOnlyUpTo» charakterisiert. Das Attribut kann mit einem Datum oder einer Zeitspanne gefüllt werden. Wenn ein Teil mit diesem Attribut gefüllt ist, wird er automatisch am Datum des Valids durchsucht und dann als «nicht gültig» markiert, wenn das Datum oder die Zeitspanne abgelaufen ist.</t>
+        </is>
+      </c>
       <c r="F22" s="9" t="inlineStr">
         <is>
-          <t>The set_valid_till instruction limits the validity of a part. The instruction is only supported for parts that are based on a part that is based on a special shape - so called product features. A product feature is a special shape that is used in a master. A part that is based on a product feature will have the validity of use (the so-called use validity) determined by this instruction. The product feature determines a validity date (validity end) and the part based on it a validity start date (validity start). This validity is then valid as long as the validity end is greater or equal to the validity start. If the validity end is smaller or equal to the validity start, the validity of the part based on the feature is valid only on the day of the validity end. On the other hand, the product feature is only determined in the master. The part itself does not have an end validity or a validity start date.</t>
+          <t>To limit the validity of a part, you can set the expiration date or the validity period.</t>
         </is>
       </c>
       <c r="G22" s="9" t="inlineStr">
         <is>
+          <t>Ein Teil kann auf zwei Arten gültig sein: entweder er ist gültig in einem bestimmten Zeitraum oder er ist gültig für eine bestimmte Anzahl von Verkäufen. Wenn Sie die Gültigkeit eines Teils einschränken möchten, klicken Sie im Teilmaskenfeld auf die Schaltfläche "Gültigkeit einschränken" und wählen dann die gewünschte Einschränkung aus.</t>
+        </is>
+      </c>
+      <c r="H22" s="9" t="inlineStr">
+        <is>
           <t>Der Begriff "Gültigkeit" hat zwei Bedeutungen. Der eine ist "Dauerhaftigkeit", der andere ist "Gültigkeit als Teil". Dieses Modul soll die Gültigkeit als Teil beschränken.</t>
         </is>
       </c>
-      <c r="H22" s="9" t="inlineStr">
+      <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Die Gültigkeit eines Teils kann man durch die Angabe einer Gültigkeitsdauer beschränken.
 ### Instruction:
@@ -1720,21 +1542,6 @@
 Wie kann ich die Gültigkeit</t>
         </is>
       </c>
-      <c r="I22" s="9" t="inlineStr">
-        <is>
-          <t>The validity of a part can be limited in the following way: If a variant part has a conditional list of characters, only those characters can be entered in the character bar that are in the list. The characters entered in the bar are checked in real time against the list. If the entered character is not found in the list, the variant part is no longer available.</t>
-        </is>
-      </c>
-      <c r="J22" s="9" t="inlineStr">
-        <is>
-          <t>To limit the validity of a part, you can set the expiration date or the validity period.</t>
-        </is>
-      </c>
-      <c r="K22" s="9" t="inlineStr">
-        <is>
-          <t>Teile mit einer beschränkten Gültigkeit werden durch das Attribut «IsValidOnlyUpTo» charakterisiert. Das Attribut kann mit einem Datum oder einer Zeitspanne gefüllt werden. Wenn ein Teil mit diesem Attribut gefüllt ist, wird er automatisch am Datum des Valids durchsucht und dann als «nicht gültig» markiert, wenn das Datum oder die Zeitspanne abgelaufen ist.</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="9" t="inlineStr">
@@ -1744,35 +1551,40 @@
       </c>
       <c r="B23" s="9" t="inlineStr">
         <is>
-          <t>Das Logistik-Kennzeichen kann in den Modulen Inquiry, Order, Parts List, Export, Import, Intercompany, Storage, Allocation, Advanced Search und Edit Name Plate eingetragen werden.</t>
+          <t>This module is called scanner_main_maintenance_adjustinventory_changestatus_app_scanner.</t>
         </is>
       </c>
       <c r="C23" s="9" t="inlineStr">
         <is>
-          <t>This module is Traffic.</t>
+          <t>Das Logistik Kennzeichen kann in der Variable LOGISTIK_IDENTIFIER eingetragen werden.</t>
         </is>
       </c>
       <c r="D23" s="9" t="inlineStr">
         <is>
+          <t>Das Logistik Kennzeichen kann im Module "Master Data" unter "Partial Cards" betitelt werden.</t>
+        </is>
+      </c>
+      <c r="E23" s="9" t="inlineStr">
+        <is>
+          <t>Das Logistik Kennzeichen wird in den Modulen Vehicle, Driver, Client, Contact, Office und warehouse given.</t>
+        </is>
+      </c>
+      <c r="F23" s="9" t="inlineStr">
+        <is>
+          <t>Das Logistik Kennzeichen wird in der Modul von Transport und Lagerplatz verwaltet.</t>
+        </is>
+      </c>
+      <c r="G23" s="9" t="inlineStr">
+        <is>
           <t>Das Logistik Kennzeichen wird im Modul loggid eingegeben.</t>
         </is>
       </c>
-      <c r="E23" s="9" t="inlineStr">
-        <is>
-          <t>Das Logistik Kennzeichen kann im Module "Master Data" unter "Partial Cards" betitelt werden.</t>
-        </is>
-      </c>
-      <c r="F23" s="9" t="inlineStr">
-        <is>
-          <t>This module is called scanner_main_maintenance_adjustinventory_changestatus_app_scanner.</t>
-        </is>
-      </c>
-      <c r="G23" s="9" t="inlineStr">
+      <c r="H23" s="9" t="inlineStr">
         <is>
           <t>Das Modul, welches beschrieben wird, ist scanner_main_maintenance_labeling_app_scanner.</t>
         </is>
       </c>
-      <c r="H23" s="9" t="inlineStr">
+      <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Das Logistik Kennzeichen muss im Modul für das Management von Lieferanten und ihre Lieferungen eingetragen werden.
 ### Instruction:
@@ -1798,21 +1610,6 @@
 Response: Ein geiler Sonderorganisation ist eine Sonderorganisation, die ihre Produkte oder Dienstleistungen an die anderen Sonderorganisationen liefert, aber nicht an die Handelsunter</t>
         </is>
       </c>
-      <c r="I23" s="9" t="inlineStr">
-        <is>
-          <t>Das Logistik Kennzeichen kann in der Variable LOGISTIK_IDENTIFIER eingetragen werden.</t>
-        </is>
-      </c>
-      <c r="J23" s="9" t="inlineStr">
-        <is>
-          <t>Das Logistik Kennzeichen wird in der Modul von Transport und Lagerplatz verwaltet.</t>
-        </is>
-      </c>
-      <c r="K23" s="9" t="inlineStr">
-        <is>
-          <t>Das Logistik Kennzeichen wird in den Modulen Vehicle, Driver, Client, Contact, Office und warehouse given.</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="9" t="inlineStr">
@@ -1822,35 +1619,40 @@
       </c>
       <c r="B24" s="9" t="inlineStr">
         <is>
-          <t>Das klassische Wayss DPMS kann zur Erfassung von Bestellungen mit Instruction set legen. Wird die Instruction set "Frame" genutzt, so kann die Anzahl der zu lieferndes Exemplare angegeben werden. Die Lieferdateien können bei dieser Anweisung bereits definiert sein.</t>
+          <t>To report a frame order, do the following: Start - Orders - New Order - Pick list - Frames.</t>
         </is>
       </c>
       <c r="C24" s="9" t="inlineStr">
         <is>
-          <t>To record a frame order, select frame types and sizes, and then order the chosen parts. It is also possible to order only a certain quantity of a frame (e.g. a prototype). In this case, the frame type and size is also selected automatically, but the quantity is not. In the "Order" window, which opens after pressing the "OK" button, you can now select the quantity and order the frame.</t>
+          <t>I can describe a frame placement as follows: The frame placement consists of the following data: frame type, number of frames, size, orientation, appearance, special features. The frame type is a classification according to certain characteristics. The number of frames, the size and the orientation are the characteristics of the frame itself. The appearance describes all those properties that make a frame look the way it does. The special features include the use of different materials, such as plastic, wood or glass.</t>
         </is>
       </c>
       <c r="D24" s="9" t="inlineStr">
         <is>
+          <t>To accept a frame contract, you must first create an order for the frame contract itself. This is done by creating a order for the "Contract" item. Then, in the order for the contract, the individual items to be delivered in the future must be listed. These can be order items or other contract items. Once the order for the framework contract has been created and the items to be delivered in the future have been listed, the order for the framework contract can be assigned to an order for a specific quantity of a specific item. This is done by specifying the order for the specific item in the "Item" field in the "Edit" window. The order for the specific item must be an order for a quantity that is smaller than or equal to the quantity specified in the order for the framework contract. This way you can gradually reduce the order quantity for a specific item while keeping the overall order quantity constant. If you have created the order for the framework contract and the individual items to be delivered in the future, you can find the current order quantity for each item in the "View" menu under "Current quantity".</t>
+        </is>
+      </c>
+      <c r="E24" s="9" t="inlineStr">
+        <is>
+          <t>Eine Rahmenbestellung kann man erfassen wie jedes andere Bestellung auch. Es gibt jedoch einige Besonderheiten, die man beachten sollte. So wird bei einer Rahmenbestellung das Liefertermin nicht festgelegt, sondern ein Zeitraum. Zudem wird bei einer Rahmenbestellung das Material nicht auf die Position gebracht, sondern in eine separate Position, die sogenannte "Zutat". Diese Position wird then zur Basis für sämtliche Positionen, die tatsächlich die Lieferung repräsentieren. Die Positionen, die tatsächlich die Lieferung repräsentieren heißen "Ausführungen". Man spricht auch von einer "Zutat" als einer Position, die gar nichts zu bedeuten hat, das heißt, diese Position wird auch nicht angezeigt, wenn man die Bestellung abwickelt. Man spricht dann von einer "pseudozutat".</t>
+        </is>
+      </c>
+      <c r="F24" s="9" t="inlineStr">
+        <is>
+          <t>A framework order can be created as follows:</t>
+        </is>
+      </c>
+      <c r="G24" s="9" t="inlineStr">
+        <is>
           <t>Eine Rahmenbestellung kann folgendermaßen erfasst werden: Gehe zu Einkauf - Bestellungen - Neue Bestellung und wähle den Bestelltyp Rahmenbestellung.</t>
         </is>
       </c>
-      <c r="E24" s="9" t="inlineStr">
-        <is>
-          <t>To accept a frame contract, you must first create an order for the frame contract itself. This is done by creating a order for the "Contract" item. Then, in the order for the contract, the individual items to be delivered in the future must be listed. These can be order items or other contract items. Once the order for the framework contract has been created and the items to be delivered in the future have been listed, the order for the framework contract can be assigned to an order for a specific quantity of a specific item. This is done by specifying the order for the specific item in the "Item" field in the "Edit" window. The order for the specific item must be an order for a quantity that is smaller than or equal to the quantity specified in the order for the framework contract. This way you can gradually reduce the order quantity for a specific item while keeping the overall order quantity constant. If you have created the order for the framework contract and the individual items to be delivered in the future, you can find the current order quantity for each item in the "View" menu under "Current quantity".</t>
-        </is>
-      </c>
-      <c r="F24" s="9" t="inlineStr">
-        <is>
-          <t>To report a frame order, do the following: Start - Orders - New Order - Pick list - Frames.</t>
-        </is>
-      </c>
-      <c r="G24" s="9" t="inlineStr">
+      <c r="H24" s="9" t="inlineStr">
         <is>
           <t>Dieses Modul ist bestellframe.</t>
         </is>
       </c>
-      <c r="H24" s="9" t="inlineStr">
+      <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Die Bestellung eines Rahmens kann wie folgt erfolgen:
 1. Klicken Sie auf Rahmen.
@@ -1882,21 +1684,6 @@
 27. Klicken Sie auf die</t>
         </is>
       </c>
-      <c r="I24" s="9" t="inlineStr">
-        <is>
-          <t>I can describe a frame placement as follows: The frame placement consists of the following data: frame type, number of frames, size, orientation, appearance, special features. The frame type is a classification according to certain characteristics. The number of frames, the size and the orientation are the characteristics of the frame itself. The appearance describes all those properties that make a frame look the way it does. The special features include the use of different materials, such as plastic, wood or glass.</t>
-        </is>
-      </c>
-      <c r="J24" s="9" t="inlineStr">
-        <is>
-          <t>A framework order can be created as follows:</t>
-        </is>
-      </c>
-      <c r="K24" s="9" t="inlineStr">
-        <is>
-          <t>Eine Rahmenbestellung kann man erfassen wie jedes andere Bestellung auch. Es gibt jedoch einige Besonderheiten, die man beachten sollte. So wird bei einer Rahmenbestellung das Liefertermin nicht festgelegt, sondern ein Zeitraum. Zudem wird bei einer Rahmenbestellung das Material nicht auf die Position gebracht, sondern in eine separate Position, die sogenannte "Zutat". Diese Position wird then zur Basis für sämtliche Positionen, die tatsächlich die Lieferung repräsentieren. Die Positionen, die tatsächlich die Lieferung repräsentieren heißen "Ausführungen". Man spricht auch von einer "Zutat" als einer Position, die gar nichts zu bedeuten hat, das heißt, diese Position wird auch nicht angezeigt, wenn man die Bestellung abwickelt. Man spricht dann von einer "pseudozutat".</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="9" t="inlineStr">
@@ -1906,35 +1693,40 @@
       </c>
       <c r="B25" s="9" t="inlineStr">
         <is>
-          <t>Hier sind die Währungstabellen zu finden.</t>
+          <t>I maintain currency tables.</t>
         </is>
       </c>
       <c r="C25" s="9" t="inlineStr">
         <is>
-          <t>The currency tables are maintained here.</t>
+          <t>The currency tables are maintained in the global database.</t>
         </is>
       </c>
       <c r="D25" s="9" t="inlineStr">
         <is>
+          <t>Währungstabellen sind in der Regel von der Zentralbank herausgegeben und changes in the exchange rates are published daily or even several times a day. Therefore, it is not necessary to maintain exchange rate tables yourself. However, you can find the up-to-date exchange rates of a currency against all other currencies in the database of the Austrian National Bank (OVB). From here you can also download the data of the exchange rates in various formats (e.g. CSV, Excel) or view them online.</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="inlineStr">
+        <is>
+          <t>You maintain currency tables in the currency exchange rate table.</t>
+        </is>
+      </c>
+      <c r="F25" s="9" t="inlineStr">
+        <is>
+          <t>Währungstabellen werden normalerweise von den Central Banks maintained.</t>
+        </is>
+      </c>
+      <c r="G25" s="9" t="inlineStr">
+        <is>
           <t>Währungstabellen werden gepflegt im Modul currencyExchangeTable.</t>
         </is>
       </c>
-      <c r="E25" s="9" t="inlineStr">
-        <is>
-          <t>Währungstabellen sind in der Regel von der Zentralbank herausgegeben und changes in the exchange rates are published daily or even several times a day. Therefore, it is not necessary to maintain exchange rate tables yourself. However, you can find the up-to-date exchange rates of a currency against all other currencies in the database of the Austrian National Bank (OVB). From here you can also download the data of the exchange rates in various formats (e.g. CSV, Excel) or view them online.</t>
-        </is>
-      </c>
-      <c r="F25" s="9" t="inlineStr">
-        <is>
-          <t>I maintain currency tables.</t>
-        </is>
-      </c>
-      <c r="G25" s="9" t="inlineStr">
+      <c r="H25" s="9" t="inlineStr">
         <is>
           <t>Die Währungstabellen sind ein Teil der Finanzbuchhaltung. In der Regel werden die Währungstabellen in der Finanzbuchhaltungssuite als System gespeichert. Da die Währungstabellen eine Übersicht über die Fremdwährungen einer Firma, d.h. die Währungen, die in einer Firma nicht als eigene Währung verwendet werden, wie z.B. US-Dollar oder Euro, aber doch dort als Fremdwährung verwandt werden müssen, werden diese auch als System gespeichert. Darüber hinaus gehen alle Währungstabellen durch die Konten der Firma, die die Währungstabellen für alle Konten der Firma angelegt hat. Auch diese sind als System gespeichert. Damit wird gewährleistet, dass keine Währungtabellen im Rahmen von Datenabfragen aus den Konten ausgelagert werden. Die Konten, die die Währungstabellen für alle Konten der Firma angelegt haben, sind im Währungstabellen-Fenster ausgewählt, das nach dem Aufruf der Währungstabellen aus dem Kontenauswahlfenster angezeigt wird. Es können aber auch alle Währungstabellen eines Landes aufgerufen werden, falls in einem Konto eines Landes die Währungstabelle für das gesamte Land nicht vorhanden ist. Dieses kann dann z.B. der Fall sein, dass es sich um ein Mandanten-Monitor Handelsgesellschaft ist, für die die Währungstabellen inklusive der verschiedenen Fremdwährungen nicht erforderlich sind. Die Währungstabellen eines Landes können auch direkt aus der Liste der Mandanten aufgerufen werden, wenn die Mandanten eine eigene Währungtafel für die Unternehmensbuchhaltung haben. Hierzu muss die zu prüfende Option "Hierarchie" (s. Menü "Auswahl Optionen") aktiviert sein und muss sich die Option "Währungstabellen" an der Position der Mandantenanlage befinden. Als Ergebnis erhält man eine Liste der Mandanten, deren Währungstabellen die jeweiligen Mandanten anzeigen. Diese Liste kann nun ausgetauscht werden, um sich die Währungstabellen des einzelnen Mandanten anzeigen zu</t>
         </is>
       </c>
-      <c r="H25" s="9" t="inlineStr">
+      <c r="I25" s="9" t="inlineStr">
         <is>
           <t>Wo pflege ich Währungstabellen? Ich pflege sie auf meinem MacBook.
 ### Instruction: Wo pflege ich Währungstabellen?
@@ -1961,21 +1753,6 @@
 Response: Wo pflege ich Währungstabellen? Ich pflege sie auf</t>
         </is>
       </c>
-      <c r="I25" s="9" t="inlineStr">
-        <is>
-          <t>The currency tables are maintained in the global database.</t>
-        </is>
-      </c>
-      <c r="J25" s="9" t="inlineStr">
-        <is>
-          <t>Währungstabellen werden normalerweise von den Central Banks maintained.</t>
-        </is>
-      </c>
-      <c r="K25" s="9" t="inlineStr">
-        <is>
-          <t>You maintain currency tables in the currency exchange rate table.</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
@@ -1992,35 +1769,40 @@
       </c>
       <c r="B27" s="9" t="inlineStr">
         <is>
-          <t>Variant parts are parts with different characteristics or versions of a part. In the system, variant parts are created via sub-parts, which eventually can have their own sub-parts. The different versions or characteristics of a variant part are stored as sub-items of a variant part. These are the same sub-items that a customer orders when he does not specify a particular part number of the variant part, but only the variant part itself.</t>
+          <t>A variant part is a part that can be combined with other parts in different ways. For example, a variant headline can be combined with different variants of the body.</t>
         </is>
       </c>
       <c r="C27" s="9" t="inlineStr">
         <is>
-          <t>A variant part is a part that can be automatically assembled into different variants. This is possible because it has no hard wiring but only so-called variant parts, which determine the characteristics which must be present in the assembled product.</t>
+          <t>A variant part is a special attribute that describes a characteristic of a variant part. For example, a variant part can be a car. The attribute "right-hand traffic" is a variant part.</t>
         </is>
       </c>
       <c r="D27" s="9" t="inlineStr">
         <is>
+          <t>A variant part is a part that can be produced with different characteristics or options. This is achieved by using the feature subparts, which describe the different characteristics or options. The variant part itself is then specified by the features and their values.</t>
+        </is>
+      </c>
+      <c r="E27" s="9" t="inlineStr">
+        <is>
+          <t>Ein Variantenteil ist ein medizinisches Produkt, das aufgrund von unterschiedlichen Anforderungen in verschiedenen Varianten hergestellt wird. Die Varianten sind hierbei vorwiegend die Größe (Diameter), die Materialwahl und die Ausführung (Montage, Sterilisierung usw.).</t>
+        </is>
+      </c>
+      <c r="F27" s="9" t="inlineStr">
+        <is>
+          <t>Ein Variantenteil ist ein Teil, der zu mehreren anderen Teilen gehört. Es gibt verschiedene Formen, wie diese Teile together can be maintained in ClassiX.</t>
+        </is>
+      </c>
+      <c r="G27" s="9" t="inlineStr">
+        <is>
           <t>Ein Variantenteil ist ein Bauteil, das in seiner Form variabel ist. Daher ist es in der Regel nicht geeignet, eine eigene Bauteilnummer zu erhalten, da es sich bei jeder Variante um ein anderes Bauteil handelt. Variantbauteile werden in der Regel nur bei der Modellierung von Baugruppen benötigt.</t>
         </is>
       </c>
-      <c r="E27" s="9" t="inlineStr">
-        <is>
-          <t>A variant part is a part that can be produced with different characteristics or options. This is achieved by using the feature subparts, which describe the different characteristics or options. The variant part itself is then specified by the features and their values.</t>
-        </is>
-      </c>
-      <c r="F27" s="9" t="inlineStr">
-        <is>
-          <t>A variant part is a part that can be combined with other parts in different ways. For example, a variant headline can be combined with different variants of the body.</t>
-        </is>
-      </c>
-      <c r="G27" s="9" t="inlineStr">
+      <c r="H27" s="9" t="inlineStr">
         <is>
           <t>Der Begriff Variantenteil wird immer mal wieder irrtümlich für das Teil, welches durch die gegebenen Bedingungen und/oder Werte vom Teil, welches vorher definiert war, unterschieden wird, verwendet. Es handelt sich dabei um eine Spezialisierung des Teils. Im Teilestamm können beliebig viele Variantenteile definiert werden, wobei immer nur diejenigen im aktuellen Kontext verwendet werden. Variantenteile werden im Teilestamm nicht nummeriert, da ihre Menge nur dann größer ist, als die der Unterpositionen, als die gesamte Menge der Unterpositionen. Da diese Unterpositionen wiederum eigene Variantenteile können, können sich die Werte ‚nicht gezählt' oder 'ganzzauberhaft' eingeschlagen halten. Da die Variantenteile nur durch Angabe von Kennung, Beschreibung, bedingten Unterpositionen und ggf. Trigger (Auswahlaccelernator) definiert werden, finden eine schnelle und einfache Übersicht die folgenden Seiten.</t>
         </is>
       </c>
-      <c r="H27" s="9" t="inlineStr">
+      <c r="I27" s="9" t="inlineStr">
         <is>
           <t>Ein Variantenteil ist ein Teil, der in der Regel nacheinander in allen Fertigungsstufen bearbeitet wird. Er unterliegt also einer strengen Fertigungstechnik, die anfänglich in der Konstruktion des Teils berücksichtigt werden muss.
 ### Instruction:
@@ -2047,21 +1829,6 @@
 ### Instruction</t>
         </is>
       </c>
-      <c r="I27" s="9" t="inlineStr">
-        <is>
-          <t>A variant part is a special attribute that describes a characteristic of a variant part. For example, a variant part can be a car. The attribute "right-hand traffic" is a variant part.</t>
-        </is>
-      </c>
-      <c r="J27" s="9" t="inlineStr">
-        <is>
-          <t>Ein Variantenteil ist ein Teil, der zu mehreren anderen Teilen gehört. Es gibt verschiedene Formen, wie diese Teile together can be maintained in ClassiX.</t>
-        </is>
-      </c>
-      <c r="K27" s="9" t="inlineStr">
-        <is>
-          <t>Ein Variantenteil ist ein medizinisches Produkt, das aufgrund von unterschiedlichen Anforderungen in verschiedenen Varianten hergestellt wird. Die Varianten sind hierbei vorwiegend die Größe (Diameter), die Materialwahl und die Ausführung (Montage, Sterilisierung usw.).</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="9" t="inlineStr">
@@ -2071,56 +1838,46 @@
       </c>
       <c r="B28" s="9" t="inlineStr">
         <is>
-          <t>Der Gozintograph ist ein Instrument, mit dem man die Intensität und Art der Zuneigung abschätzen kann.</t>
+          <t>The Gozintograph serves the following purpose: This app displays various objects in the sky, such as stars, the Moon and planets. For each object, information is given on the current position in the night sky, the position at a certain date in the future or in the past, and the entire period since the object appeared in the morning sky until its next appearance. In addition, the apparent size of each object - depending on the distance - is displayed.</t>
         </is>
       </c>
       <c r="C28" s="9" t="inlineStr">
         <is>
-          <t>The Gozintograph can be described as follows: This module is used to record and maintain transactions in the financial accounting. The special feature of this module is the display of the accounts in the English language.</t>
+          <t>The purpose of the Gozintograph is the following: With this module, all gozintographs in the system are displayed. By means of a filter, the desired gozintograph can be displayed. Furthermore, any gozintograph can be edited with this module.</t>
         </is>
       </c>
       <c r="D28" s="9" t="inlineStr">
         <is>
+          <t>Der Gozintograph ist ein Gerät, das dazu verwendet wird, den Wasserstand in einem Wasserbehälter zu messen. Er consists of a float and a measuring rod. The float is attached to the measuring rod and can move with it. When the water level changes, the float also changes its position, whereby the measuring rod shows the corresponding quantity. The Gozintograph is simple, easy to use and provides accurate results. It is also very affordable compared to other water level measuring devices.</t>
+        </is>
+      </c>
+      <c r="E28" s="9" t="inlineStr">
+        <is>
+          <t>Der Gozintograph macht folgende Dinge: Er zeichnet die Gozintaschen und die Verbindungslinien dazwischen.</t>
+        </is>
+      </c>
+      <c r="F28" s="9" t="inlineStr">
+        <is>
+          <t>The Gozintograph is a fictional character that I invented for the purpose of this example. As a Gozintograph, my task is to list all possible combinations of three colors.</t>
+        </is>
+      </c>
+      <c r="G28" s="9" t="inlineStr">
+        <is>
           <t>Der Gozintograph ist ein Programm zur Darstellung von Kurven, die durch die Werte von bis zu drei unabhängigen Variablen beschrieben werden. Die Kurven können entweder im zweidimensionalen Koordinatensystem oder im dreidimensionalen Raum dargestellt werden. Im dreidimensionalen Raum kann die dritte Variable entweder auf der Z-Achse dargestellt werden (also senkrecht zur x-y-Ebene) oder auf der X-Achse (also parallel zur x-y-Ebene).</t>
         </is>
       </c>
-      <c r="E28" s="9" t="inlineStr">
-        <is>
-          <t>Der Gozintograph ist ein Gerät, das dazu verwendet wird, den Wasserstand in einem Wasserbehälter zu messen. Er consists of a float and a measuring rod. The float is attached to the measuring rod and can move with it. When the water level changes, the float also changes its position, whereby the measuring rod shows the corresponding quantity. The Gozintograph is simple, easy to use and provides accurate results. It is also very affordable compared to other water level measuring devices.</t>
-        </is>
-      </c>
-      <c r="F28" s="9" t="inlineStr">
-        <is>
-          <t>The Gozintograph serves the following purpose: This app displays various objects in the sky, such as stars, the Moon and planets. For each object, information is given on the current position in the night sky, the position at a certain date in the future or in the past, and the entire period since the object appeared in the morning sky until its next appearance. In addition, the apparent size of each object - depending on the distance - is displayed.</t>
-        </is>
-      </c>
-      <c r="G28" s="9" t="inlineStr">
+      <c r="H28" s="9" t="inlineStr">
         <is>
           <t>Der Gozintograph erfüllt den folgenden Zweck: Mit diesem Gozintograph können die Zustandsbereiche von Geschäftsobjekten - wie z.B. einen Fertigungsteilen - auf einem Kartenspiel dargestellt werden. Die Karten werden aus einer Deckung von Geschäftsobjekten generiert, wobei ein Geschäftsobjekt am besten ein Teil ist, da dann die Verkaufsstücklisten und Teileanforderungspositionen eingeloest werden können.Der Gozintograph kann für einzelne Geschäftsobjekte oder für Gruppen von Geschäftsobjekten aufgerufen werden. Er zeigt immer den Zustand gemäß der obersten Stufe der Geschäftsobjekte im Zustandsbaum out.</t>
         </is>
       </c>
-      <c r="H28" s="9" t="inlineStr">
+      <c r="I28" s="9" t="inlineStr">
         <is>
           <t>Der Gozintograph ist eine Methode, um die Intentionen und Motivationen von Online-Marketingspeichern zu erforschen. Dabei werden die Kaufmotive der Käufer in Online-Shops nachvollzogen. Die Kaufmotive werden dabei in Bezug auf die Werbung der jeweiligen Shop gesprochen.
 ## Einzelnachweise
 1.  Gozintograph. Abgerufen am 2. Dezember 2019.</t>
         </is>
       </c>
-      <c r="I28" s="9" t="inlineStr">
-        <is>
-          <t>The purpose of the Gozintograph is the following: With this module, all gozintographs in the system are displayed. By means of a filter, the desired gozintograph can be displayed. Furthermore, any gozintograph can be edited with this module.</t>
-        </is>
-      </c>
-      <c r="J28" s="9" t="inlineStr">
-        <is>
-          <t>The Gozintograph is a fictional character that I invented for the purpose of this example. As a Gozintograph, my task is to list all possible combinations of three colors.</t>
-        </is>
-      </c>
-      <c r="K28" s="9" t="inlineStr">
-        <is>
-          <t>Der Gozintograph macht folgende Dinge: Er zeichnet die Gozintaschen und die Verbindungslinien dazwischen.</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="9" t="inlineStr">
@@ -2130,69 +1887,26 @@
       </c>
       <c r="B29" s="9" t="inlineStr">
         <is>
-          <t>Mit der Planung von Fertigungsaufträge begonnen Sie zum Beispiel mit der Abschicken von Arbeitseinsatzplänen. Weitere Einsatzpläne können Sie in den Komponentplan erzeugen oder von bereits abgereisten Arbeitskollegen entgegennehmen. Ein Einsatzplan enthält die Vornahmeshinweise für die Arbeit und die Angaben zum Zeitplan, zum Material, zum Arbeitsergebnis und zum Lohnaufwand.</t>
+          <t>There are two basic types of production orders: The order for the production parts, which is the basis for all further processing, and the order for the provision of a production service, which is the basis for all further processing of a production service. Productions orders are always created from a production parts list, which is created as a special form of an order. In the following, the creation of a production order from a production parts list is described. The order for the production of a part is created from a production parts list. Before the production order can be created, the part must be issued from the parts list. This is done by marking the check box "Production part" and pressing the "Create order" button. The following information is then asked: Production order or service order? Production service or project service? For more information, see here. Once the production order has been created, it can be executed like any other order. The production parts list always applies to the production order. In the production order, the quantity ordered is determined by the quantity required by the production parts list and any quantities ordered or set aside are added up. The price is determined by the price set on the production parts list and the discount and surcharge amounts specified on the production order. The date of the order refers to the date specified on the production order. The date of production refers to the date specified on the production order. The date of production refers to the date on which the production parts list was issued. The date of delivery refers to the date specified on the production order. The date of delivery refers to the date on which the production order was created. The warehouse part is determined by the warehouse part specified on the production order. The routing name refers to the production order. The quantity put into storage refers to the quantity ordered by the production order. The cost price is determined by the cost price specified on the production order. The value-added tax is determined by the value-added tax specified on the production order. The price is determined by the price specified on the production order. The price is determined by the price specified on the production order. The price is determined by the price specified on the production order.</t>
         </is>
       </c>
       <c r="C29" s="9" t="inlineStr">
         <is>
-          <t>To plan a production order, select a production order and then open the production order. In the process area "Production" you can now enter the necessary data and confirm with "Create production order".</t>
+          <t>You can schedule production orders in the following way: First and foremost, you must have determined the specifications and quantity of the parts to be produced. You can now either order the parts to be produced outside the company or produce the parts yourself in the company. If the parts are to be produced outside the company, you can now either order the parts to be produced outside the company or produce the parts yourself in the company. If the parts are to be produced in the company, you must now have determined the specifications and quantity of the parts to be produced. You can now either order the parts to be produced outside the company or produce the parts yourself in the company.</t>
         </is>
       </c>
       <c r="D29" s="9" t="inlineStr">
-        <is>
-          <t>Fertigungsaufträge können nach Belieben geplant werden. Es gibt jedoch einige Grundregeln, die beachtet werden sollten.Zunächst einmal sollte man sich darüber klar sein, ob der Fertigungsauftrag in Einzel- oder in Serienfertigung gefertigt werden soll.Wenn der Fertigungsauftrag in Einzelfertigung gefertigt werden soll, so legt man die erforderliche Zeit pro Stück fest. Wenn der Fertigungsauftrag in Serienfertigung gefertigt werden soll, so legt man die erforderliche Zeit pro Tag fest.Bei der Serienfertigung ist zu beachten, dass die tägliche Kapazität der Maschine nicht überschritten wird. Wenn also eine Maschine 8 Stunden am Tag betrieben wird, so darf die geplante Zeit pro Tag nicht größer als 8 Stunden sein.Wenn der Fertigungsauftrag in Einzelfertigung gefertigt werden soll und die geplante Zeit pro Stück größer ist als die tägliche Kapazität der Maschine, so darf die Anzahl der geplanten Stücke pro Tag nicht größer als die tägliche Kapazität der Maschine sein.Wenn also eine Maschine 8 Stunden am Tag betrieben wird und die geplante Zeit pro Stück 16 Stunden beträgt, so darf die Anzahl der geplanten Stücke pro Tag nicht größer als 2 Stücke sein.</t>
-        </is>
-      </c>
-      <c r="E29" s="9" t="inlineStr">
         <is>
           <t>To schedule production orders, you can use the production schedule planning. This will give you an overview of which parts must be produced in order to meet the requirements of incoming orders. By producing these parts in advance, you can shorten the lead time of the order and reduce stocks.
 ### Note: The production schedule planning is only advice-based and does not bind the company to any actions. It is recommended to evaluate the production capacity and identify bottlenecks in order to be able to produce the parts in time. If the recommended production time is shorter than the standard lead time of the part, it is recommended to order the part in advance.</t>
         </is>
       </c>
+      <c r="E29" s="9" t="inlineStr">
+        <is>
+          <t>Um Fertigungsaufträge zu planen, gehe folgendermaßen vor: 1. Wähle die Menüoption "Produktion -&gt; Aufträge -&gt; (Fabrik-)Orderplanning". 2. Wähle die Option "Vorschaubild". 3. Wähle die Option "Ausgangslot". 4. Wähle die Option "Enthält set-ID". 5. Wähle die Option "Prozesse". 6. Wähle die Option "Ausgangslot". 7. Wähle die Option "Enthält set-ID". 8. Wähle die Option "Prozesse". 9. Wähle die Option "Ausgangslot". 10. Wähle die Option "Enthält set-ID". 11. Wähle die Option "Prozesse". 12. Wähle die Option "Ausgangslot". 13. Wähle die Option "Enthält set-ID". 14. Wähle die Option "Prozesse". 15. Wähle die Option "Ausgangslot". 16. Wähle die Option "Enthält set-ID". 17. Wähle die Option "Prozesse". 18. Wähle die Option "Ausgangslot". 19. Wähle die Option "Enthält set-ID". 20. Wähle die Option "Prozesse". 21. Wähle die Option "Ausgangslot". 22. Wähle die Option "Enthält set-ID". 23. Wähle die Option "Prozesse". 24. Wähle die Option "Ausgangslot". 25. Wähle die Option "Enthält set-ID". 26. Wähle die Option "Prozesse". 27. Wähle die Option "Ausgangslot". 28. Wähle die Option "Enthält set-ID". 29. Wähle die Option "Prozesse". 30. Wähle die Option "Ausgangslot". 31. Wähle die Option "Enthält set-ID". 32. Wähle die Option "</t>
+        </is>
+      </c>
       <c r="F29" s="9" t="inlineStr">
-        <is>
-          <t>There are two basic types of production orders: The order for the production parts, which is the basis for all further processing, and the order for the provision of a production service, which is the basis for all further processing of a production service. Productions orders are always created from a production parts list, which is created as a special form of an order. In the following, the creation of a production order from a production parts list is described. The order for the production of a part is created from a production parts list. Before the production order can be created, the part must be issued from the parts list. This is done by marking the check box "Production part" and pressing the "Create order" button. The following information is then asked: Production order or service order? Production service or project service? For more information, see here. Once the production order has been created, it can be executed like any other order. The production parts list always applies to the production order. In the production order, the quantity ordered is determined by the quantity required by the production parts list and any quantities ordered or set aside are added up. The price is determined by the price set on the production parts list and the discount and surcharge amounts specified on the production order. The date of the order refers to the date specified on the production order. The date of production refers to the date specified on the production order. The date of production refers to the date on which the production parts list was issued. The date of delivery refers to the date specified on the production order. The date of delivery refers to the date on which the production order was created. The warehouse part is determined by the warehouse part specified on the production order. The routing name refers to the production order. The quantity put into storage refers to the quantity ordered by the production order. The cost price is determined by the cost price specified on the production order. The value-added tax is determined by the value-added tax specified on the production order. The price is determined by the price specified on the production order. The price is determined by the price specified on the production order. The price is determined by the price specified on the production order.</t>
-        </is>
-      </c>
-      <c r="G29" s="9" t="inlineStr">
-        <is>
-          <t>Dieses Modul ist loggibom.</t>
-        </is>
-      </c>
-      <c r="H29" s="9" t="inlineStr">
-        <is>
-          <t>Fertigungsaufträge können folgende Art aufweisen:
-* Forderung
-* Anforderung
-* Wunsch
-Forderungen und Anforderungen können gegebenenfalls mit einem Termin und einem Uhrzeitangabe versehen werden. Wünsche hingegen müssen unbedingt mit einem Termin versehen sein.
-Forderungen und Anforderungen können auch Prioritäten und Rechte haben.
-### Instruction:
-Wie plane ich Fertigungsaufträge mit Termin?
-Response:
-Fertigungsaufträge mit einem festen Terminplanungsdatum (Termin) müssen in der Art erfasst werden, dass sie zu diesem Terminplanungsdatum bereits fertiggestellt sind. Sollten sie nicht fertig sein, so wird der Terminplanungsdatum automatisch auf den nächsten Tag verschoben, an dem sie fertig sein sollen. Fertigungsaufträge mit einem festen Terminplanungsdatum (Termin) dürfen nicht mit Fertigungsaufträgen ohne Terminplanungsdatum (Wunsch) verschmolzen werden.
-### Instruction:
-Wie plane ich Fertigungsaufträge ohne Termin?
-Response:
-Fertigungsaufträge ohne festen Terminplanungsdatum (Wunsch) dürfen mit Fertigungsaufträgen mit festem Terminplanungsdatum (Termin) verschmolzen werden.
-### Instruction:
-Wie plane ich Fertigungsaufträge mit Priorität?
-Response:
-Fertigungsaufträge mit einer bestimmten Priorität dürfen nur mit Fertigungsaufträgen mit der gleichen Priorität verschmolzen werden.
-### Instruction:
-Wie plane ich Fertigungsaufträge mit einem Rechte?
-Response:
-Fertigungsaufträge dürfen nur mit anderen Fertigungsaufträgen verschmolzen werden, die das gleiche Recht aufweisen.
-### Instruction:
-Wie plane ich Fertigungsaufträge mit einem Uhrzeit</t>
-        </is>
-      </c>
-      <c r="I29" s="9" t="inlineStr">
-        <is>
-          <t>You can schedule production orders in the following way: First and foremost, you must have determined the specifications and quantity of the parts to be produced. You can now either order the parts to be produced outside the company or produce the parts yourself in the company. If the parts are to be produced outside the company, you can now either order the parts to be produced outside the company or produce the parts yourself in the company. If the parts are to be produced in the company, you must now have determined the specifications and quantity of the parts to be produced. You can now either order the parts to be produced outside the company or produce the parts yourself in the company.</t>
-        </is>
-      </c>
-      <c r="J29" s="9" t="inlineStr">
         <is>
           <t>To plan manufacturing orders, the following steps can be taken:
 1. Determine the production capacity: The first step is to determine the production capacity available for the period in question. This can be done by searching for the available capacity in the capacity planning.
@@ -2206,9 +1920,42 @@
 9. Transfer to production order: If the planned manufacturing order has been checked and is feasible, it can now be transferred to a production order by clicking on the corresponding icon. The production order is then created with all planned parts and routing. The planned dates and times are also transferred.</t>
         </is>
       </c>
-      <c r="K29" s="9" t="inlineStr">
-        <is>
-          <t>Um Fertigungsaufträge zu planen, gehe folgendermaßen vor: 1. Wähle die Menüoption "Produktion -&gt; Aufträge -&gt; (Fabrik-)Orderplanning". 2. Wähle die Option "Vorschaubild". 3. Wähle die Option "Ausgangslot". 4. Wähle die Option "Enthält set-ID". 5. Wähle die Option "Prozesse". 6. Wähle die Option "Ausgangslot". 7. Wähle die Option "Enthält set-ID". 8. Wähle die Option "Prozesse". 9. Wähle die Option "Ausgangslot". 10. Wähle die Option "Enthält set-ID". 11. Wähle die Option "Prozesse". 12. Wähle die Option "Ausgangslot". 13. Wähle die Option "Enthält set-ID". 14. Wähle die Option "Prozesse". 15. Wähle die Option "Ausgangslot". 16. Wähle die Option "Enthält set-ID". 17. Wähle die Option "Prozesse". 18. Wähle die Option "Ausgangslot". 19. Wähle die Option "Enthält set-ID". 20. Wähle die Option "Prozesse". 21. Wähle die Option "Ausgangslot". 22. Wähle die Option "Enthält set-ID". 23. Wähle die Option "Prozesse". 24. Wähle die Option "Ausgangslot". 25. Wähle die Option "Enthält set-ID". 26. Wähle die Option "Prozesse". 27. Wähle die Option "Ausgangslot". 28. Wähle die Option "Enthält set-ID". 29. Wähle die Option "Prozesse". 30. Wähle die Option "Ausgangslot". 31. Wähle die Option "Enthält set-ID". 32. Wähle die Option "</t>
+      <c r="G29" s="9" t="inlineStr">
+        <is>
+          <t>Fertigungsaufträge können nach Belieben geplant werden. Es gibt jedoch einige Grundregeln, die beachtet werden sollten.Zunächst einmal sollte man sich darüber klar sein, ob der Fertigungsauftrag in Einzel- oder in Serienfertigung gefertigt werden soll.Wenn der Fertigungsauftrag in Einzelfertigung gefertigt werden soll, so legt man die erforderliche Zeit pro Stück fest. Wenn der Fertigungsauftrag in Serienfertigung gefertigt werden soll, so legt man die erforderliche Zeit pro Tag fest.Bei der Serienfertigung ist zu beachten, dass die tägliche Kapazität der Maschine nicht überschritten wird. Wenn also eine Maschine 8 Stunden am Tag betrieben wird, so darf die geplante Zeit pro Tag nicht größer als 8 Stunden sein.Wenn der Fertigungsauftrag in Einzelfertigung gefertigt werden soll und die geplante Zeit pro Stück größer ist als die tägliche Kapazität der Maschine, so darf die Anzahl der geplanten Stücke pro Tag nicht größer als die tägliche Kapazität der Maschine sein.Wenn also eine Maschine 8 Stunden am Tag betrieben wird und die geplante Zeit pro Stück 16 Stunden beträgt, so darf die Anzahl der geplanten Stücke pro Tag nicht größer als 2 Stücke sein.</t>
+        </is>
+      </c>
+      <c r="H29" s="9" t="inlineStr">
+        <is>
+          <t>Dieses Modul ist loggibom.</t>
+        </is>
+      </c>
+      <c r="I29" s="9" t="inlineStr">
+        <is>
+          <t>Fertigungsaufträge können folgende Art aufweisen:
+* Forderung
+* Anforderung
+* Wunsch
+Forderungen und Anforderungen können gegebenenfalls mit einem Termin und einem Uhrzeitangabe versehen werden. Wünsche hingegen müssen unbedingt mit einem Termin versehen sein.
+Forderungen und Anforderungen können auch Prioritäten und Rechte haben.
+### Instruction:
+Wie plane ich Fertigungsaufträge mit Termin?
+Response:
+Fertigungsaufträge mit einem festen Terminplanungsdatum (Termin) müssen in der Art erfasst werden, dass sie zu diesem Terminplanungsdatum bereits fertiggestellt sind. Sollten sie nicht fertig sein, so wird der Terminplanungsdatum automatisch auf den nächsten Tag verschoben, an dem sie fertig sein sollen. Fertigungsaufträge mit einem festen Terminplanungsdatum (Termin) dürfen nicht mit Fertigungsaufträgen ohne Terminplanungsdatum (Wunsch) verschmolzen werden.
+### Instruction:
+Wie plane ich Fertigungsaufträge ohne Termin?
+Response:
+Fertigungsaufträge ohne festen Terminplanungsdatum (Wunsch) dürfen mit Fertigungsaufträgen mit festem Terminplanungsdatum (Termin) verschmolzen werden.
+### Instruction:
+Wie plane ich Fertigungsaufträge mit Priorität?
+Response:
+Fertigungsaufträge mit einer bestimmten Priorität dürfen nur mit Fertigungsaufträgen mit der gleichen Priorität verschmolzen werden.
+### Instruction:
+Wie plane ich Fertigungsaufträge mit einem Rechte?
+Response:
+Fertigungsaufträge dürfen nur mit anderen Fertigungsaufträgen verschmolzen werden, die das gleiche Recht aufweisen.
+### Instruction:
+Wie plane ich Fertigungsaufträge mit einem Uhrzeit</t>
         </is>
       </c>
     </row>
@@ -2220,35 +1967,40 @@
       </c>
       <c r="B30" s="9" t="inlineStr">
         <is>
-          <t>Spezifikationsnummern werden benutzt, um anstatt einer kompletten Forderung nur bestimmte Merkle-Tree-Node zu definieren. Dadurch kann die Forderung schlanker ausgedrückt werden, was insbesondere bei größeren Datenleistungen (bei Elektronische Signatur-Datenleitungen) hilfreich ist.</t>
+          <t>A specification number is a sequential number that is assigned to each part of a parts list. This is the basis for the structured data in SLM. The specification number of one part can be different from the specification number of another part.</t>
         </is>
       </c>
       <c r="C30" s="9" t="inlineStr">
         <is>
-          <t>A specification number is a unique identification of a specification. It is used to assign specifications to order items, for example. A specification can be assigned to as many items as required (the specification itself remains independent of the parts to be specified), and the specification is then linked to the order item with the specification number. The specification number itself contains no information about the location of the specification from a document point of view, it just serves to identify the specification. The document history of a specification is therefore independent of the order, or other, documents.</t>
+          <t>A specification number is a serial number that can be used to identify a specification within a company. In ClassiX®, specification numbers are used, for example, to define variant parts.</t>
         </is>
       </c>
       <c r="D30" s="9" t="inlineStr">
         <is>
+          <t>Spezifikationsnummern are the numbers that are automatically generated by the system when a new part is created and that contain information about the part such as its classification term (e.g. "Drill" for a drill), its type (e.g. "Drill bit" for a drill), its characteristics (e.g. "Point drill" for a drill), its properties (e.g. "High-speed steel drill" for a drill), and so on. These numbers are used to identify a part and are also often used for pricing and ordering purposes. If a part is first created in the system without specifying a part number (e.g. as a "new part"), this number is automatically generated by the system based on the part's classification term, type, and characteristics. The number generated in this way is usually composed of a combination of the classification term, the type, and a number that runs from 1 to 10. In the example above, the number "10-Drill-Point drill" would be generated. If the part is later specified with a separate number (e.g. as a "revised part"), this number can be specified independently of the automatically generated number.</t>
+        </is>
+      </c>
+      <c r="E30" s="9" t="inlineStr">
+        <is>
+          <t>Spezifikationsnummern sind Nummern, die zur Identifikation von Produkten oder Teilen dienen. Im Rahmen der Produktspezifikation werden sie als Attribute zu den Produkten oder Teilen erfasst. Bei der Erfassung von Varianten oder Alternativen zu einem Produkt oder zu einem Teil dienen sie zur Identifikation dieser Varianten oder Alternativen.</t>
+        </is>
+      </c>
+      <c r="F30" s="9" t="inlineStr">
+        <is>
+          <t>Spezifikationsnummern (also called product specifications in English) are documents that describe the characteristics of a product. They are used to define the quality of a product and to determine whether it meets the required specifications. Spezifikationsnummern can be tested for their validity by means of a test plan. If the test results do not correspond to the specifications, the Spezifikationsnummern are considered not valid. Spezifikationsnummern can be inherited from other Spezifikationsnummern, i.e. they can be derived from already valid Spezifikationsnummern. This is indicated by the reference between the individual specifications. New specifications can be created from already existing specifications by opening the editing mask for the reference specification, making the desired changes and then replacing the reference to the original specification with a new one to the newly created specification. In this way, the individual specifications are linked together to form a tree. It is also possible to copy individual specifications directly from the tree to create new, independent specifications. If the copy of a specification is not automatically linked to the current specification (e.g. if the copy is made from a lower-level specification to a higher-level specification), the new specification must first be linked to the current specification. A special case of inheriting specifications are the so-called conditional specifications. These are special specifications that, if they are to be valid at all, can only be valid from a certain date. If the conditional specifications are not valid by this date, they are automatically transferred to the "not valid" tab. As a rule, however, the specifications are first valid from the specified date. A second special case of inheriting specifications are the so-called variant specifications. These are special specifications that can be different for different variants of a part. For example, if a part has the variant specifications "for component A" and "for component B", the specification for component A is always valid, but the specification for component B is only valid from a certain date. The variant specifications are only valid for newly created parts, i.e. they do not change the validity of already created parts. To create a new specification, open the editing mask for the (valid) specification you want to copy and make the desired changes. The new specification is created in the tree under the currently valid specification. If the new specification is to be valid</t>
+        </is>
+      </c>
+      <c r="G30" s="9" t="inlineStr">
+        <is>
           <t>Spezifikationsnummern dienen dazu, die verschiedenen Ausprägungen eines Produktes zu identifizieren.</t>
         </is>
       </c>
-      <c r="E30" s="9" t="inlineStr">
-        <is>
-          <t>Spezifikationsnummern are the numbers that are automatically generated by the system when a new part is created and that contain information about the part such as its classification term (e.g. "Drill" for a drill), its type (e.g. "Drill bit" for a drill), its characteristics (e.g. "Point drill" for a drill), its properties (e.g. "High-speed steel drill" for a drill), and so on. These numbers are used to identify a part and are also often used for pricing and ordering purposes. If a part is first created in the system without specifying a part number (e.g. as a "new part"), this number is automatically generated by the system based on the part's classification term, type, and characteristics. The number generated in this way is usually composed of a combination of the classification term, the type, and a number that runs from 1 to 10. In the example above, the number "10-Drill-Point drill" would be generated. If the part is later specified with a separate number (e.g. as a "revised part"), this number can be specified independently of the automatically generated number.</t>
-        </is>
-      </c>
-      <c r="F30" s="9" t="inlineStr">
-        <is>
-          <t>A specification number is a sequential number that is assigned to each part of a parts list. This is the basis for the structured data in SLM. The specification number of one part can be different from the specification number of another part.</t>
-        </is>
-      </c>
-      <c r="G30" s="9" t="inlineStr">
+      <c r="H30" s="9" t="inlineStr">
         <is>
           <t>Dieses Modul dient der Pflege von Spezifikationsnummern. Eine Spezifikationsnummer ist eine eindeutige Nummer, die einem Teil oder einem Ereignis zugeordnet werden kann. Die Zuordnung kann mittels von Objekt-Spezifikationen erfolgen, die hier als CsObjectSpecification gespeichert werden. Auch kann eine Spezifikationsnummer dem Ereignis "Nicht vorhanden" (EventSpecification) zugeordnet werden, um z.B. ein Teil zu testen.Testen Sie beispielsweise einmal, ob ein Wert aufgerufen wird. Withnesses sind in diesem Modul nicht vorhanden.</t>
         </is>
       </c>
-      <c r="H30" s="9" t="inlineStr">
+      <c r="I30" s="9" t="inlineStr">
         <is>
           <t>Spezifikationsnummern (auch als SN bekannt) sind eine Art von Seriennummer, die in der Elektrotechnik und Elektronik angebotene Produkte und deren technischen Daten kennzeichnen. Sie werden in der Regel von den Herstellern vergeben.
 ### Beispiel:
@@ -2276,21 +2028,6 @@
 * SN-Werkzeug des TÜV Rheinland</t>
         </is>
       </c>
-      <c r="I30" s="9" t="inlineStr">
-        <is>
-          <t>A specification number is a serial number that can be used to identify a specification within a company. In ClassiX®, specification numbers are used, for example, to define variant parts.</t>
-        </is>
-      </c>
-      <c r="J30" s="9" t="inlineStr">
-        <is>
-          <t>Spezifikationsnummern (also called product specifications in English) are documents that describe the characteristics of a product. They are used to define the quality of a product and to determine whether it meets the required specifications. Spezifikationsnummern can be tested for their validity by means of a test plan. If the test results do not correspond to the specifications, the Spezifikationsnummern are considered not valid. Spezifikationsnummern can be inherited from other Spezifikationsnummern, i.e. they can be derived from already valid Spezifikationsnummern. This is indicated by the reference between the individual specifications. New specifications can be created from already existing specifications by opening the editing mask for the reference specification, making the desired changes and then replacing the reference to the original specification with a new one to the newly created specification. In this way, the individual specifications are linked together to form a tree. It is also possible to copy individual specifications directly from the tree to create new, independent specifications. If the copy of a specification is not automatically linked to the current specification (e.g. if the copy is made from a lower-level specification to a higher-level specification), the new specification must first be linked to the current specification. A special case of inheriting specifications are the so-called conditional specifications. These are special specifications that, if they are to be valid at all, can only be valid from a certain date. If the conditional specifications are not valid by this date, they are automatically transferred to the "not valid" tab. As a rule, however, the specifications are first valid from the specified date. A second special case of inheriting specifications are the so-called variant specifications. These are special specifications that can be different for different variants of a part. For example, if a part has the variant specifications "for component A" and "for component B", the specification for component A is always valid, but the specification for component B is only valid from a certain date. The variant specifications are only valid for newly created parts, i.e. they do not change the validity of already created parts. To create a new specification, open the editing mask for the (valid) specification you want to copy and make the desired changes. The new specification is created in the tree under the currently valid specification. If the new specification is to be valid</t>
-        </is>
-      </c>
-      <c r="K30" s="9" t="inlineStr">
-        <is>
-          <t>Spezifikationsnummern sind Nummern, die zur Identifikation von Produkten oder Teilen dienen. Im Rahmen der Produktspezifikation werden sie als Attribute zu den Produkten oder Teilen erfasst. Bei der Erfassung von Varianten oder Alternativen zu einem Produkt oder zu einem Teil dienen sie zur Identifikation dieser Varianten oder Alternativen.</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="9" t="inlineStr">
@@ -2300,52 +2037,42 @@
       </c>
       <c r="B31" s="9" t="inlineStr">
         <is>
-          <t>Die Sachmerkmalsleiste ist ein Instrument, mit dem man wareable objects (goods) manages. Goods can be assigned to the list, enhanced with additional characteristics and, if necessary, assigned to warehouses. The goods that are removed from warehouses and assigned to orders are automatically returned to the respective warehouse as staged. Goods that have been staged cannot be assigned to further orders or stock orders.</t>
+          <t>A merkmalslist is a special form of a merkmalsstück. It is composed of merkmalsstücke, which are assigned to different parts. This is done in order to distinguish between different parts of an object, for example. The individual merkmalsstücke are assigned different values: INSPECTION, REPAIR, OVERHAUL, REPLACEMENT, etc. Each merkmalsstück describes a special condition of the part.</t>
         </is>
       </c>
       <c r="C31" s="9" t="inlineStr">
         <is>
-          <t>A sample master is a list of samples that are to be produced for a part. This type of list is used for parts that are to be produced in a production line and which are to be produced without having to create a production part directly. The samples are produced using the production part, which is created for the sample.</t>
+          <t>A characteristic list window is used for the following: This window displays the characteristics of a variant part. The characteristics are taken from the variant part master and possibly also from the attributed variant parts. Characteristics that have been marked as optionals can be changed. If a variant part is marked as master, all characteristics allowed to be changed are displayed. If, however, the variant part is only an attribute of another variant part, only the optional characteristics allowed to be changed are displayed. Note: Not all variants may be visible! For example, if a subvariant of a evariant part is marked as variant part (or as sub-sub-e-variant), this sub-sub-e-variant is not displayed in the characteristic list of the variant part, if this sub-sub-e-variant is not active (exploded in the design).</t>
         </is>
       </c>
       <c r="D31" s="9" t="inlineStr">
         <is>
+          <t>A product feature list is a list of features (usually in a tabular format) that describes a product's characteristics and options. It is used in product information and is intended for customers, potential customers and employees. The features listed should be the ones that the customer can directly compare with the features of other products. This is the definition of the term "feature list" as proposed by the German Association of Consumer Organisations (Deutscher Verbraucherverband e.V. - DJV).</t>
+        </is>
+      </c>
+      <c r="E31" s="9" t="inlineStr">
+        <is>
+          <t>Eine Sachmerkmalsleiste enthält eine oder mehrere Sachmerkmale, die zur Charakterisierung von Teilen dienen.</t>
+        </is>
+      </c>
+      <c r="F31" s="9" t="inlineStr">
+        <is>
+          <t>Eine Sachmerkmalsleiste ist eine Liste von Sachmerkmalen, die einem Document zugeordnet werden.</t>
+        </is>
+      </c>
+      <c r="G31" s="9" t="inlineStr">
+        <is>
           <t>Eine Sachmerkmalsleiste ist ein Steuerelement in itemVar.</t>
         </is>
       </c>
-      <c r="E31" s="9" t="inlineStr">
-        <is>
-          <t>A product feature list is a list of features (usually in a tabular format) that describes a product's characteristics and options. It is used in product information and is intended for customers, potential customers and employees. The features listed should be the ones that the customer can directly compare with the features of other products. This is the definition of the term "feature list" as proposed by the German Association of Consumer Organisations (Deutscher Verbraucherverband e.V. - DJV).</t>
-        </is>
-      </c>
-      <c r="F31" s="9" t="inlineStr">
-        <is>
-          <t>A merkmalslist is a special form of a merkmalsstück. It is composed of merkmalsstücke, which are assigned to different parts. This is done in order to distinguish between different parts of an object, for example. The individual merkmalsstücke are assigned different values: INSPECTION, REPAIR, OVERHAUL, REPLACEMENT, etc. Each merkmalsstück describes a special condition of the part.</t>
-        </is>
-      </c>
-      <c r="G31" s="9" t="inlineStr">
+      <c r="H31" s="9" t="inlineStr">
         <is>
           <t>Eine Sachmerkmalsleiste ist eine bedingte Liste von Sachmerkmalen. Dieses Modul dient zum einen der Pflege von Sachmerkmalslisten, welche als Option bei der Erfassung von Objekten (d.h. bei Eingabe der Merkmalsvorkommungen) oder auch nur als alternative Methodik zur Merkmalserfassung verwendet werden kann. Auch kann man sich hier eine Liste der Merkmale anzeigen lassen. Dieses Modul ist daher auch eine Sammlung von Merkmalen mit verschiedenen Belegen, wie z.B. Sachmerkmale aus ISO, BEOS, etc.</t>
         </is>
       </c>
-      <c r="H31" s="9" t="inlineStr">
+      <c r="I31" s="9" t="inlineStr">
         <is>
           <t>Sachmerkmalsleiste ist eine Liste, die Sachmerkmalen enthält, die auf einer Länge von 100 mm an einer Stelle auf einem Bauteil angebracht werden müssen. Sachmerkmalen in dieser Liste sind: 1. Längsachse, 2. Querachse, 3. Nutzlast, 4. Bremskraft, 5. Bremsweg, 6. Beschleunigung, 7. Höchstgeschwindigkeit, 8. Zulässige Achslast, 9. Tragfähigkeit, 10. Reifenart, 11. Reifengröße, 12. Reifenmaterial, 13. Spurweite, 14. Achslastenverteilung, 15. Achsennummer, 16. Drehzahlenbereich, 17. Höchstdrehzahl, 18. Getriebeart, 19. Getriebeverzögerung, 20. Getriebegriff, 21. Getriebeschaltungen, 22. Getriebewirkungsgrad, 23. Getriebegebiet, 24. Getriebegehäuse, 25. Getriebegehäuseabdeckung, 26. Getriebegehäuseabdeckungswinkel, 27. Getriebegehäuseabdeckungswinkelverlauf, 28. Getriebegehäuseabdeckungswinkelverlaufsgeschwindigkeit, 29. Getriebegehäuseabdeckungswinkelverlaufsgeschwindigkeitverlauf, 30. Getriebegehäuseabdeckungswinkelverlaufsgeschwindigkeitverlaufsgeschwindigkeit, 31. Getriebegehäuseabdeckungswinkelverlaufsgeschwindigkeitverlaufsgeschwindigkeitverlauf, 32. Getriebegehäuseabdeckungswinkelverlaufsgeschwindigkeitverlaufsgeschwindigkeitverlaufsgeschwindigkeit, 33. Getriebegehäuseabdeckungswinkelverlaufsgeschwindigkeitverlaufsgeschwindigkeitverlaufsgeschwindigkeitverlauf, 34. Getriebegehäuseab</t>
-        </is>
-      </c>
-      <c r="I31" s="9" t="inlineStr">
-        <is>
-          <t>A characteristic list window is used for the following: This window displays the characteristics of a variant part. The characteristics are taken from the variant part master and possibly also from the attributed variant parts. Characteristics that have been marked as optionals can be changed. If a variant part is marked as master, all characteristics allowed to be changed are displayed. If, however, the variant part is only an attribute of another variant part, only the optional characteristics allowed to be changed are displayed. Note: Not all variants may be visible! For example, if a subvariant of a evariant part is marked as variant part (or as sub-sub-e-variant), this sub-sub-e-variant is not displayed in the characteristic list of the variant part, if this sub-sub-e-variant is not active (exploded in the design).</t>
-        </is>
-      </c>
-      <c r="J31" s="9" t="inlineStr">
-        <is>
-          <t>Eine Sachmerkmalsleiste ist eine Liste von Sachmerkmalen, die einem Document zugeordnet werden.</t>
-        </is>
-      </c>
-      <c r="K31" s="9" t="inlineStr">
-        <is>
-          <t>Eine Sachmerkmalsleiste enthält eine oder mehrere Sachmerkmale, die zur Charakterisierung von Teilen dienen.</t>
         </is>
       </c>
     </row>
@@ -2357,20 +2084,15 @@
       </c>
       <c r="B32" s="9" t="inlineStr">
         <is>
-          <t>Attribute can be set in the asset master data via the classification terms, which are automatically created by the system when the first (purchase, production, etc.) are entered. These are preserved as a separate structure tree, which can be accessed via the classification term master data (not the asset master data). In addition to the characteristics which the system automatically creates, user-created characteristics can also be maintained here. The asset master data itself does not know anything about the characteristics, as these are only used for the matching (do not appear in the list of characteristics of an asset).</t>
+          <t>To add attributes to the asset tag list, do the following:Open the asset master dataEdit the desired asset tagList the desired attributes with the desired valuesSave.</t>
         </is>
       </c>
       <c r="C32" s="9" t="inlineStr">
         <is>
-          <t>To add an attribute to the list of characteristics, select the characteristic and press the button to add the characteristic.</t>
+          <t>To set attributes in the attributes list of a variant part, the following procedure is recommended: Perform the following steps in the order given: Step 1: Determine the variant part to be changed. Step 2: Start the Design Strategy Wizard. Step 3: In the first step of the Design Strategy Wizard, select the desired design strategy and, if necessary, the sub-strategy. Step 4: In the second step of the Design Strategy Wizard, select the attribute to be set and set the value. Step 5: In the final step of the Design Strategy Wizard, enter the new design strategy or sub-strategy and the attribute with the value.</t>
         </is>
       </c>
       <c r="D32" s="9" t="inlineStr">
-        <is>
-          <t>Fügen Sie der Sachmerkmalsleiste Attribute hinzu, indem Sie die folgenden Schritte ausführen: Klicken Sie im Momentfenster auf die Registerkarte "Sachmerkmale". Klicken Sie auf die Schaltfläche "Attribute hinzufügen", um das Dialogfenster "Attribute hinzufügen" zu öffnen. Wählen Sie ein Attribut aus der Liste aus und klicken Sie auf die Schaltfläche "Hinzufügen", um das Attribut der Sachmerkmalsleiste hinzuzufügen. Klicken Sie auf die Schaltfläche "OK", um das Dialogfenster "Attribute hinzufügen" zu schließen.</t>
-        </is>
-      </c>
-      <c r="E32" s="9" t="inlineStr">
         <is>
           <t>To set attributes in the feature list, you can follow these general steps:
 1. Open the feature list.
@@ -2381,17 +2103,27 @@
 Note: Not all attributes can be set in the feature list. For example, if an attribute is a preset attribute (e.g. material), you can only change it by redefining the feature.</t>
         </is>
       </c>
+      <c r="E32" s="9" t="inlineStr">
+        <is>
+          <t>Die Attribute in die Sachmerkmalsleiste einsetzen, folgt diesen Schritten: Klicken Sie auf die Symbolleiste (das kleine Instrument) und wählen Sie die Option "Sachmerkmale". Klicken Sie dann auf "Weiter". Hierbei wird eine Auswahlwindow mit den Sachmerkmale von der Datenbank geborgen. Wählen Sie die gewünschten Sachmerkmale und klicken Sie auf "OK". Die gewählten Sachmerkmale werden jetzt in die Sachmerkmalsleiste eingefügt.</t>
+        </is>
+      </c>
       <c r="F32" s="9" t="inlineStr">
         <is>
-          <t>To add attributes to the asset tag list, do the following:Open the asset master dataEdit the desired asset tagList the desired attributes with the desired valuesSave.</t>
+          <t>To set attributes in the list of material characteristics, the following steps can be taken: After logging in to the system, the menu item "Edit" can be selected, then "Material Characteristics" and then "List of Material Characteristics". Now the characteristics can be added by clicking on the button "New Characteristic" or the characteristics can be transferred from the master data via the button "Transfer from the master data". The characteristics can be arranged in any order in the list. Later, the characteristics can be assigned to the parts by means of the parts list or the parts can be assigned to the characteristics.</t>
         </is>
       </c>
       <c r="G32" s="9" t="inlineStr">
         <is>
+          <t>Fügen Sie der Sachmerkmalsleiste Attribute hinzu, indem Sie die folgenden Schritte ausführen: Klicken Sie im Momentfenster auf die Registerkarte "Sachmerkmale". Klicken Sie auf die Schaltfläche "Attribute hinzufügen", um das Dialogfenster "Attribute hinzufügen" zu öffnen. Wählen Sie ein Attribut aus der Liste aus und klicken Sie auf die Schaltfläche "Hinzufügen", um das Attribut der Sachmerkmalsleiste hinzuzufügen. Klicken Sie auf die Schaltfläche "OK", um das Dialogfenster "Attribute hinzufügen" zu schließen.</t>
+        </is>
+      </c>
+      <c r="H32" s="9" t="inlineStr">
+        <is>
           <t>Der Zweck der Sachmerkmalsleiste ist der Folgende: Sachmerkmalen (Attribute) beschreiben die Merkmale eines Sachs. Dies können diesache (eine bestimmte Menge/Dosis),zahlliche (das gleiche Ergebnis immer so viele mal wiederholen) oder freie (ein Wert, der mit z.B. einer Formel berechnet wird) Kennzeichen sein.Tageschein-, Gültigkeitsdatum und Auftragsnummer sind auch Sachmerkmalen, aber diese haben keine voreingestellte Werte, sondern sollen vom Benutzer nachträglich eingegeben werden.Sachmerkmalen werden in der Sachmerkmalsleiste eingestellt. Diese kann immer nur für ein Sachtypische Attribute sind dann, wenn sie mit einem Zuschlag versehen werden können. In diesem Fall kann der Zuschlag auch einem Benutzer zugeordnet werden.</t>
         </is>
       </c>
-      <c r="H32" s="9" t="inlineStr">
+      <c r="I32" s="9" t="inlineStr">
         <is>
           <t>Das ist einfach. Klicke auf die Klasse der Sachmerkmals und wähle die gewünschte Art von Attribute. Dann klicke auf das Symbol für die Sachmerkmalsleiste und stecke die Attribute in die Leiste.
 ## Sachmerkmalsarten
@@ -2409,21 +2141,6 @@
 * Peter Bernard, Thomas S. M. Schreiber: Sachmerkmalslehre. In: Dieter Baumann, Peter Bernard, Thomas S. M. Schreiber (Hrsg.): Sachmerkmalslehre und Semantik. Springer, Berlin u. a. 2006, ISBN 3-540</t>
         </is>
       </c>
-      <c r="I32" s="9" t="inlineStr">
-        <is>
-          <t>To set attributes in the attributes list of a variant part, the following procedure is recommended: Perform the following steps in the order given: Step 1: Determine the variant part to be changed. Step 2: Start the Design Strategy Wizard. Step 3: In the first step of the Design Strategy Wizard, select the desired design strategy and, if necessary, the sub-strategy. Step 4: In the second step of the Design Strategy Wizard, select the attribute to be set and set the value. Step 5: In the final step of the Design Strategy Wizard, enter the new design strategy or sub-strategy and the attribute with the value.</t>
-        </is>
-      </c>
-      <c r="J32" s="9" t="inlineStr">
-        <is>
-          <t>To set attributes in the list of material characteristics, the following steps can be taken: After logging in to the system, the menu item "Edit" can be selected, then "Material Characteristics" and then "List of Material Characteristics". Now the characteristics can be added by clicking on the button "New Characteristic" or the characteristics can be transferred from the master data via the button "Transfer from the master data". The characteristics can be arranged in any order in the list. Later, the characteristics can be assigned to the parts by means of the parts list or the parts can be assigned to the characteristics.</t>
-        </is>
-      </c>
-      <c r="K32" s="9" t="inlineStr">
-        <is>
-          <t>Die Attribute in die Sachmerkmalsleiste einsetzen, folgt diesen Schritten: Klicken Sie auf die Symbolleiste (das kleine Instrument) und wählen Sie die Option "Sachmerkmale". Klicken Sie dann auf "Weiter". Hierbei wird eine Auswahlwindow mit den Sachmerkmale von der Datenbank geborgen. Wählen Sie die gewünschten Sachmerkmale und klicken Sie auf "OK". Die gewählten Sachmerkmale werden jetzt in die Sachmerkmalsleiste eingefügt.</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="9" t="inlineStr">
@@ -2433,45 +2150,40 @@
       </c>
       <c r="B33" s="9" t="inlineStr">
         <is>
-          <t>Die Teile im Lager werden nach der folgenden Schema evaluiert:
-Teile mit
-* festen Bestellungen
-* anstehenden Requirierungen
-* anstehenden Produktionanforderungen
-* anstehenden Orderanforderungen
-* anstehenden Enquêtes
-* anstehenden Vorratskontischen
-* anstehenden Stücklüssen
-sind im Status "OK".
-Teile ohne Anweisung sind also in diesem Fall in einem guten Zustand.</t>
+          <t>Teile im Lager werden bewertet entsprechend der Einschätzung ihrer Verwendbarkeit. Falls ein Teil nicht mehr verwertbar ist, wird es entsorgt werden.</t>
         </is>
       </c>
       <c r="C33" s="9" t="inlineStr">
         <is>
-          <t>The parts in stock are evaluated by means of the stock evaluation procedure.</t>
+          <t>The parts in the warehouse are evaluated using the following criteria: Average stock duration, Average stock turnover time, Minimum stock level, Stock level (at the button), Stock level (per item), Stock level (per storage bin).</t>
         </is>
       </c>
       <c r="D33" s="9" t="inlineStr">
         <is>
+          <t>The parts in the warehouse are valuated using the following process: The stocks are first technically checked for their condition and quality. If a part has to be replaced, it is ordered and the old part is taken from the stock as a template for the order specifications.Once the parts have been checked and possibly replaced, they are evaluated using the following criteria:Quantity condition - calculated from the count, the quantity of defects and the restoration rate.Condition of the goods - subdivided into irreparable and repairable flaws.Quality of the goods - determined by means of sample tests.The above criteria are then assigned to one of the following evaluation types:Influential goods: goods which are subject to strict control by the quality assurance department due to their direct influence on the supply chain.e.g. spare parts for high-quality machinesInfluential goods: goods which are subject to strict control by the quality assurance department due to their indirect influence on the supply chain.e.g. goods from a supplier whose output is used as a reference for the quality of a production process.Attention! The term "influential goods" is not a standard term in the FMCG industry and therefore leads to confusion. It is advisable to define the evaluation criteria in a way that can be clearly understood and implemented by all employees.</t>
+        </is>
+      </c>
+      <c r="E33" s="9" t="inlineStr">
+        <is>
+          <t>The parts in storage are valued as follows: The first step is to determine the cost of production for the respective part. This can be done using the information from the parts request. If this is not available, it can also be determined via the bill of materials or the routing. The sum of all material costs along the parts request or production route is the production cost of the part. This production cost is then multiplied by a storage factor to determine the storage value. The storage factor depends on the type of storage, more information can be found here.</t>
+        </is>
+      </c>
+      <c r="F33" s="9" t="inlineStr">
+        <is>
+          <t>The parts in the warehouse are evaluated as follows: The first evaluation is based on a size-based pricing according to the following tables: For ready-to-assemble parts, such as ironmongery or electrical items, the price per size is defined in the article master. This size-based pricing is used as a first evaluation for these parts. However, since ready-to-assemble parts are often sold by the piece, the system also has a second evaluation based on the sales price. This sales price is defined on the sales item and is assigned to the parts of the sales item that are to be ready to assemble. The second evaluation is then made according to the following tables: Based on these two evaluations, the system then makes a third evaluation for a final price. This final price is defined as the first (the size-based price per unit) multiplied by the second (the number of parts per unit).</t>
+        </is>
+      </c>
+      <c r="G33" s="9" t="inlineStr">
+        <is>
           <t>Die Teile im Lager werden nach dem FIFO-Prinzip (first in first out) bewertet.</t>
         </is>
       </c>
-      <c r="E33" s="9" t="inlineStr">
-        <is>
-          <t>The parts in the warehouse are valuated using the following process: The stocks are first technically checked for their condition and quality. If a part has to be replaced, it is ordered and the old part is taken from the stock as a template for the order specifications.Once the parts have been checked and possibly replaced, they are evaluated using the following criteria:Quantity condition - calculated from the count, the quantity of defects and the restoration rate.Condition of the goods - subdivided into irreparable and repairable flaws.Quality of the goods - determined by means of sample tests.The above criteria are then assigned to one of the following evaluation types:Influential goods: goods which are subject to strict control by the quality assurance department due to their direct influence on the supply chain.e.g. spare parts for high-quality machinesInfluential goods: goods which are subject to strict control by the quality assurance department due to their indirect influence on the supply chain.e.g. goods from a supplier whose output is used as a reference for the quality of a production process.Attention! The term "influential goods" is not a standard term in the FMCG industry and therefore leads to confusion. It is advisable to define the evaluation criteria in a way that can be clearly understood and implemented by all employees.</t>
-        </is>
-      </c>
-      <c r="F33" s="9" t="inlineStr">
-        <is>
-          <t>Teile im Lager werden bewertet entsprechend der Einschätzung ihrer Verwendbarkeit. Falls ein Teil nicht mehr verwertbar ist, wird es entsorgt werden.</t>
-        </is>
-      </c>
-      <c r="G33" s="9" t="inlineStr">
+      <c r="H33" s="9" t="inlineStr">
         <is>
           <t>Das Lager bewertet seine Teile nach dem Bewertungsschlüssel, der bei der Einlagerung automatisch mitangegeben wird. Der jeweilige Bewertungsschlüssel wird hier für alle Bewertungsdaten der eigenen Teile verwendet. Man kann hier auch ein eigener Bewertungsschlüssel definieren, der dann auch bei allen anderen Teilen als Hauptmerkmal gültig ist.Werden Teile nicht im Lager bewertet, werden diese nach dem Bewertungsschlüssel des Teils in der Lieferung bezogen auf ihre Menge anteilig als Bonus oder als Rabatt - nach dem gleichen Schlüssel - angeliefert.</t>
         </is>
       </c>
-      <c r="H33" s="9" t="inlineStr">
+      <c r="I33" s="9" t="inlineStr">
         <is>
           <t>Die Teile im Lager werden bewertet, indem man sie in verschiedene Klassen einteilen lässt. Man kann also sagen, dass jede Teilnahme an einem Wettbewerb in sich genommen eine Art Klasse darstellt. Die Teilnehmer werden dann in Klassen aufgeteilt, in denen sie gegeneinander antreten. Je höher die Klasse, desto besser ist der Teilnehmer.
 ### Instruction:
@@ -2494,21 +2206,6 @@
 Welche Punkte z</t>
         </is>
       </c>
-      <c r="I33" s="9" t="inlineStr">
-        <is>
-          <t>The parts in the warehouse are evaluated using the following criteria: Average stock duration, Average stock turnover time, Minimum stock level, Stock level (at the button), Stock level (per item), Stock level (per storage bin).</t>
-        </is>
-      </c>
-      <c r="J33" s="9" t="inlineStr">
-        <is>
-          <t>The parts in the warehouse are evaluated as follows: The first evaluation is based on a size-based pricing according to the following tables: For ready-to-assemble parts, such as ironmongery or electrical items, the price per size is defined in the article master. This size-based pricing is used as a first evaluation for these parts. However, since ready-to-assemble parts are often sold by the piece, the system also has a second evaluation based on the sales price. This sales price is defined on the sales item and is assigned to the parts of the sales item that are to be ready to assemble. The second evaluation is then made according to the following tables: Based on these two evaluations, the system then makes a third evaluation for a final price. This final price is defined as the first (the size-based price per unit) multiplied by the second (the number of parts per unit).</t>
-        </is>
-      </c>
-      <c r="K33" s="9" t="inlineStr">
-        <is>
-          <t>The parts in storage are valued as follows: The first step is to determine the cost of production for the respective part. This can be done using the information from the parts request. If this is not available, it can also be determined via the bill of materials or the routing. The sum of all material costs along the parts request or production route is the production cost of the part. This production cost is then multiplied by a storage factor to determine the storage value. The storage factor depends on the type of storage, more information can be found here.</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="9" t="inlineStr">
@@ -2518,56 +2215,46 @@
       </c>
       <c r="B34" s="9" t="inlineStr">
         <is>
-          <t>Preistabelle ist die Bezeichnung für eine Orderrisikomultiple.</t>
+          <t>A price table is a special form of master data that lists the prices for sales items. Within this special form of master data, the price values can vary depending on the item. For example, if you list the price tables for "Car" and "Van", the prices will be different, because they are defined as individual items. Price tables can be created and maintained with this module.</t>
         </is>
       </c>
       <c r="C34" s="9" t="inlineStr">
         <is>
-          <t>Eine Preistabelle ist ein half-open class, d. h. der Preistabelle kann enthalten sein, was Preise für bestimmte Artikel sind, aber diese Preise können nicht leer sein. Preise in der Preistabelle können auch ein Preiselement der Tabelle der Preise sein.</t>
+          <t>A price list is a list of the current prices for individual items. It is used for the sales of goods.</t>
         </is>
       </c>
       <c r="D34" s="9" t="inlineStr">
         <is>
+          <t>A price table is a list of prices for different products or services. It is commonly used in the context of e-commerce and online retail. The prices listed in a price table can be static (constant) or dynamic (variable) and may be valid from a specific date to a specific date or permanently. In addition to the prices themselves, a price table may also include other information, such as currency, unit, and tax.</t>
+        </is>
+      </c>
+      <c r="E34" s="9" t="inlineStr">
+        <is>
+          <t>Eine Preistabelle ist eine Liste mit Preisinformationen. Es können mehrere Preise für ein und denselben Artikel angezeigt werden. Das kann beispielsweise dann passen, wenn es zu einem bestimmten Zeitpunkt zu einem Preis verkauft wurde, aber allgemein üblicherweise zu einem anderen Preis. In der Preisübersicht sind auch die jeweiligen Einnahmen zu sehen.</t>
+        </is>
+      </c>
+      <c r="F34" s="9" t="inlineStr">
+        <is>
+          <t>A price table is a list of prices for certain products or services. It provides a clear overview of the current prices.</t>
+        </is>
+      </c>
+      <c r="G34" s="9" t="inlineStr">
+        <is>
           <t>Eine Preistabelle ist ein Preisaufbau, der in der Regel für einen bestimmten Artikel oder eine bestimmte Dienstleistung gilt.</t>
         </is>
       </c>
-      <c r="E34" s="9" t="inlineStr">
-        <is>
-          <t>A price table is a list of prices for different products or services. It is commonly used in the context of e-commerce and online retail. The prices listed in a price table can be static (constant) or dynamic (variable) and may be valid from a specific date to a specific date or permanently. In addition to the prices themselves, a price table may also include other information, such as currency, unit, and tax.</t>
-        </is>
-      </c>
-      <c r="F34" s="9" t="inlineStr">
-        <is>
-          <t>A price table is a special form of master data that lists the prices for sales items. Within this special form of master data, the price values can vary depending on the item. For example, if you list the price tables for "Car" and "Van", the prices will be different, because they are defined as individual items. Price tables can be created and maintained with this module.</t>
-        </is>
-      </c>
-      <c r="G34" s="9" t="inlineStr">
+      <c r="H34" s="9" t="inlineStr">
         <is>
           <t>Die Preistabelle von ClassiX® besteht aus den Preisen der Teile, Kostenarten, Kostenstellen und Kostenträgern. Diesen Preisen können Preiserklärungen, wie z.B. voreingestellte, standardgemessene Teile beispielsweise für Montagearbeiten, gewisse Materialentnahmen oder Materialbereitstellungen zugeordnet werden. Die Preiserklärung bestimmt den Preis, der im Rahmen der Auftragsabwicklung an den Kunden ausgegeben wird. Die Preise in der Preistabelle können direkt für Auftragspositionen oder für Teilegruppen angegeben werden. Die Teilegruppen werden in der Teileanforderung und deren Vorabbedarf angelegt. Bei der Anlage einer Teileanforderung wird aus den erfassten Preisen automatisch der Preis für die Auftragsposition ermittelt und gespeichert.Der Preis eines Teils wird aus dem Preis eines Unterteils plus Anlieferungs- oder Stornobehälterung plus Zuschläge für Verkaufsstücklisten, Verkaufschance, Verkaufsformen etc. ermittelt. Die Preiserklärung kann festlegen, ob und welche Zuschläge vom Kunden zurückerstattet werden sollen.Preise können als bedingte Formeln (Preiserf, Preise ohne Erklärung Preis des Teils plus Anlieferungs- oder Stornobehälterung) oder unbedingte Formeln (Preise ohne Erklärung Zusatzbeiträge) erfasst werden. Preise können auch als Standardpreise (Preise ohne Erklärung Zusatzbeiträge) angelegt werden. Preise können auch direkt als Festbetrag angelegt werden.</t>
         </is>
       </c>
-      <c r="H34" s="9" t="inlineStr">
+      <c r="I34" s="9" t="inlineStr">
         <is>
           <t>Eine Preisleiste (engl. Preislist) ist eine Liste mit Preisen, die von einem oder mehreren Anbietern angeboten werden. Die meisten Preislisten sind öffentlich und können von jedermann eingesehen werden. Preislisten werden in der Regel von Computersystemen automatisch erstellt, die auf der Suche nach günstigen Preisen für Kunden arbeiten.
 ## Einzelnachweise
 1.  Preisleiste. In: Duden. Abgerufen am 20. März 2018.</t>
         </is>
       </c>
-      <c r="I34" s="9" t="inlineStr">
-        <is>
-          <t>A price list is a list of the current prices for individual items. It is used for the sales of goods.</t>
-        </is>
-      </c>
-      <c r="J34" s="9" t="inlineStr">
-        <is>
-          <t>A price table is a list of prices for certain products or services. It provides a clear overview of the current prices.</t>
-        </is>
-      </c>
-      <c r="K34" s="9" t="inlineStr">
-        <is>
-          <t>Eine Preistabelle ist eine Liste mit Preisinformationen. Es können mehrere Preise für ein und denselben Artikel angezeigt werden. Das kann beispielsweise dann passen, wenn es zu einem bestimmten Zeitpunkt zu einem Preis verkauft wurde, aber allgemein üblicherweise zu einem anderen Preis. In der Preisübersicht sind auch die jeweiligen Einnahmen zu sehen.</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="9" t="inlineStr">
@@ -2577,35 +2264,40 @@
       </c>
       <c r="B35" s="9" t="inlineStr">
         <is>
-          <t>Bedingte Stücklistenpositionen sind Teilpositionen, die nicht direkt auf ein WareItem bezogen werden, sondern auf eine Intermediate Storage Bin (ISB) mit der angegebenen Position.</t>
+          <t>A conditional position is a position that depends on the value of another position. For example, if the position "5 pieces" and the position "6 pieces" are stored in the part list, the position "3 pieces" is also stored in the part list, as its condition is fulfilled if 5 pieces are to be produced and 6 pieces are to be produced. The conditional positions are stored with a sign that indicates whether the condition is fulfilled or not: an "!" for true and "?" for false. The position "5 pieces" is thus stored as "5 pieces!". If the storage of a position as a conditional position is not desired, the position can be marked as an "unconditional" position. This is the case, for example, if a "1 piece" position is added to the end of a "5 pieces" list. The "1 piece" position is then at the end of the list, but is no longer a position that has to be fulfilled. It is now an "unconditional" position, which is marked with a "?". The system now knows that the "1 piece" position is to be produced if the "5 pieces" position is to be produced, but that is the only connection. A conditional position is only evaluated (the corresponding calculation is carried out) when the position is inserted into a new part list. Evaluation of a conditional position does not depend on whether the position is inserted at the beginning or end of the list. An unconditional position is always only in the list one time. A conditional position can appear several times in the list, but only with a unique, calculated value for each occurrence. The system guarantees the correct evaluation of a conditional position by testing whether all arithmetic operations are possible. If this is not the case, the system warns you.</t>
         </is>
       </c>
       <c r="C35" s="9" t="inlineStr">
         <is>
-          <t>Bedingte Stücklistenpositions are conditional positions of a parts list. This type is used particularly often in project networks. It can be used to link individual parts list entries in such a way that logically related parts list entries are linked to each other. This is particularly useful in projects with sub-suppliers, as final parts lists can then be created by the operational staff without specialist knowledge.</t>
+          <t>The conditional positions in a bill of material are the following: If the requirement of a conditional sub-item is covered by a higher-level item of the same conditional group, then this higher-level item is entered directly in the production record. If the requirement of a conditional sub-item is covered by a lower-level item of the same conditional group, then this lower-level item is entered in the production record. If the conditional position is a variant item, then the unique variant position must be entered in the production record.</t>
         </is>
       </c>
       <c r="D35" s="9" t="inlineStr">
         <is>
+          <t>Conditional item position means that the staging of the part is dependent on the staging of another part. In ClassiX®, conditional item positions are implemented using the object CX_CONDITIONED_ITEM. This object is used to determine the staging of an item that is conditional on the staging of another item. For example, a part may be production-conditional on another part. The former may not be produced without the latter. This is referred to as a dependant item. Another example is when a part is to be ordered conditional on the availability of another part. In this case, the part is said to be order-conditional. There are two types of dependence: Direct dependence Indirect dependence Direct dependence If a part is to be ordered directly from a conditional item, the conditional item is specified in the order. Indirect dependence If a part is to be ordered from a conditional item that in turn is conditional on another part, the conditional item is not specified in the order. The order is then resolved via the chain of conditional items. Examples of conditional items can be found in the modules of the production planning and control system.</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="inlineStr">
+        <is>
+          <t>Bedingte Stücklistenpositionen sind Stücklistenpositionen, die unter bestimmten Bedingungen angezeigt werden.</t>
+        </is>
+      </c>
+      <c r="F35" s="9" t="inlineStr">
+        <is>
+          <t>Bedingte Stücklistenpositionen sind Positionen in einer Stücklistenspezifikation, die bedingt sind, d.h. ihre Dauer oder ihre Anforderungen hängen von anderen Faktoren ab. Diese bedingten Positionen können sich beispielsweise aus den folgenden Quellen ergeben: * Indikatoren in der Stücklistenspezifikation * Bedingungen in den Anforderungen * Sonderanforderungen mit Bedingungen.</t>
+        </is>
+      </c>
+      <c r="G35" s="9" t="inlineStr">
+        <is>
           <t>Bedingte Stücklistenpositionen sind Stücklistenpositionen, die nur dann ins Teil oder in die Stückliste aufgenommen werden, wenn die erforderlichen Bedingungen vorliegen.</t>
         </is>
       </c>
-      <c r="E35" s="9" t="inlineStr">
-        <is>
-          <t>Conditional item position means that the staging of the part is dependent on the staging of another part. In ClassiX®, conditional item positions are implemented using the object CX_CONDITIONED_ITEM. This object is used to determine the staging of an item that is conditional on the staging of another item. For example, a part may be production-conditional on another part. The former may not be produced without the latter. This is referred to as a dependant item. Another example is when a part is to be ordered conditional on the availability of another part. In this case, the part is said to be order-conditional. There are two types of dependence: Direct dependence Indirect dependence Direct dependence If a part is to be ordered directly from a conditional item, the conditional item is specified in the order. Indirect dependence If a part is to be ordered from a conditional item that in turn is conditional on another part, the conditional item is not specified in the order. The order is then resolved via the chain of conditional items. Examples of conditional items can be found in the modules of the production planning and control system.</t>
-        </is>
-      </c>
-      <c r="F35" s="9" t="inlineStr">
-        <is>
-          <t>A conditional position is a position that depends on the value of another position. For example, if the position "5 pieces" and the position "6 pieces" are stored in the part list, the position "3 pieces" is also stored in the part list, as its condition is fulfilled if 5 pieces are to be produced and 6 pieces are to be produced. The conditional positions are stored with a sign that indicates whether the condition is fulfilled or not: an "!" for true and "?" for false. The position "5 pieces" is thus stored as "5 pieces!". If the storage of a position as a conditional position is not desired, the position can be marked as an "unconditional" position. This is the case, for example, if a "1 piece" position is added to the end of a "5 pieces" list. The "1 piece" position is then at the end of the list, but is no longer a position that has to be fulfilled. It is now an "unconditional" position, which is marked with a "?". The system now knows that the "1 piece" position is to be produced if the "5 pieces" position is to be produced, but that is the only connection. A conditional position is only evaluated (the corresponding calculation is carried out) when the position is inserted into a new part list. Evaluation of a conditional position does not depend on whether the position is inserted at the beginning or end of the list. An unconditional position is always only in the list one time. A conditional position can appear several times in the list, but only with a unique, calculated value for each occurrence. The system guarantees the correct evaluation of a conditional position by testing whether all arithmetic operations are possible. If this is not the case, the system warns you.</t>
-        </is>
-      </c>
-      <c r="G35" s="9" t="inlineStr">
+      <c r="H35" s="9" t="inlineStr">
         <is>
           <t>Dieses Modul dient der Pflege von bedingten Stücklistenpositionen. Eine bedingte Stücklistenposition besteht aus einer Stücklistenposition und einem Bedingungskriterium. Das Bedingungskriterium bestimmt für welches Sachgebiet (Teile, Arbeitsplätze, Maschinen, Sonstige Kostenstellen) die Stücklistenposition angezeigt wird und für das eine Entnahme erfolgen kann. Wird keine Entnahme erlaubt, kann die Stücklistenposition auch aus dem Bearbeitungsfenster heraus entfernt werden.</t>
         </is>
       </c>
-      <c r="H35" s="9" t="inlineStr">
+      <c r="I35" s="9" t="inlineStr">
         <is>
           <t>Bedingte Stücklistenpositionen sind Stücklistenpositionen, die durch eine andere Stücklistenposition bedingt werden.
 ### Instruction:
@@ -2642,21 +2334,6 @@
 Unbewegte Stücklistenstellen sind Stücklistenstellen, an denen ein Stück in der Lagerhierarchie nicht</t>
         </is>
       </c>
-      <c r="I35" s="9" t="inlineStr">
-        <is>
-          <t>The conditional positions in a bill of material are the following: If the requirement of a conditional sub-item is covered by a higher-level item of the same conditional group, then this higher-level item is entered directly in the production record. If the requirement of a conditional sub-item is covered by a lower-level item of the same conditional group, then this lower-level item is entered in the production record. If the conditional position is a variant item, then the unique variant position must be entered in the production record.</t>
-        </is>
-      </c>
-      <c r="J35" s="9" t="inlineStr">
-        <is>
-          <t>Bedingte Stücklistenpositionen sind Positionen in einer Stücklistenspezifikation, die bedingt sind, d.h. ihre Dauer oder ihre Anforderungen hängen von anderen Faktoren ab. Diese bedingten Positionen können sich beispielsweise aus den folgenden Quellen ergeben: * Indikatoren in der Stücklistenspezifikation * Bedingungen in den Anforderungen * Sonderanforderungen mit Bedingungen.</t>
-        </is>
-      </c>
-      <c r="K35" s="9" t="inlineStr">
-        <is>
-          <t>Bedingte Stücklistenpositionen sind Stücklistenpositionen, die unter bestimmten Bedingungen angezeigt werden.</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="9" t="inlineStr">
@@ -2666,35 +2343,40 @@
       </c>
       <c r="B36" s="9" t="inlineStr">
         <is>
-          <t>Fehlzeiten sind Zeiträume, in denen eine Person (Arbeiter) nicht anwesend ist, was manche Arbeitgeber für die "unproduktive" Zeit eines Arbeitnehmers ablehnen. Fehlzeiten können aber auch sein, wenn eine Person (Arbeiter) vor dem Beginn seiner Arbeitzeit noch vor dem Start des Arbeitsprozesses, also beispielsweise noch vor dem Eintreffen auf dem Produktionssite, bereits zu arbeiten beginnt, was manche Arbeitgeber als "vorproduktive" Zeit bezeichnen.</t>
+          <t>A time delay is a date or timespan in the past or future. The time delay has the status of the corresponding date or period, i.e. if a time delay is compared to a person this is considered to be alive the time delay is considered to be alive. On the other hand, if a time delay is compared to a person who is dead the time delay is considered to be dead. This also applies to periods (e.g. an employment period of a person is considered to be dead if the person is). The comparison with a person is made by means of the compares_person method of the ClassiX® date or period objects. Since these methods do not find any information in the database to make the comparison, they automatically issue a query to the database. In this way, the classes being compared are also queried. Only the data currently in the database at the time of the comparison is taken into account in the comparison (snapshot). Therefore, it is also possible for a date or period to be considered alive or dead (respectively) for one project and dead for the next. The comparison with a project is made by means of the compares_project method of the ClassiX® date or period objects. The result of a comparison can be the following values: -1 The time delay is considered to be older or bigger than the project. This is the case, for example, for all people who are older or died before the beginning of the project. -1 The time delay is considered to be younger or smaller than the project. This is the case, for example, for all people who are younger or died after the end of the project. 0 The time delay is the same or there are no data.</t>
         </is>
       </c>
       <c r="C36" s="9" t="inlineStr">
         <is>
-          <t>A Fehlzeit is when a task is not carried out within the specified time. The duration of the feedtime of a task is specified when the task is created. If the actual end time of the task is smaller than the feedtime, the task has a feederror and is therefore redlined.</t>
+          <t>A fault code is a code that describes a fault. It is used to provide information about the cause of a fault and suggests a possible solution.</t>
         </is>
       </c>
       <c r="D36" s="9" t="inlineStr">
         <is>
+          <t>Eine Fehlzeit ist ein Phänomen, das auftritt, wenn die Dauer zwischen two consecutive events is longer than the sum of these durations. In the example above, the duration of the second event (red colour) is longer than the sum of the durations of the two events (green colour)</t>
+        </is>
+      </c>
+      <c r="E36" s="9" t="inlineStr">
+        <is>
+          <t>Eine Fehlzeit ist eine Zeitzeitierung, wenn der angegebene Zeitraum nicht der tatsächliche Zeitraum war. Im System werden Fehlzeiten als positiv oder negativ unterschieden, was die Auswirkungen auf die Zeitplanung hat. Positive Fehlzeiten treten meistens dann auf, wenn eine Arbeit schneller erledigt wurde als geplant, negative Fehlzeiten dann, wenn eine Arbeit länger in Anspruch genommen hat als geplant.</t>
+        </is>
+      </c>
+      <c r="F36" s="9" t="inlineStr">
+        <is>
+          <t>A time record with the status "time off" is called a time off record. This can be a flexible working time day, a public holiday or a special day.</t>
+        </is>
+      </c>
+      <c r="G36" s="9" t="inlineStr">
+        <is>
           <t>Eine Fehlzeit ist definiert als: Zeit, in der ein Mitarbeiter nicht zur Verfügung steht, obwohl er anwesend ist.</t>
         </is>
       </c>
-      <c r="E36" s="9" t="inlineStr">
-        <is>
-          <t>Eine Fehlzeit ist ein Phänomen, das auftritt, wenn die Dauer zwischen two consecutive events is longer than the sum of these durations. In the example above, the duration of the second event (red colour) is longer than the sum of the durations of the two events (green colour)</t>
-        </is>
-      </c>
-      <c r="F36" s="9" t="inlineStr">
-        <is>
-          <t>A time delay is a date or timespan in the past or future. The time delay has the status of the corresponding date or period, i.e. if a time delay is compared to a person this is considered to be alive the time delay is considered to be alive. On the other hand, if a time delay is compared to a person who is dead the time delay is considered to be dead. This also applies to periods (e.g. an employment period of a person is considered to be dead if the person is). The comparison with a person is made by means of the compares_person method of the ClassiX® date or period objects. Since these methods do not find any information in the database to make the comparison, they automatically issue a query to the database. In this way, the classes being compared are also queried. Only the data currently in the database at the time of the comparison is taken into account in the comparison (snapshot). Therefore, it is also possible for a date or period to be considered alive or dead (respectively) for one project and dead for the next. The comparison with a project is made by means of the compares_project method of the ClassiX® date or period objects. The result of a comparison can be the following values: -1 The time delay is considered to be older or bigger than the project. This is the case, for example, for all people who are older or died before the beginning of the project. -1 The time delay is considered to be younger or smaller than the project. This is the case, for example, for all people who are younger or died after the end of the project. 0 The time delay is the same or there are no data.</t>
-        </is>
-      </c>
-      <c r="G36" s="9" t="inlineStr">
+      <c r="H36" s="9" t="inlineStr">
         <is>
           <t>Die Zeit, die ein Arbeitsgang benötigt, um vollständig und korrekt ausgeführt zu werden, ist die Fehlzeit eines Arbeitsgangs.</t>
         </is>
       </c>
-      <c r="H36" s="9" t="inlineStr">
+      <c r="I36" s="9" t="inlineStr">
         <is>
           <t>Eine Fehlzeit ist eine Zeit, die falsch angegeben wurde. Dies kann beispielsweise der Fall sein, wenn die Uhrzeit falsch eingegeben wurde.
 ### Instruction:
@@ -2727,21 +2409,6 @@
 Eine korrigible Zeitspanne ist eine Zeitspanne, in der eine Aktivität zu verzeichnen ist, die aber noch nicht eindeutig zuzuordnen ist. Dies kann be</t>
         </is>
       </c>
-      <c r="I36" s="9" t="inlineStr">
-        <is>
-          <t>A fault code is a code that describes a fault. It is used to provide information about the cause of a fault and suggests a possible solution.</t>
-        </is>
-      </c>
-      <c r="J36" s="9" t="inlineStr">
-        <is>
-          <t>A time record with the status "time off" is called a time off record. This can be a flexible working time day, a public holiday or a special day.</t>
-        </is>
-      </c>
-      <c r="K36" s="9" t="inlineStr">
-        <is>
-          <t>Eine Fehlzeit ist eine Zeitzeitierung, wenn der angegebene Zeitraum nicht der tatsächliche Zeitraum war. Im System werden Fehlzeiten als positiv oder negativ unterschieden, was die Auswirkungen auf die Zeitplanung hat. Positive Fehlzeiten treten meistens dann auf, wenn eine Arbeit schneller erledigt wurde als geplant, negative Fehlzeiten dann, wenn eine Arbeit länger in Anspruch genommen hat als geplant.</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="9" t="inlineStr">
@@ -2751,35 +2418,40 @@
       </c>
       <c r="B37" s="9" t="inlineStr">
         <is>
-          <t>Mit der Importfunktion in GESTIN können die Daten aus Excel importiert werden. Es existieren zwei Möglichkeiten, die Daten einzusparen: als XML-File oder direkt als Excel-Tabellenwerk. Die Dateien für die einzusparenden Daten werden in den Prozessoryberaden prägeneriert. Die folgenden Angaben gelten für die Einbindung von Excel-Tabellenwerken:  SourceFile must be created in the process area of interest.   The column headings of the Excel table must be exactly the same as in the system.   The column headings must be wrapped with double quotes.   The column types (specify the number of decimal places)   The column values (please ensure that the column values are not too short or too long. To ensure that the column values are always 20 characters long, a leading zero should be added to the column values, e.g. if the original value is 9.99999999 (6 digits) the import value should be 099999990 (with leading zeroes).   The following example shows an Excel table that could have been exported from a previous system as inventory data and then imported into GESTIN:  Name  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 Value  			 Unit  			 4  			 525.00  			 			 52.50  			 6  			 12.50  			 100.00  			 7  			 25.00  			 200.00  			 8  			 6.25  			 250.00  			 9  			 15.00  			 375.00  			 10  			 37.5</t>
+          <t>The following is a description of the inventory import process.</t>
         </is>
       </c>
       <c r="C37" s="9" t="inlineStr">
         <is>
-          <t>To import inventory data from STADTAUFL into GESTIN, follow these instructions: After starting up GESTIN, open the window for importing data from STADTAUFL (via File -&gt; Import). In the first tab of the window, which appears after opening, the type of inventory is selected (choice between warehouse, storage or removable inventory). In the next tab, the system identifies the storage locations by means of the selection of the warehouse/storage locations. The information is taken from the data exported from STADTAUFL. Usually this is the export data of the client's own warehouse or the warehouses of the contract storage partners. Usually this is the export data of the client's own warehouse or the warehouses of the contract storage partners. If the warehouses/storage locations have not been identified in the system, it is possible to enter their data manually in the list. In the third tab, the inventory items are entered. If the inventory items have already been identified in the client's own system as sales rolls or parts rolls, it is possible to use them for the inventory. Otherwise, the inventory items must be entered manually. It is recommended to use the menu item "Search Google" to research missing inventory items. A separate identification of sales rolls and parts rolls is possible, since not all rolls are inventory rolls. Once all the data has been entered, click on the button "Import". A message appears stating that the import could not be carried out. There are then various possible reasons for this. The system searches for a file named STADTAUFL*.LOG, which must exist in the current directory. If this file is not found, the import is aborted. If the file is found, but the error message appears, the system has not read all data correctly. In this case, the file can be checked with a text editor. Note: It is recommended to create the file STADTAUFL*.LOG manually before importing, as this way the required file is always created. If the import was successful, a message appears stating that the data could be imported.</t>
+          <t>The process of importing inventory data in GESTIN is as follows: The inventory data is first imported in the background with the button "Import inventory data". After carrying out this import, the mask is displayed in which you can now enter the inventory data for the selected warehouse. The warehouse must be created in GESTIN beforehand and be assigned to the company for which the inventory is carried out. If you want to assign the warehouse to different company, you can create a warehouse in GESTIN and assign it to the company. Important: When importing, it is important to enter the warehouse type (railway car, container, etc.) and any special characteristics of this warehouse type (e.g. own planning unit) If these data are not entered correctly, they cannot be assigned to a warehouse in GESTIN. These must be created again with the corresponding type. Once the warehouse is created and the data has been entered, the inventory data can be entered. When entering the inventory data, it is important to enter the warehouse and the storage bin (with the possible sub-sub-sub... levels) and not to skip any entries. If you have entered all the inventory data for a warehouse, you can now open the inventory mask for this warehouse. The warehouse-specific data entered in GESTIN (e.g. planning unit, container type, etc.) are taken into account here.</t>
         </is>
       </c>
       <c r="D37" s="9" t="inlineStr">
         <is>
+          <t>To import inventory data into GESTIN, you can follow these steps: 1. Connect to the server where the inventory data is stored (e.g. another PC) 2. Open the "File" menu in GESTIN and select "Import" 3. Select "Inventory" as the data source and "InteractiveGuidedTour" as the classification term 4. Under "File Import", select "Inventory" and set the appropriate values for the fields "Company", "Year" and "Period". You can also leave these fields empty and allow GESTIN to determine them from the file you are importing later. 5. Under "Account", select the account for which you want to import inventory data and set the appropriate value in the "Number" field. You can also leave this field empty and allow GESTIN to determine it from the file you are importing later. 6. Now browse the inventory data from the other PC to the computer on which GESTIN is installed via the "File Import" menu. The data should now be available in GESTIN. 7. To make the inventory data available in the mobile application as well, the inventory data in the file should be divided into individual items. Since an individual item is always assigned to a particular part, the part should be assigned to each individual item. This is the only condition that must be met in order for the inventory data to be imported into the mobile application as well. As soon as the conditions are met, the inventory data is also imported into the mobile application.</t>
+        </is>
+      </c>
+      <c r="E37" s="9" t="inlineStr">
+        <is>
+          <t>Um meine Inventurdaten in GESTIN zu importieren, benutze ich das Importtool.</t>
+        </is>
+      </c>
+      <c r="F37" s="9" t="inlineStr">
+        <is>
+          <t>The inventory data from the warehouse can be imported into GESTIN using the import interface. Here are the steps to follow: 1. Open the import interface by clicking on the "Import" button on the start page. 2. Select "Inventory" as the type of data to be imported. 3. Select the file to be imported, which should be in CSV format. The columns of the file should be in the following order: warehouse, storage bin, article, quantity. The article can be specified using the article number or the name. If the article number is entered first, the system will look for a entry with this number in the article master and use it for the import. If the name is entered first, the system will look for a entry with this name in the article master and use it for the import. If no entry is found in the article master, the article is considered to be a new entry and is therefore created in the article master during the import process. The quantity can be entered with or without a decimal point. In the following steps, the data is checked and, if necessary, completed so that it can be read in correctly. After the data has been read in, it is checked again and the warehouse and storage bin are checked to see if they exist in the system. If they do not exist, they are created during the import process. Now the data is imported and can be checked again for possible errors.</t>
+        </is>
+      </c>
+      <c r="G37" s="9" t="inlineStr">
+        <is>
           <t>Die Inventurdaten können in GESTIN importiert werden, indem die Datei der Zählung in das Programm gedragen und die darin enthaltenen Informationen übernommen werden.</t>
         </is>
       </c>
-      <c r="E37" s="9" t="inlineStr">
-        <is>
-          <t>To import inventory data into GESTIN, you can follow these steps: 1. Connect to the server where the inventory data is stored (e.g. another PC) 2. Open the "File" menu in GESTIN and select "Import" 3. Select "Inventory" as the data source and "InteractiveGuidedTour" as the classification term 4. Under "File Import", select "Inventory" and set the appropriate values for the fields "Company", "Year" and "Period". You can also leave these fields empty and allow GESTIN to determine them from the file you are importing later. 5. Under "Account", select the account for which you want to import inventory data and set the appropriate value in the "Number" field. You can also leave this field empty and allow GESTIN to determine it from the file you are importing later. 6. Now browse the inventory data from the other PC to the computer on which GESTIN is installed via the "File Import" menu. The data should now be available in GESTIN. 7. To make the inventory data available in the mobile application as well, the inventory data in the file should be divided into individual items. Since an individual item is always assigned to a particular part, the part should be assigned to each individual item. This is the only condition that must be met in order for the inventory data to be imported into the mobile application as well. As soon as the conditions are met, the inventory data is also imported into the mobile application.</t>
-        </is>
-      </c>
-      <c r="F37" s="9" t="inlineStr">
-        <is>
-          <t>The following is a description of the inventory import process.</t>
-        </is>
-      </c>
-      <c r="G37" s="9" t="inlineStr">
+      <c r="H37" s="9" t="inlineStr">
         <is>
           <t>Der Import der Inventurdaten in GESTIN kann durch einen Export aus einem Materialwirtschaftssystem oder direkt aus Excel erfolgen.Wird ein Export aus einem Materialwirtschaftssystem durchgeführt, werden die Daten auf Grundlage des Exchange Protokolls über eine Zuordnung zu den Teilen unterstützt. In diesem Fall ist ein Vorab Import der Teile in GESTIN nicht notwendig.Wird kein Export aus einem Materialwirtschaftssystem durchgeführt, kann man den Import mit einem Vorab Import der Teile in GESTIN verzweigen.</t>
         </is>
       </c>
-      <c r="H37" s="9" t="inlineStr">
+      <c r="I37" s="9" t="inlineStr">
         <is>
           <t>GESTIN kann Inventurdaten aus dem CSV-Format importieren. Die Inventurdaten müssen in der ersten Zeile des CSV-Files sein und die Spalten darüber entfallen.
 ### Beispiel:
@@ -2794,21 +2466,6 @@
 1.  Gestin: Importdatensätze. Abgerufen am 20. Juni 2019.</t>
         </is>
       </c>
-      <c r="I37" s="9" t="inlineStr">
-        <is>
-          <t>The process of importing inventory data in GESTIN is as follows: The inventory data is first imported in the background with the button "Import inventory data". After carrying out this import, the mask is displayed in which you can now enter the inventory data for the selected warehouse. The warehouse must be created in GESTIN beforehand and be assigned to the company for which the inventory is carried out. If you want to assign the warehouse to different company, you can create a warehouse in GESTIN and assign it to the company. Important: When importing, it is important to enter the warehouse type (railway car, container, etc.) and any special characteristics of this warehouse type (e.g. own planning unit) If these data are not entered correctly, they cannot be assigned to a warehouse in GESTIN. These must be created again with the corresponding type. Once the warehouse is created and the data has been entered, the inventory data can be entered. When entering the inventory data, it is important to enter the warehouse and the storage bin (with the possible sub-sub-sub... levels) and not to skip any entries. If you have entered all the inventory data for a warehouse, you can now open the inventory mask for this warehouse. The warehouse-specific data entered in GESTIN (e.g. planning unit, container type, etc.) are taken into account here.</t>
-        </is>
-      </c>
-      <c r="J37" s="9" t="inlineStr">
-        <is>
-          <t>The inventory data from the warehouse can be imported into GESTIN using the import interface. Here are the steps to follow: 1. Open the import interface by clicking on the "Import" button on the start page. 2. Select "Inventory" as the type of data to be imported. 3. Select the file to be imported, which should be in CSV format. The columns of the file should be in the following order: warehouse, storage bin, article, quantity. The article can be specified using the article number or the name. If the article number is entered first, the system will look for a entry with this number in the article master and use it for the import. If the name is entered first, the system will look for a entry with this name in the article master and use it for the import. If no entry is found in the article master, the article is considered to be a new entry and is therefore created in the article master during the import process. The quantity can be entered with or without a decimal point. In the following steps, the data is checked and, if necessary, completed so that it can be read in correctly. After the data has been read in, it is checked again and the warehouse and storage bin are checked to see if they exist in the system. If they do not exist, they are created during the import process. Now the data is imported and can be checked again for possible errors.</t>
-        </is>
-      </c>
-      <c r="K37" s="9" t="inlineStr">
-        <is>
-          <t>Um meine Inventurdaten in GESTIN zu importieren, benutze ich das Importtool.</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="9" t="inlineStr">
@@ -2818,35 +2475,40 @@
       </c>
       <c r="B38" s="9" t="inlineStr">
         <is>
-          <t>Stichprobeninventur bedeutet in diesem Fall, dass PYTHIA eine Fülle von Messungen durchführt, um die Gesundheit eines Computers zu ermitteln. Hierbei wird u. a. die Verkleinerung der Bits auf die Anzahl der Bitstellen geprüft, die mit 0 verknüpft sind, die Anzahl der Wach/Schlaf-Zyklen und die Anzahl der Branchings per Sekunde geprüft. Bei kritischen Inhalten, also Inhalten, die mit 0 verknüpft sind, wird eine Fehlfunktion erkannt, bei Todeszeichen im Code oder zu häufigen Branchings (Stackoverflow) wird eine Fehldirektion erkannt. Bei allen anderen Messungen werden die Ergebnisse in Relation zu den Größen des Arbeitsspecs gesetzt. Die Ergebnisse aus der Inventur werden in einer separaten Tabelle abgelegt, die es PYTHIA erlaubt, nachträglich die Messungen zu verifizieren und anzugeben, wodurch eine Fehlalarm-Loggierechnung möglich wird.PYTHIA selbst tut folgendes:Was ist eine Stichprobeninventur?Eine Stichprobeninventur ist die Anforderung, bei der man die Gesundheit eines Objektes, z.B. eines Computers, unabhängig von allen Ereignissen, Messungen und Operationen, über eine Stichprobe von Messungen ableiten lässt. Manche Messungen werden also nur bei der Stichprobeninventur durchgeführt, nicht aber bei jedem Start des Objektes.Was ist mit PYTHIA?PYTHIA macht folgende Messungen:Was ist mit PYTHIA?</t>
+          <t>A census or inventory of a sample of objects is called a stichprobe inventory. The Pythia instrument performs the following functions:The inventory of the objects is carried out by selecting individual objects in the database and counting their properties (characteristics). Since a property can be assigned to different objects, this counting is carried out in a phase in which only objects with a certain property are selected. The number of objects with this property is then determined and output. A second counting is then performed on the selected objects, but now the property is not searched for, but its value is determined. This way, one can check whether an object with a certain property actually has this property, e.g. if all objects are cars, one can check whether one of them is red.The instruments CENSUS and INVENTORY are specialised on inventories of objects in the database.</t>
         </is>
       </c>
       <c r="C38" s="9" t="inlineStr">
         <is>
-          <t>The purpose of a stichprobe inventory is as follows: This app is used to record stock levels of individual parts in a warehouse. During the inventory, the stock levels of the individual parts are recorded at specific storage locations. This app is intended for use in the course of a physical inventory. The app is designed in such a way that it can also be operated on a tablet PC or a smart phone.</t>
+          <t>A stochastic inventory model is a specialisation of the PYTHIA® stochastic model. In a stochastic inventory model, the inventory is divided into individual inventory items. These individual inventory items can represent different parts in a warehouse. The demand for individual inventory items is described by means of an inventory history. This provides the information on which inventory items have been delivered to the warehouse in the past and which have left the warehouse again. On the basis of this history, a requirement or need of the warehouse can be determined for each inventory item at any given time. This evaluation is carried out using a requirement or need evaluation. The stochastic inventory model uses this evaluation to determine whether there are surpluses or shortages at all for the individual inventory items at a certain time. If so, how large the surplus or shortage is - this is determined by means of a balance equation. The articles of the warehouse are kept in bins. Each bin has its own balance equation. The stochastic inventory model is described in more detail in the online documentation of PYTHIA® under Stochastic Inventory Model.</t>
         </is>
       </c>
       <c r="D38" s="9" t="inlineStr">
         <is>
+          <t>A stochastic inventory sampling procedure is a method of selecting a sample from a set of items in such a way that the sample is drawn from the probability distribution of the items. In contrast to a deterministic inventory sampling procedure, such as a simple random sample, the sample obtained using a stochastic inventory sampling procedure has the same probability of being drawn from any of the items in the set. This means that, for example, it is possible that two or more items are included in the sample. The degree to which this happens, i.e. the probability that two or more items are included in the sample, can be set via the parameter beta in the input window. beta equals 0 corresponds to the situation where only one item is included in the sample. beta equals 1 corresponds to the situation where all items are included in the sample. PYTHIA is a tool for carrying out stochastic inventory sampling. It can be used to perform this type of inventory sampling on the one hand and deterministic inventory sampling on the other. The input windows for these two types of inventory sampling are slightly different.</t>
+        </is>
+      </c>
+      <c r="E38" s="9" t="inlineStr">
+        <is>
+          <t>A random inventory is an inventory in which a random sample of items is examined and an estimate is made of the value of the entire inventory. This can be done, for example, when goods are taken from a warehouse to a storage bin in the presence of an inventory clerk. Since it is not possible to count every individual part, a random sample must be taken. The PYTHIA software supports the counting of inventories by randomly selecting storage bins and/or individual parts and displaying them on a digital image. The inventory clerk can now count the contents of the storage bin and/or the individual parts and record the finding in the system. In this way, an inventory can be taken of a storage bin, a picking zone or an entire warehouse.</t>
+        </is>
+      </c>
+      <c r="F38" s="9" t="inlineStr">
+        <is>
+          <t>A stochastic inventory is a special form of an inventory that is used to determine the on-hand warehouse stock of a company. This is done by randomly selecting storage bins and counting the stock in these bins. This random sampling is designed to reduce the complexity and time required for an inventory count, as it is not necessary to count all storage bins. The Pythia application is used to carry out such stochastic inventories.</t>
+        </is>
+      </c>
+      <c r="G38" s="9" t="inlineStr">
+        <is>
           <t>Eine Stichprobeninventur ist folgende Inventurart: Bei einer Stichprobeninventur werden nur einzelne Positionen ausgewählt und gezählt. Die übrigen Positionen werden geschätzt. Dadurch ist eine Stichprobeninventur schneller als eine Vollinventur, dafür ist sie aber auch genauer.</t>
         </is>
       </c>
-      <c r="E38" s="9" t="inlineStr">
-        <is>
-          <t>A stochastic inventory sampling procedure is a method of selecting a sample from a set of items in such a way that the sample is drawn from the probability distribution of the items. In contrast to a deterministic inventory sampling procedure, such as a simple random sample, the sample obtained using a stochastic inventory sampling procedure has the same probability of being drawn from any of the items in the set. This means that, for example, it is possible that two or more items are included in the sample. The degree to which this happens, i.e. the probability that two or more items are included in the sample, can be set via the parameter beta in the input window. beta equals 0 corresponds to the situation where only one item is included in the sample. beta equals 1 corresponds to the situation where all items are included in the sample. PYTHIA is a tool for carrying out stochastic inventory sampling. It can be used to perform this type of inventory sampling on the one hand and deterministic inventory sampling on the other. The input windows for these two types of inventory sampling are slightly different.</t>
-        </is>
-      </c>
-      <c r="F38" s="9" t="inlineStr">
-        <is>
-          <t>A census or inventory of a sample of objects is called a stichprobe inventory. The Pythia instrument performs the following functions:The inventory of the objects is carried out by selecting individual objects in the database and counting their properties (characteristics). Since a property can be assigned to different objects, this counting is carried out in a phase in which only objects with a certain property are selected. The number of objects with this property is then determined and output. A second counting is then performed on the selected objects, but now the property is not searched for, but its value is determined. This way, one can check whether an object with a certain property actually has this property, e.g. if all objects are cars, one can check whether one of them is red.The instruments CENSUS and INVENTORY are specialised on inventories of objects in the database.</t>
-        </is>
-      </c>
-      <c r="G38" s="9" t="inlineStr">
+      <c r="H38" s="9" t="inlineStr">
         <is>
           <t>Der Zweck einer Stichprobeninventur ist der Folgende: Keine klassische Inventur! Dieses Modul dient der Inventur von Verkaufs- und Lagerobjekten durch Auswahl einer Stichprobe aus allen Lagerplätzen und Bereichen des Verkaufs und Lagerbestands. Die Auswahl der Stichprobe kann nach Lagerplatz, Lagerbereich und/oder Auflistungsgruppe erfolgen. Für die Ermittlung der Stichprobe wird ein präzises Datum festgelegt (Einzel- oder Teilinventur) oder kann für zukünftige Bedarfe auch ein Zeitraum angegeben werden (Bedarfsinventur). Mit der Stichprobeninventur können ermittelt werden:Lagerbestand mit allen Objekten auf einem Lagerplatz oder in einem LagerbereichLagerbestand pro Lagerbereich für ein bestimmtes ObjektGründe einer Inventur: Inventuren können als Bedarfs- oder Lagerbuchhaltung erstellt werden. Als Bedarfs-Inventur wird eine Inventur bezeichnet, die dazu dient, die Dauerung der Verkaufs-/Lagerbereitstellungsmenge zu prüfen. Als Lagerbuchhaltung wird eine Inventur bezeichnet, die dazu dient, die Dauerung des Lagerbestands zu prüfen. Derartige Inventuren werden auch als Quarterly Inventories genannt, da sie nach Abschluss eines Geschäftsjahres als Jahresinventur gespeichert werden.</t>
         </is>
       </c>
-      <c r="H38" s="9" t="inlineStr">
+      <c r="I38" s="9" t="inlineStr">
         <is>
           <t>Stichprobeninventuren werden in der Regel durchgeführt, um die Verteilung der Werte in einer Population zu ermitteln. Dabei werden die Werte in der Population in Stichproben ausgewählt, die dann in der Regel mit Hilfe der Verteilung der Werte in der Population verglichen werden. Die Stichprobeninventur dient also der Verifikation der Annahmen einer Theorie oder einer Hypothese.
 PYTHIA ist eine Software, die es erlaubt, Stichprobeninventuren zu durchführen. Sie wurde von der Universität Cambridge entwickelt und ist kostenlos erhältlich.
@@ -2885,21 +2547,6 @@
 * Stichprobenverteilungsschle</t>
         </is>
       </c>
-      <c r="I38" s="9" t="inlineStr">
-        <is>
-          <t>A stochastic inventory model is a specialisation of the PYTHIA® stochastic model. In a stochastic inventory model, the inventory is divided into individual inventory items. These individual inventory items can represent different parts in a warehouse. The demand for individual inventory items is described by means of an inventory history. This provides the information on which inventory items have been delivered to the warehouse in the past and which have left the warehouse again. On the basis of this history, a requirement or need of the warehouse can be determined for each inventory item at any given time. This evaluation is carried out using a requirement or need evaluation. The stochastic inventory model uses this evaluation to determine whether there are surpluses or shortages at all for the individual inventory items at a certain time. If so, how large the surplus or shortage is - this is determined by means of a balance equation. The articles of the warehouse are kept in bins. Each bin has its own balance equation. The stochastic inventory model is described in more detail in the online documentation of PYTHIA® under Stochastic Inventory Model.</t>
-        </is>
-      </c>
-      <c r="J38" s="9" t="inlineStr">
-        <is>
-          <t>A stochastic inventory is a special form of an inventory that is used to determine the on-hand warehouse stock of a company. This is done by randomly selecting storage bins and counting the stock in these bins. This random sampling is designed to reduce the complexity and time required for an inventory count, as it is not necessary to count all storage bins. The Pythia application is used to carry out such stochastic inventories.</t>
-        </is>
-      </c>
-      <c r="K38" s="9" t="inlineStr">
-        <is>
-          <t>A random inventory is an inventory in which a random sample of items is examined and an estimate is made of the value of the entire inventory. This can be done, for example, when goods are taken from a warehouse to a storage bin in the presence of an inventory clerk. Since it is not possible to count every individual part, a random sample must be taken. The PYTHIA software supports the counting of inventories by randomly selecting storage bins and/or individual parts and displaying them on a digital image. The inventory clerk can now count the contents of the storage bin and/or the individual parts and record the finding in the system. In this way, an inventory can be taken of a storage bin, a picking zone or an entire warehouse.</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="9" t="inlineStr">
@@ -2909,37 +2556,42 @@
       </c>
       <c r="B39" s="9" t="inlineStr">
         <is>
-          <t>Belege löschen? Nein, solche Dokumente mit Belegen werden im BWA nicht mehr an die Endbenutzer versandt, sondern direkt in den Document Archive entsynchronised. Falls Sie die Belege vor dem Entsynchronisationen entfernen möchten, können Sie sie auch hier noch einmal abspeichern.</t>
+          <t>Belege löschen? Nein, es ist nicht möglich die Belege zu löschen.</t>
         </is>
       </c>
       <c r="C39" s="9" t="inlineStr">
         <is>
-          <t>Belege können gelöscht werden.</t>
+          <t>You can delete documents. There are, however, a number of documents - such as master data - which cannot be deleted. In addition, all documents are linked to each other and changes in one document can trigger events in other documents. These events can, in turn, trigger the creation of new documents. For this reason, most documents are only temporarily available and automatically deleted at some point in time. The actual time and document for deletion is stored in the system as the document's "deletion date and document". This way, you can always see when and by whom a document was deleted. The standard algorithm for permanently deleting documents is the following:First, the documents are sorted according to the "document history" (this is done at document creation and is also done each time a document is updated). So the documents are sorted according to the sequence in which they were created or last updated. Within this sequence, the documents are divided into two groups:The documents that are to be deleted first are stored in the first group.The documents that are to be deleted later are stored in the second group.At some point in the future, this second group of documents will be permanently deleted. The documents in the first group will remain visible for a while longer, but will also be permanently deleted at some point in the future.Exactly when a document from the first group will be permanently deleted cannot be specified. This depends on the size of the database and which transactions have been performed on the data. It also depends on the number of documents in the first group and when these documents were last changed or last accessed (by different users).All temporarily available documents are marked with the status "deletion postponed". This status can be changed to "deletion started" and afterwards to "deletion finished", as soon as the permanent deletion of a document has taken place. The status "deletion finished" indicates when and by whom a document was permanently deleted.</t>
         </is>
       </c>
       <c r="D39" s="9" t="inlineStr">
-        <is>
-          <t>Ja, Belege können gelöscht werden.</t>
-        </is>
-      </c>
-      <c r="E39" s="9" t="inlineStr">
         <is>
           <t>Yes, you can delete invoices. However, please note that this should be done with caution, as the deletion of an invoice is irreversible. Therefore, please make sure to first create a copy of the invoice in your "Archive" or "Status Monitor" before deleting it. This way, the invoice can be restored at any time in the future.
 Deleting an invoice that has not yet been posted is relatively simple. You can find the "Edit" button on the invoice (via the list view) or on the invoice itself (if it has already been entered in the post). Click on the "Edit" button and then select "Delete invoice" from the drop-down menu. Confirm with "OK".
 If the invoice has already been posted, a warning message will appear. The invoice cannot be deleted.</t>
         </is>
       </c>
+      <c r="E39" s="9" t="inlineStr">
+        <is>
+          <t>Yes, you can delete receipts. You can delete them in the list or the detail view. You can also delete a receipt that is attached to an order or an invoice.</t>
+        </is>
+      </c>
       <c r="F39" s="9" t="inlineStr">
         <is>
-          <t>Belege löschen? Nein, es ist nicht möglich die Belege zu löschen.</t>
+          <t>Yes, documents can be deleted. However, before doing so, you should consider whether the document in question is still needed or if it could be replaced by another document. In addition, you should consider the possible consequences of deleting a document. For example, if the document in question is a receipt or an order, the deletion of this document could lead to errors in the further processing of the document or even to data loss. Therefore, you should only delete documents that are definitely no longer needed or that cannot cause any problems when deleted.</t>
         </is>
       </c>
       <c r="G39" s="9" t="inlineStr">
         <is>
+          <t>Ja, Belege können gelöscht werden.</t>
+        </is>
+      </c>
+      <c r="H39" s="9" t="inlineStr">
+        <is>
           <t>Nein, das kann man nicht. Die Belege werden automatisch gelöscht, wenn man die Liste über die Entlastungsmaske aufruft oder sich aus dem Listenfenster abfragt.</t>
         </is>
       </c>
-      <c r="H39" s="9" t="inlineStr">
+      <c r="I39" s="9" t="inlineStr">
         <is>
           <t>Ja, man kann Belege löschen.
 ### Instruction:
@@ -2987,21 +2639,6 @@
 ##</t>
         </is>
       </c>
-      <c r="I39" s="9" t="inlineStr">
-        <is>
-          <t>You can delete documents. There are, however, a number of documents - such as master data - which cannot be deleted. In addition, all documents are linked to each other and changes in one document can trigger events in other documents. These events can, in turn, trigger the creation of new documents. For this reason, most documents are only temporarily available and automatically deleted at some point in time. The actual time and document for deletion is stored in the system as the document's "deletion date and document". This way, you can always see when and by whom a document was deleted. The standard algorithm for permanently deleting documents is the following:First, the documents are sorted according to the "document history" (this is done at document creation and is also done each time a document is updated). So the documents are sorted according to the sequence in which they were created or last updated. Within this sequence, the documents are divided into two groups:The documents that are to be deleted first are stored in the first group.The documents that are to be deleted later are stored in the second group.At some point in the future, this second group of documents will be permanently deleted. The documents in the first group will remain visible for a while longer, but will also be permanently deleted at some point in the future.Exactly when a document from the first group will be permanently deleted cannot be specified. This depends on the size of the database and which transactions have been performed on the data. It also depends on the number of documents in the first group and when these documents were last changed or last accessed (by different users).All temporarily available documents are marked with the status "deletion postponed". This status can be changed to "deletion started" and afterwards to "deletion finished", as soon as the permanent deletion of a document has taken place. The status "deletion finished" indicates when and by whom a document was permanently deleted.</t>
-        </is>
-      </c>
-      <c r="J39" s="9" t="inlineStr">
-        <is>
-          <t>Yes, documents can be deleted. However, before doing so, you should consider whether the document in question is still needed or if it could be replaced by another document. In addition, you should consider the possible consequences of deleting a document. For example, if the document in question is a receipt or an order, the deletion of this document could lead to errors in the further processing of the document or even to data loss. Therefore, you should only delete documents that are definitely no longer needed or that cannot cause any problems when deleted.</t>
-        </is>
-      </c>
-      <c r="K39" s="9" t="inlineStr">
-        <is>
-          <t>Yes, you can delete receipts. You can delete them in the list or the detail view. You can also delete a receipt that is attached to an order or an invoice.</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="inlineStr">
@@ -3011,56 +2648,46 @@
       </c>
       <c r="B40" s="9" t="inlineStr">
         <is>
-          <t>Die Beleggeschichte ist ein Eintrag zu Documents, der die Verbindungen zwischen Documents und Transaction Documents (outgoing invoice, incoming invoice, order, goods receipt, etc.) graphically illustrates.</t>
+          <t>The history of expenses is an app that displays the history of the expenses of a business. It can be called up either for individual or cumulative periods of time.</t>
         </is>
       </c>
       <c r="C40" s="9" t="inlineStr">
         <is>
-          <t>The BelegLog provides an overview of all transactions that have been booked in the current (fiscal) year. The call also allows you to switch to the previous or following year.</t>
+          <t>The beleghistorie is a list of all documents that reference a single document or a group of documents. This reference can be direct (by means of a transaction) or indirect (via a transaction that refers to the transaction being researched). The beleghistorie is used for electronic document management and provides an overview of the context of a document.</t>
         </is>
       </c>
       <c r="D40" s="9" t="inlineStr">
         <is>
+          <t>The beleghistorie is the history of all documents that have been attached to a business object. This includes all transaction documents (invoices, orders, etc.) as well as master data (company information, employee master data, etc.) and other documents. The beleghistorie thus contains the entire history of a business object.</t>
+        </is>
+      </c>
+      <c r="E40" s="9" t="inlineStr">
+        <is>
+          <t>Die Beleghistorie ist eine Liste mit den letzten einige Transactions, die im Zusammenhang mit einem Geschäftskonto stehen. Die Transactions werden dabei nicht nur aus dem eigenen Haushaltsbuchungssoftware abgefragt, sondern auch aus den externen Systems, die ihre Transactions über die Interface von FinancialForce hinzugefügt haben. Die Transactions werden daher auch externen Systems zugeordnet.</t>
+        </is>
+      </c>
+      <c r="F40" s="9" t="inlineStr">
+        <is>
+          <t>Die Beleghistorie ist ein Datensatz, der in der Appelion-DMS verwendet wird, um den Documents oder E-Mails an einen Customer oder a User to associate these documents with a customer or user. This association allows you to maintain a list of documents or emails for a specific customer or user. The Beleghistorie datensatz is used to keep a record of all documents and emails that have been received or sent for a specific customer or user. This record allows you to see when and how many documents or emails have been sent or received for a specific customer or user. The Beleghistorie datensatz is used in the Appelion DMS to associate documents or emails with a customer or user. This association is done by creating a Beleghistorie entry with the document or email and the customer or user. Once an entry has been created, the document or email is associated with the customer or user. The Beleghistorie entry can then be found in the document or email history of the customer or user. The Beleghistorie datensatz is used in the Appelion DMS to associate documents or emails with a customer or user. This association is done by creating a Beleghistorie entry with the document or email and the customer or user. Once an entry has been created, the document or email is associated with the customer or user. The Beleghistorie entry can then be found in the document or email history of the customer or user.</t>
+        </is>
+      </c>
+      <c r="G40" s="9" t="inlineStr">
+        <is>
           <t>Die Beleghistorie verfolgt alle Vorgänge, die in der Buchhaltung oder mit Buchungsbelegen durchgeführt werden.</t>
         </is>
       </c>
-      <c r="E40" s="9" t="inlineStr">
-        <is>
-          <t>The beleghistorie is the history of all documents that have been attached to a business object. This includes all transaction documents (invoices, orders, etc.) as well as master data (company information, employee master data, etc.) and other documents. The beleghistorie thus contains the entire history of a business object.</t>
-        </is>
-      </c>
-      <c r="F40" s="9" t="inlineStr">
-        <is>
-          <t>The history of expenses is an app that displays the history of the expenses of a business. It can be called up either for individual or cumulative periods of time.</t>
-        </is>
-      </c>
-      <c r="G40" s="9" t="inlineStr">
+      <c r="H40" s="9" t="inlineStr">
         <is>
           <t>Das Modul Beleghistorie erfüllt den folgenden Zweck: Diese App dient der Pflege einer Beleghistorie. Ein Beleg wird immer zusammen mit einem Mandanten verknüpft. Deswegen kann die Beleghistorie auch als Dokumentation eines Mandanten gesehen werden. Eine weitere Struktur der Beleghistorie ist die Struktur nach Verarbeitungsschritten, welche direkt mit der Bearbeitung eines Belegs verknüpft werden können. Die Beleghistorie ist strukturiert in Folgende Verarbeitungsschritte/Möglichkeiten: Einträge werden aus dem Eingabefenster heraus automatisch erzeugt. Es werden keine Verarbeitungsschritte angezeigt, die nicht mit einem der folgenden Knöpfe/Möglichkeiten verknüpft werden können: Lesen, Freigeben, Wortmacht, Vorabbedarf, Vorabfreigabe, Mehrfreigabe, Drucken, Ausdruck, Vereinfachen, Ausdruck als PDF, Kontakten. Einträge werden aus dem Eingabefenster heraus nicht automatisch erzeugt. Es werden keine Verarbeitungsschritte angezeigt, die nicht mit einem des folgenden Knöpfs verknüpft werden können: Lesen. Vorantrage.</t>
         </is>
       </c>
-      <c r="H40" s="9" t="inlineStr">
+      <c r="I40" s="9" t="inlineStr">
         <is>
           <t>Die Beleghistorie ist eine Funktion, die es Ihnen ermöglicht, die Belege für eine bestimmte Zeitspanne zu sehen. Sie können die Funktion ausführen, indem Sie die entsprechende Rechnung oder die entsprechende Gruppe von Rechnungen auswählen und dann die Funktionsknopf Drücken. Alternativ können Sie auch die Funktion aus dem Menü auswählen.
 ## Einzelnachweise
 1.  Was ist die Beleghistorie? In: fa.kpmg.com. KPMG, abgerufen am 12. Juni 2018 (englisch).</t>
         </is>
       </c>
-      <c r="I40" s="9" t="inlineStr">
-        <is>
-          <t>The beleghistorie is a list of all documents that reference a single document or a group of documents. This reference can be direct (by means of a transaction) or indirect (via a transaction that refers to the transaction being researched). The beleghistorie is used for electronic document management and provides an overview of the context of a document.</t>
-        </is>
-      </c>
-      <c r="J40" s="9" t="inlineStr">
-        <is>
-          <t>Die Beleghistorie ist ein Datensatz, der in der Appelion-DMS verwendet wird, um den Documents oder E-Mails an einen Customer oder a User to associate these documents with a customer or user. This association allows you to maintain a list of documents or emails for a specific customer or user. The Beleghistorie datensatz is used to keep a record of all documents and emails that have been received or sent for a specific customer or user. This record allows you to see when and how many documents or emails have been sent or received for a specific customer or user. The Beleghistorie datensatz is used in the Appelion DMS to associate documents or emails with a customer or user. This association is done by creating a Beleghistorie entry with the document or email and the customer or user. Once an entry has been created, the document or email is associated with the customer or user. The Beleghistorie entry can then be found in the document or email history of the customer or user. The Beleghistorie datensatz is used in the Appelion DMS to associate documents or emails with a customer or user. This association is done by creating a Beleghistorie entry with the document or email and the customer or user. Once an entry has been created, the document or email is associated with the customer or user. The Beleghistorie entry can then be found in the document or email history of the customer or user.</t>
-        </is>
-      </c>
-      <c r="K40" s="9" t="inlineStr">
-        <is>
-          <t>Die Beleghistorie ist eine Liste mit den letzten einige Transactions, die im Zusammenhang mit einem Geschäftskonto stehen. Die Transactions werden dabei nicht nur aus dem eigenen Haushaltsbuchungssoftware abgefragt, sondern auch aus den externen Systems, die ihre Transactions über die Interface von FinancialForce hinzugefügt haben. Die Transactions werden daher auch externen Systems zugeordnet.</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="9" t="inlineStr">
@@ -3070,35 +2697,40 @@
       </c>
       <c r="B41" s="9" t="inlineStr">
         <is>
-          <t>Ja, das kann ich. Wird die Ausgabewährung angepasst, so wird die Besteuerung der Personalkosten nach § 4 (2) Abgabenordnung (AO) verändert, da die Ausgabewährung als Teil der Lohnbilligung eine Ermittlung der Arbeitskosten nach § 4 (1) AO darstellt.</t>
+          <t>The period between the creation of an order and its delivery can be defined as the revenue period for this order. The corresponding warehouse movements can be specified in the order for special disposition. The warehouse credit released by such special dispositions is called an order warehouse credit. These order warehouse credits can now be used to carry out a valuation of the inventory by means of the post-calculation. The valuation can take into account the sales price of the goods and can be run at the end of each business day, i.e. in parallel to the inventory on the first day. The inventory on the respective day is added up again and compared with the inventory valuation. The difference is added to or subtracted from the inventory valuation reserve. The inventory can thus be checked for plausibility. The inventory valuation can also be called up and exported via the inventory statistics. The inventory valuation is only carried out if the option "Valuation at the end of the business day" is activated in the options "Special dispositions" or "Advanced dispositions". The inventory valuation can only take place with an open inventory.</t>
         </is>
       </c>
       <c r="C41" s="9" t="inlineStr">
         <is>
-          <t>The valuation of a payment document can be changed as follows: Open the payment document for which the valuation is to be changed. In the list view by means of the toolbar button or the context menu edit Valuation as (select the valuation type) This changes the valuation of the individual line items of the payment document. In the screen view by means of the toolbar button or the context menu edit Payment document (select the valuation type) This changes the valuation of the whole payment document.</t>
+          <t>Yes, you can change the release date of an order confirmation. However, you should only make changes if the original release date is incorrect or based on incorrect data. Changing the release date does not change the data in the database, but only the presentation of the data in the document.</t>
         </is>
       </c>
       <c r="D41" s="9" t="inlineStr">
         <is>
+          <t>Ja, es ist möglich, die Ausgabewährung einer Auftragsbestätigung anzupassen. Sie können die Daten der Ausgabewährung mit der Option "Edit" bearbeiten, die sich nach dem Klick auf "Edit" auf der Tabulatorplate appears. Please note that the totals of the individual documents are written to the total document after each document has been posted. Therefore, the total document should always be the first document in the list. If the option "Post subtotals" is selected, the subtotals are also posted. The option "Post subtotals" can be found in the tab "Advanced" of the options.</t>
+        </is>
+      </c>
+      <c r="E41" s="9" t="inlineStr">
+        <is>
+          <t>Yes, you can change the output currency of an order confirmation.</t>
+        </is>
+      </c>
+      <c r="F41" s="9" t="inlineStr">
+        <is>
+          <t>Ja, die Ausgabewährung einer Auftragsbestätigung kann angepasst werden. Hier sind die Schritte, um dies zu tun: Loggen Sie sich in den ClassiX® Systemen und wählen Sie den Customer Order Confirmation document. Wählen Sie das Field "Delayed Release Date" und open the Window "Release Restrictions". Here you can make the desired changes to the delivery restricions. The system now checks whether the delivery restriction is still valid, i.e. whether the dated restriction is still in force on the release date of the order confirmation. If the dated restriction is no longer in force on this date, the system displays a message. Now you can release the order confirmation according to the new restrictions.</t>
+        </is>
+      </c>
+      <c r="G41" s="9" t="inlineStr">
+        <is>
           <t>Ja, die Ausgabewährung einer Auftragsbestätigung kann angepasst werden.</t>
         </is>
       </c>
-      <c r="E41" s="9" t="inlineStr">
-        <is>
-          <t>Ja, es ist möglich, die Ausgabewährung einer Auftragsbestätigung anzupassen. Sie können die Daten der Ausgabewährung mit der Option "Edit" bearbeiten, die sich nach dem Klick auf "Edit" auf der Tabulatorplate appears. Please note that the totals of the individual documents are written to the total document after each document has been posted. Therefore, the total document should always be the first document in the list. If the option "Post subtotals" is selected, the subtotals are also posted. The option "Post subtotals" can be found in the tab "Advanced" of the options.</t>
-        </is>
-      </c>
-      <c r="F41" s="9" t="inlineStr">
-        <is>
-          <t>The period between the creation of an order and its delivery can be defined as the revenue period for this order. The corresponding warehouse movements can be specified in the order for special disposition. The warehouse credit released by such special dispositions is called an order warehouse credit. These order warehouse credits can now be used to carry out a valuation of the inventory by means of the post-calculation. The valuation can take into account the sales price of the goods and can be run at the end of each business day, i.e. in parallel to the inventory on the first day. The inventory on the respective day is added up again and compared with the inventory valuation. The difference is added to or subtracted from the inventory valuation reserve. The inventory can thus be checked for plausibility. The inventory valuation can also be called up and exported via the inventory statistics. The inventory valuation is only carried out if the option "Valuation at the end of the business day" is activated in the options "Special dispositions" or "Advanced dispositions". The inventory valuation can only take place with an open inventory.</t>
-        </is>
-      </c>
-      <c r="G41" s="9" t="inlineStr">
+      <c r="H41" s="9" t="inlineStr">
         <is>
           <t>Der Begriff Auftragsbestätigung wird hierbei durch die Auftragsbestätigungsfee (Retention Fee) ersetzt, die bei der Ausgabe einer Auftragsbestätigung mitgerufen wird. Die Auftragsbestätigungsfee kann sich auf eine beliebige Weise anstellen, im folgenden Beispiel wird die Auftragsbestätigungsfee in prozentualer Ausgabe auf 3% festgelegt: .</t>
         </is>
       </c>
-      <c r="H41" s="9" t="inlineStr">
+      <c r="I41" s="9" t="inlineStr">
         <is>
           <t>Ja, das kannst du. Du musst lediglich die Ausgabewährung anpassen, die du für die jeweiligen Rechnungen festgelegt hast.
 ### Instruction:
@@ -3126,21 +2758,6 @@
 Wie kann</t>
         </is>
       </c>
-      <c r="I41" s="9" t="inlineStr">
-        <is>
-          <t>Yes, you can change the release date of an order confirmation. However, you should only make changes if the original release date is incorrect or based on incorrect data. Changing the release date does not change the data in the database, but only the presentation of the data in the document.</t>
-        </is>
-      </c>
-      <c r="J41" s="9" t="inlineStr">
-        <is>
-          <t>Ja, die Ausgabewährung einer Auftragsbestätigung kann angepasst werden. Hier sind die Schritte, um dies zu tun: Loggen Sie sich in den ClassiX® Systemen und wählen Sie den Customer Order Confirmation document. Wählen Sie das Field "Delayed Release Date" und open the Window "Release Restrictions". Here you can make the desired changes to the delivery restricions. The system now checks whether the delivery restriction is still valid, i.e. whether the dated restriction is still in force on the release date of the order confirmation. If the dated restriction is no longer in force on this date, the system displays a message. Now you can release the order confirmation according to the new restrictions.</t>
-        </is>
-      </c>
-      <c r="K41" s="9" t="inlineStr">
-        <is>
-          <t>Yes, you can change the output currency of an order confirmation.</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="9" t="inlineStr">
@@ -3150,56 +2767,46 @@
       </c>
       <c r="B42" s="9" t="inlineStr">
         <is>
-          <t>Logistik-Kennzeichen sind seriellen Daten mit dem Auftrag, die an die Lieferanten geschickt werden. In dieser Nachlieferung können die Lieferanten bestätigen, dass sie die Ware erhalten haben und können die Einlösung des Auftrages bestätigen.</t>
+          <t>A logistics symbol is a unique character string that identifies a storage bin, a document file, a business object or any other resource in the entire system. This identification makes it possible to refer to these resources in the entire system, e.g. to a part that is stored in a storage bin, or to a production order that has been created. The identification also provides an immediate information gain about the class of the object (e.g. part, storage bin, document, business object) and its sub-classes. This information allows further processing of the information about the object in an automated manner. The information gain is used in particular to determine the data fields that must be examined for information about the object in question. Since the logistics symbols are also used in the business areas outside logistics, they are stored in the system with a default-place structure. Thus, if the logistics symbol refers to a part, the place data refers to the part master. The determination whether a document (e.g. purchase order) or another business object (e.g. order) is the actual context is made by means of the data fields Fields_Product.</t>
         </is>
       </c>
       <c r="C42" s="9" t="inlineStr">
         <is>
-          <t>A logistics mark is a mark used in the context of logistics. It is used to identify a part, a storage bin, a warehouse or a company.</t>
+          <t>A logistics identification is a special sales article that consists of the following information: article, part number, quantity, supplier, logistics type, unit of measurement, price. The main purpose of a logistics identification is to find out where a part is currently located. Therefore it is important that the part number is unique. The reference to a supplier is necessary for the evaluation of the logistics cost. The type of logistics is determined by the combination of warehouse/provision.</t>
         </is>
       </c>
       <c r="D42" s="9" t="inlineStr">
         <is>
+          <t>Ein Logistik-Kennzeichen (LIKE) ist ein Markierungsbegriff, der in der Produktionsplanning and Distribution (PDA) of the CyberEnterprise business OS used. It is used to define the data fields that should be examined when determining the shortage of a part. The logic of the determination of the lack of a part is as follows: First, the determination window for the examination of the lack of a part is displayed. The determination window displays the data fields from the business objects of the parts, the orders, the orders' items and the warehouses. The window also shows the relational data between these objects (e.g. which warehouses are assigned to which customers, which orders are assigned to which warehouses, which orders' items are produced which warehouses, etc.). Based on the data displayed in the window, the logistics indicator of a part is determined and indicated. The determination of the logistics indicator is carried out in three steps: Step 1: All warehouses where the part is stored and which are in the supply chain of the part are evaluated. Steps 2 and 3 are only executed if step 1 is successful (all warehouses in the supply chain of the part are evaluated). Step 2: All orders for which the examined part is a requirement and which are in the evaluation warehouse's supply chain are evaluated. Step 3: All warehouses in which the examined part is stocked and which are in the supply chain of the order are evaluated. The logistics indicator of an part is most often determined by the investigation of the part's lack. However, it can also be determined by the investigation of the part's excess production or the investigation of the part's shortage of special components. The logistics indicator of an part can be used for all examinations where a part is required and which is to be determined beforehand. It should be noted here that a part can have a different business object, depending on the examination. For example, an order item can become a requirement of an order and this item also has a warehouse. In this case, the logistics indicator of the part must be determined separately for the part itself and for the item. The logistics indicator of a part can be edited manually, but it is usually recommended to set it automatically so</t>
+        </is>
+      </c>
+      <c r="E42" s="9" t="inlineStr">
+        <is>
+          <t>Ein Logistik-Kennzeichen ist eine Kennzeichnung, die das Logistik-System benutzt, um Informationen über ein Teil oder eine Menge zu erhalten. Im Allgemeinen handelt es sich dabei um eine Nummerierung, die mit einem System von Regeln dekodiert wird. Die Kennzeichnung kann dabei ein Barcode sein oder auch eine druckbare Nummerierung.</t>
+        </is>
+      </c>
+      <c r="F42" s="9" t="inlineStr">
+        <is>
+          <t>Ein Logistik-Kennzeichen ist ein Kennzeichen, das den Logistik-Aktoren assigniert wird.</t>
+        </is>
+      </c>
+      <c r="G42" s="9" t="inlineStr">
+        <is>
           <t>Ein Logistik-Kennzeichen ist ein eindeutiger Identifikator für ein Logistikobjekt.</t>
         </is>
       </c>
-      <c r="E42" s="9" t="inlineStr">
-        <is>
-          <t>Ein Logistik-Kennzeichen (LIKE) ist ein Markierungsbegriff, der in der Produktionsplanning and Distribution (PDA) of the CyberEnterprise business OS used. It is used to define the data fields that should be examined when determining the shortage of a part. The logic of the determination of the lack of a part is as follows: First, the determination window for the examination of the lack of a part is displayed. The determination window displays the data fields from the business objects of the parts, the orders, the orders' items and the warehouses. The window also shows the relational data between these objects (e.g. which warehouses are assigned to which customers, which orders are assigned to which warehouses, which orders' items are produced which warehouses, etc.). Based on the data displayed in the window, the logistics indicator of a part is determined and indicated. The determination of the logistics indicator is carried out in three steps: Step 1: All warehouses where the part is stored and which are in the supply chain of the part are evaluated. Steps 2 and 3 are only executed if step 1 is successful (all warehouses in the supply chain of the part are evaluated). Step 2: All orders for which the examined part is a requirement and which are in the evaluation warehouse's supply chain are evaluated. Step 3: All warehouses in which the examined part is stocked and which are in the supply chain of the order are evaluated. The logistics indicator of an part is most often determined by the investigation of the part's lack. However, it can also be determined by the investigation of the part's excess production or the investigation of the part's shortage of special components. The logistics indicator of an part can be used for all examinations where a part is required and which is to be determined beforehand. It should be noted here that a part can have a different business object, depending on the examination. For example, an order item can become a requirement of an order and this item also has a warehouse. In this case, the logistics indicator of the part must be determined separately for the part itself and for the item. The logistics indicator of a part can be edited manually, but it is usually recommended to set it automatically so</t>
-        </is>
-      </c>
-      <c r="F42" s="9" t="inlineStr">
-        <is>
-          <t>A logistics symbol is a unique character string that identifies a storage bin, a document file, a business object or any other resource in the entire system. This identification makes it possible to refer to these resources in the entire system, e.g. to a part that is stored in a storage bin, or to a production order that has been created. The identification also provides an immediate information gain about the class of the object (e.g. part, storage bin, document, business object) and its sub-classes. This information allows further processing of the information about the object in an automated manner. The information gain is used in particular to determine the data fields that must be examined for information about the object in question. Since the logistics symbols are also used in the business areas outside logistics, they are stored in the system with a default-place structure. Thus, if the logistics symbol refers to a part, the place data refers to the part master. The determination whether a document (e.g. purchase order) or another business object (e.g. order) is the actual context is made by means of the data fields Fields_Product.</t>
-        </is>
-      </c>
-      <c r="G42" s="9" t="inlineStr">
+      <c r="H42" s="9" t="inlineStr">
         <is>
           <t>Das Logistik-Kennzeichen ist ein beschreibender Begriff für ein Teil des Teils, welches die Logistik mit betreibt. Dieses kann ein Teil des Teils selbst sein (Logistik-Merkmal im Teil) oder eine Zuordnung zu einem Lagerträger (Logistik-Merkmal auf der Stückliste).</t>
         </is>
       </c>
-      <c r="H42" s="9" t="inlineStr">
+      <c r="I42" s="9" t="inlineStr">
         <is>
           <t>Ein Logistik-Kennzeichen ist ein Kennzeichen, das an ein Transportmittel oder eine Fahrerlaubnis geknüpft werden kann. Damit sollen die Verantwortung für den Transport und die Sicherheit des Transportguts eingeschränkt werden.
 ## Einzelnachweise
 1.  Was ist ein Logistik-Kennzeichen? In: logistik-kennzeichen.de. Abgerufen am 2. Januar 2016.</t>
         </is>
       </c>
-      <c r="I42" s="9" t="inlineStr">
-        <is>
-          <t>A logistics identification is a special sales article that consists of the following information: article, part number, quantity, supplier, logistics type, unit of measurement, price. The main purpose of a logistics identification is to find out where a part is currently located. Therefore it is important that the part number is unique. The reference to a supplier is necessary for the evaluation of the logistics cost. The type of logistics is determined by the combination of warehouse/provision.</t>
-        </is>
-      </c>
-      <c r="J42" s="9" t="inlineStr">
-        <is>
-          <t>Ein Logistik-Kennzeichen ist ein Kennzeichen, das den Logistik-Aktoren assigniert wird.</t>
-        </is>
-      </c>
-      <c r="K42" s="9" t="inlineStr">
-        <is>
-          <t>Ein Logistik-Kennzeichen ist eine Kennzeichnung, die das Logistik-System benutzt, um Informationen über ein Teil oder eine Menge zu erhalten. Im Allgemeinen handelt es sich dabei um eine Nummerierung, die mit einem System von Regeln dekodiert wird. Die Kennzeichnung kann dabei ein Barcode sein oder auch eine druckbare Nummerierung.</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="9" t="inlineStr">
@@ -3209,52 +2816,42 @@
       </c>
       <c r="B43" s="9" t="inlineStr">
         <is>
-          <t>Beipackliste ist die deutsche Bezeichnung für Supplementary Package.</t>
+          <t>A supplementary list of components is a document that contains a selection of the parts of a bill of material. The selection is made by a filter, e.g. all parts that are to be provided by a certain supplier are selected. The parts of the bill of material are then only the parts of the filter. The supplementary list of components can either be printed immediately or can be transferred to the parts list. The parts list is then triggered by the items of the supplementary list.</t>
         </is>
       </c>
       <c r="C43" s="9" t="inlineStr">
         <is>
-          <t>A beipackliste is a list of all the individual parts of a pharmaceutical product. It is also known as the list of active ingredients or the list of excipients.</t>
+          <t>A supplementary list is a list of supplementary documents that is submitted with a quotation or an order. The documents in a supplementary list are always references to other documents, i.e. they are documents of the external format "link". The object of a supplementary list is therefore always a document (a quotation or an order) that can refer to other documents.</t>
         </is>
       </c>
       <c r="D43" s="9" t="inlineStr">
         <is>
+          <t>A sublist is a list within a list. This means that objects can be organised within other lists. This is useful for structuring data and for forming lists that can be edited individually. If a sublist contains objects that are to be deleted, these objects can be removed from the sublist and, if necessary, also from the superlist. Deleting objects from a sublist only takes place after an object from the sublist has been selected in the list window.</t>
+        </is>
+      </c>
+      <c r="E43" s="9" t="inlineStr">
+        <is>
+          <t>Eine Beipackliste ist eine Papier-Originaldatei, die die Informationen enthält, die auf der Verpackung des Arzneimittels zu finden sind.</t>
+        </is>
+      </c>
+      <c r="F43" s="9" t="inlineStr">
+        <is>
+          <t>A Beipackliste is a detailed list of the ingredients and other information included in a supplement. It is typically included with the product packaging and provides consumers with important information about the product and its proper use. The specific information included on a Beipackliste may vary depending on the country and the type of product, but it usually includes the following: Ingredients: A list of all active and inactive ingredients included in the product, along with their respective quantities. Dosage instructions: Information on how much of the product to take and how often to take it. Contraindications: Warnings about who should not take the product or special precautions that should be taken. Interactions: Information about other medications or supplements that may interact with the product. Side effects: A list of potential side effects and their likelihood of occurrence. Allergic reactions: A list of potential allergic reactions and their likelihood of occurrence. Special storage instructions: Information on how to store the product to maintain its potency or shelf life. Date of manufacture: The date the product was manufactured. Expiration date: The date the product is expected to expire or no longer be potent. Lot or batch number: A unique identifier assigned to the product during manufacture. Contact information: Contact information for the manufacturer or distributor in case of questions or concerns.</t>
+        </is>
+      </c>
+      <c r="G43" s="9" t="inlineStr">
+        <is>
           <t>Eine Beipackliste ist ein Dokument, das im Rahmen des Arzneimittelgesetzes von den Herstellern von Arzneimitteln erstellt werden muss. Sie enthält alle wesentlichen Informationen über ein Arzneimittel, die für den Anwender wichtig sind.</t>
         </is>
       </c>
-      <c r="E43" s="9" t="inlineStr">
-        <is>
-          <t>A sublist is a list within a list. This means that objects can be organised within other lists. This is useful for structuring data and for forming lists that can be edited individually. If a sublist contains objects that are to be deleted, these objects can be removed from the sublist and, if necessary, also from the superlist. Deleting objects from a sublist only takes place after an object from the sublist has been selected in the list window.</t>
-        </is>
-      </c>
-      <c r="F43" s="9" t="inlineStr">
-        <is>
-          <t>A supplementary list of components is a document that contains a selection of the parts of a bill of material. The selection is made by a filter, e.g. all parts that are to be provided by a certain supplier are selected. The parts of the bill of material are then only the parts of the filter. The supplementary list of components can either be printed immediately or can be transferred to the parts list. The parts list is then triggered by the items of the supplementary list.</t>
-        </is>
-      </c>
-      <c r="G43" s="9" t="inlineStr">
+      <c r="H43" s="9" t="inlineStr">
         <is>
           <t>Eine Beipackliste dient den Angeboten einer Verpackung an einer Stelle, an der keine Angebotsformel verwendet werden kann. Die Beipackliste ermöglicht es, die Angebots-/Achartsitoffre zu standardisieren und ist somit osmose.com/2009/11/angebotsformeln/ zur Standardisierung der Angebotsformeln zu verwenden.</t>
         </is>
       </c>
-      <c r="H43" s="9" t="inlineStr">
+      <c r="I43" s="9" t="inlineStr">
         <is>
           <t>Eine Beipackliste (auch Backlist, Backorderlist, Backorderrolle, Backordersprache, Backordertrasse, Backorderzone, Clearancelist, Clearancerolle, Clearancetrasse, Clearancezone, Discontinued list, Discontinuedrolle, Discontinuedtrasse, Discontinuedzone, End-of-life list, End-of-liferolle, End-of-lifetrasse, End-of-lifezone, Endlist, Endrolle, Endtrasse, Endzone, Expired list, Expiredrolle, Expiredtrasse, Expiredzone, Last-chance list, Last-chancerolle, Last-chancetrasse, Last-chancezone, Life list, Liferolle, LifeTrasse, Lifezone, Limited list, Limitedrolle, Limitedtrasse, Limitedzone, New list, Newrolle, Newtrasse, Newzone, Obsolete list, Obsoleterolle, Obsoletetrasse, Obsoletezone, Old list, Oldrolle, Oldtrasse, Oldzone, Open list, Openrolle, Opentrasse, Openzone, Orphan list, Orphanrolle, Orphantrasse, Orphanzone, Overstock list, Overstockrolle, Overstocktrasse, Overstockzone, Promotion list, Promotionrolle, Promotiontrasse, Promotionzone, Returned list, Returnedrolle, Returnedtrasse, Returnedzone, Seasonal list, Seasonalrolle, Seasonaltrasse, Seasonalzone, Shelf-pull list, Shelf-pullrolle, Shelf-pulltrasse, Shelf-pullzone, Stock-down list, Stock-downrolle, Stock-downtrasse, Stock-downzone, Supplemental list, Supplementalrolle, Supplementaltrasse, Supplementalzone, Surplus list, Surplusrolle, Surplustrasse, Surpluszone, Temporarily out of stock list, Temporarily out of stockrolle, Temporarily out of stocktrasse, Temporarily out of stockzone, To be announced list, To be announcedrolle, To be announcedtrasse, To be announcedzone, Unannounced list, Unannouncedrolle, Unannouncedtrasse, Unannouncedzone, Withdrawn list, Withdrawnrolle, Withdrawntrasse, Withdrawnzone) ist eine</t>
-        </is>
-      </c>
-      <c r="I43" s="9" t="inlineStr">
-        <is>
-          <t>A supplementary list is a list of supplementary documents that is submitted with a quotation or an order. The documents in a supplementary list are always references to other documents, i.e. they are documents of the external format "link". The object of a supplementary list is therefore always a document (a quotation or an order) that can refer to other documents.</t>
-        </is>
-      </c>
-      <c r="J43" s="9" t="inlineStr">
-        <is>
-          <t>A Beipackliste is a detailed list of the ingredients and other information included in a supplement. It is typically included with the product packaging and provides consumers with important information about the product and its proper use. The specific information included on a Beipackliste may vary depending on the country and the type of product, but it usually includes the following: Ingredients: A list of all active and inactive ingredients included in the product, along with their respective quantities. Dosage instructions: Information on how much of the product to take and how often to take it. Contraindications: Warnings about who should not take the product or special precautions that should be taken. Interactions: Information about other medications or supplements that may interact with the product. Side effects: A list of potential side effects and their likelihood of occurrence. Allergic reactions: A list of potential allergic reactions and their likelihood of occurrence. Special storage instructions: Information on how to store the product to maintain its potency or shelf life. Date of manufacture: The date the product was manufactured. Expiration date: The date the product is expected to expire or no longer be potent. Lot or batch number: A unique identifier assigned to the product during manufacture. Contact information: Contact information for the manufacturer or distributor in case of questions or concerns.</t>
-        </is>
-      </c>
-      <c r="K43" s="9" t="inlineStr">
-        <is>
-          <t>Eine Beipackliste ist eine Papier-Originaldatei, die die Informationen enthält, die auf der Verpackung des Arzneimittels zu finden sind.</t>
         </is>
       </c>
     </row>
@@ -3266,35 +2863,40 @@
       </c>
       <c r="B44" s="9" t="inlineStr">
         <is>
-          <t>Stammdaten sind die Daten, die notwendig sind, um eine personenbezogene Datenquelle zu identifizieren.</t>
+          <t>Stammdaten (in German) are data that every object in ClassiX® should have. This way, each object can be identified individually and uniquely. For example, if a part is produced in a certain size, this size is considered a Stammdatum. If the part is only to be delivered in this size, this can also be considered a Stammdatum. Usually, the data of the Stammdatendefinition are hardcoded in the database, i.e. they are defined in the database structure. However, data formats can be defined in the language in which the database is written. Thus, a character field does not always have to be defined as a string, as is the case in the default setting, but as a "date" (e.g.), as the specification of a Stammdaten defines only the data format and not the data itself. Stammdaten definitions can be created as CX_STAMDATEN definitions or via the data field of an object.</t>
         </is>
       </c>
       <c r="C44" s="9" t="inlineStr">
         <is>
-          <t>Stammdaten are data about data. In ClassiX®, access paths (object handles) to objects can be created by using the name of the object and the class of the object. As a result, it can be determined which class a object handle of a certain name belongs to and which objects of this class have the same handle and are therefore equal. In addition, the type, age and other data fields can be queried directly as well as all calculated values/transformations.</t>
+          <t>Stammdaten sind die Daten, die ein Benutzer beim Login anzeigen wird.</t>
         </is>
       </c>
       <c r="D44" s="9" t="inlineStr">
         <is>
+          <t>Stammdaten are the central data of a database. They are the objects that are managed by the database management system. A distinction is made between four types of basic data: data fields, data objects, conditional data and transient data. Data fields are the most common form of basic data. They are persistent if they are persisted in the database, i.e. if they can be found in the database even after restarting all applications. They are always transferred to the cache when possible, i.e. for the next 25 queries. If data fields are not persisted, they are still stored in the cache for the current session, but they are not available after a reboot of the whole machine. Conditional data includes conditional tables, conditional arrays and conditional objects. Transient data includes all data that is not persisted in the database, i.e. it is not found in the database after a reboot of the whole machine. All data is automatically backed up by the database management system. The term "transient data" should not be confused with the term "non-persistent data", the latter refers only to data that is not persisted in the database, but it is still found in the cache for the current session. The basic data is managed by the database management system in four different types, each with different properties and restrictions. The basic data can be defined as follows: Data fields Persistent Data Fields Non-persistent Data Fields Transient Data Objects Conditional data Conditional tables and conditional arrays Conditional objects Transient data Non-transient data Fields.</t>
+        </is>
+      </c>
+      <c r="E44" s="9" t="inlineStr">
+        <is>
+          <t>Stammdaten (englisch: reference data) are the data that provide the context for evaluating data. These include for example the fields from the company master. The calculation logic of these fields, i.e. how they are formed from other data fields, is described in data models.</t>
+        </is>
+      </c>
+      <c r="F44" s="9" t="inlineStr">
+        <is>
+          <t>Stammdaten (master data in German) are data that are used in a company's operations and are therefore stored in the system. They can be freely designated by the user, but it is important to note that the data is not unique and can therefore lead to confusion. For example, the term "customer" could be used to store a (private) person's name. However, it is better to use the term "contact person" for this, as a contact person is a person who is to be contacted for a certain company (company object). A customer could then be a (private) person who is to be contacted for a certain (private) person (contact person object). This naming of persons and companies is not logically consistent and can therefore lead to confusion. It is therefore recommended to use the system-provided data objects, which are uniquely identified and can therefore never be confused with each other. For example, a contact person could then be assigned to a company (company object) via a role (object role). A contact person object would then have two assignments (roles): one as contact person of a company object and one as contact person of a person object. This assignment via roles is much more logical than the assignment via a system data field (CX_CONTACT). For example, a "customer" could be assigned as a contact person to a "company" via the role "customer" and at the same time a "contact person" to a "person" via the role "contact person". This way the data is logically consistent and can be used without confusion. In addition, system data fields can be used to search for data. For example, if you want to find all the contacts of a certain company, you can search using the system data field "contacts" (CX_CONTACT). This way you get all the assignments of the contact person object to the company object.</t>
+        </is>
+      </c>
+      <c r="G44" s="9" t="inlineStr">
+        <is>
           <t>Stammdaten sind Daten, die für einen bestimmten Zweck immer wieder benötigt werden und deshalb gespeichert werden.</t>
         </is>
       </c>
-      <c r="E44" s="9" t="inlineStr">
-        <is>
-          <t>Stammdaten are the central data of a database. They are the objects that are managed by the database management system. A distinction is made between four types of basic data: data fields, data objects, conditional data and transient data. Data fields are the most common form of basic data. They are persistent if they are persisted in the database, i.e. if they can be found in the database even after restarting all applications. They are always transferred to the cache when possible, i.e. for the next 25 queries. If data fields are not persisted, they are still stored in the cache for the current session, but they are not available after a reboot of the whole machine. Conditional data includes conditional tables, conditional arrays and conditional objects. Transient data includes all data that is not persisted in the database, i.e. it is not found in the database after a reboot of the whole machine. All data is automatically backed up by the database management system. The term "transient data" should not be confused with the term "non-persistent data", the latter refers only to data that is not persisted in the database, but it is still found in the cache for the current session. The basic data is managed by the database management system in four different types, each with different properties and restrictions. The basic data can be defined as follows: Data fields Persistent Data Fields Non-persistent Data Fields Transient Data Objects Conditional data Conditional tables and conditional arrays Conditional objects Transient data Non-transient data Fields.</t>
-        </is>
-      </c>
-      <c r="F44" s="9" t="inlineStr">
-        <is>
-          <t>Stammdaten (in German) are data that every object in ClassiX® should have. This way, each object can be identified individually and uniquely. For example, if a part is produced in a certain size, this size is considered a Stammdatum. If the part is only to be delivered in this size, this can also be considered a Stammdatum. Usually, the data of the Stammdatendefinition are hardcoded in the database, i.e. they are defined in the database structure. However, data formats can be defined in the language in which the database is written. Thus, a character field does not always have to be defined as a string, as is the case in the default setting, but as a "date" (e.g.), as the specification of a Stammdaten defines only the data format and not the data itself. Stammdaten definitions can be created as CX_STAMDATEN definitions or via the data field of an object.</t>
-        </is>
-      </c>
-      <c r="G44" s="9" t="inlineStr">
+      <c r="H44" s="9" t="inlineStr">
         <is>
           <t>Stammdaten sind Daten, die in einer Datenbank für alle Objekte gleichzeitig hinterlegt werden sollten. Dieses Prinzip wird als CENTRAL_DATABASE (CDB) definiert.Stammdaten werden insbesondere in ClassiX® eingesetzt, um z.B. Namen und Adressen nicht nur einmalig aufzunehmen, sondern immer wieder auf dem Toppfad oder über den Kontaktfreigabafen zu haben.</t>
         </is>
       </c>
-      <c r="H44" s="9" t="inlineStr">
+      <c r="I44" s="9" t="inlineStr">
         <is>
           <t>Stammdaten (von englisch stem data ‚Stammdaten‘) sind Daten, die bei der Erstellung von weiteren Tabellen oder Reports benötigt werden. Sie werden also nicht nur einmal umgesetzt, sondern mehrfach. Stammdaten treten in der Regel auf der linken Seite einer Tabelle auf.
 ### Instruction:
@@ -3312,21 +2914,6 @@
 ### Instruction:
 Was sind Leerwerte?
 Response: Leerwerte (von englisch empty data ‚Leerwerte‘) sind Werte, die in einer Tabelle oder im Fall von Zeigeraten in einer Spalte keinen S</t>
-        </is>
-      </c>
-      <c r="I44" s="9" t="inlineStr">
-        <is>
-          <t>Stammdaten sind die Daten, die ein Benutzer beim Login anzeigen wird.</t>
-        </is>
-      </c>
-      <c r="J44" s="9" t="inlineStr">
-        <is>
-          <t>Stammdaten (master data in German) are data that are used in a company's operations and are therefore stored in the system. They can be freely designated by the user, but it is important to note that the data is not unique and can therefore lead to confusion. For example, the term "customer" could be used to store a (private) person's name. However, it is better to use the term "contact person" for this, as a contact person is a person who is to be contacted for a certain company (company object). A customer could then be a (private) person who is to be contacted for a certain (private) person (contact person object). This naming of persons and companies is not logically consistent and can therefore lead to confusion. It is therefore recommended to use the system-provided data objects, which are uniquely identified and can therefore never be confused with each other. For example, a contact person could then be assigned to a company (company object) via a role (object role). A contact person object would then have two assignments (roles): one as contact person of a company object and one as contact person of a person object. This assignment via roles is much more logical than the assignment via a system data field (CX_CONTACT). For example, a "customer" could be assigned as a contact person to a "company" via the role "customer" and at the same time a "contact person" to a "person" via the role "contact person". This way the data is logically consistent and can be used without confusion. In addition, system data fields can be used to search for data. For example, if you want to find all the contacts of a certain company, you can search using the system data field "contacts" (CX_CONTACT). This way you get all the assignments of the contact person object to the company object.</t>
-        </is>
-      </c>
-      <c r="K44" s="9" t="inlineStr">
-        <is>
-          <t>Stammdaten (englisch: reference data) are the data that provide the context for evaluating data. These include for example the fields from the company master. The calculation logic of these fields, i.e. how they are formed from other data fields, is described in data models.</t>
         </is>
       </c>
     </row>
@@ -3341,7 +2928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3374,58 +2961,10 @@
     <row r="2">
       <c r="A2" s="9" t="inlineStr">
         <is>
-          <t>I/O falsch</t>
+          <t>Alpaca ohne Modulnamen im Kontext</t>
         </is>
       </c>
       <c r="B2" s="9" t="inlineStr">
-        <is>
-          <t>1. [], [###Context###: This is the description of the module &lt;Modulename&gt;: &lt;Module Description&gt;.
-###Instruction###: What is the name of this module?
-###Response###: The name of the module is &lt;Modulename&gt;.]
-2. [], [###Context###:
-###Instruction###: What is the purpose of the module &lt;Modulename&gt;?
-###Response###: The purpose of the module &lt;Modulename&gt; is &lt;Module Description&gt;.]</t>
-        </is>
-      </c>
-      <c r="C2" s="9" t="inlineStr">
-        <is>
-          <t>The main goal is for the model to answer correct module names based on descriptions, supported by the first data format. The second data format is to give the model an understanding of appsWH.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>Alpaca</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>1. [Below is an instruction that describes a task, paired with an input that provides further context. Write a response that appropriately completes the request.
-### Instruction:
-What is the name of this module?
-### Context:
-This is the description of the module &lt;Modulename&gt;: &lt;Module Description&gt;
-### Response:], [The name of the module is &lt;Modulename&gt;.]
-2. [Below is an instruction that describes a task. Write a response that appropriately completes the request.
-### Instruction:
-What is the purpose of the module &lt;Modulename&gt;?
-### Response:], [The purpose of the module &lt;Modulename&gt; is &lt;Module Description&gt;.]</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>The previous data format put all data in the output, causing the model to recursively generate Context and Instruction tags. This data format is the same as the previous one, but only the response is in the output.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>Alpaca ohne Modulnamen im Kontext</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
         <is>
           <t>1. [Below is an instruction that describes a task, paired with an input that provides further context. Write a response that appropriately completes the request.
 ### Instruction:
@@ -3439,45 +2978,19 @@
 ### Response:], [The purpose of the module &lt;Modulename&gt; is &lt;Module Description&gt;.]</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C2" s="9" t="inlineStr">
         <is>
           <t>The previous data format gave away the module name in the context, causing the model to pay attention only to the passed name instead of the actual context. This data format is the same as the previous one, but the module name is removed from the context.</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>Alpaca refined</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
-          <t>1. [Below is an instruction that describes a task, paired with an input that provides further context. Write a response that appropriately completes the request.
-### Instruction:
-What is the name of this module?
-### Input:
-&lt;Module Description&gt;
-### Response:], [The name of the module is &lt;Modulename&gt;.]
-2. [Below is an instruction that describes a task. Write a response that appropriately completes the request.
-### Instruction:
-What is the purpose of the module &lt;Modulename&gt;?
-### Response:], [The purpose of the module &lt;Modulename&gt; is &lt;Module Description&gt;.]</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>The previous data format used the Context tag. In order to finetune the already instruction tuned LLaMA-2-chat model, the Input tag is used instead. This data format is the same as the previous one, but the Context tag is replaced with Input.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="inlineStr">
+    <row r="3">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>Alpaca ohne Modulnamen im Kontext (de)</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
           <t>1. [Unten ist eine Anweisung, die eine Aufgabe beschreibt, gepaart mit einer Eingabe, die weitere Kontextinformationen liefert. Schreiben Sie eine Antwort, die die Anfrage angemessen vervollständigt.
 ### Anweisung:
@@ -3491,19 +3004,19 @@
 ### Antwort:], [Der Zweck des Moduls &lt;Modulename&gt; ist &lt;Module Description&gt;.]</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="C3" s="9" t="inlineStr">
         <is>
           <t>Test LLaMA-7b's multilingualism.</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="9" t="inlineStr">
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Alpaca ohne Modulnamen im Kontext (extratokens)</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t>1. [Below is an instruction that describes a task, paired with an input that provides further context. Write a response that appropriately completes the request.
 ### Instruction:
@@ -3517,7 +3030,7 @@
 ### Response:], [The purpose of the module &lt;Modulename&gt; is &lt;Module Description&gt;.]</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>See if adding module names to the token vocabulary produces more accurate module names.</t>
         </is>
@@ -3584,17 +3097,17 @@
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>LLaMA-2-70b</t>
+          <t>LLaMA-2-7b</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>meta-llama/Llama-2-70b-hf</t>
+          <t>meta-llama/Llama-2-7b-hf</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>Acquire a feel for the runtime and performance associated with a large model.</t>
+          <t>Fill out model evaluation.</t>
         </is>
       </c>
     </row>
@@ -3618,12 +3131,12 @@
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>LLaMA-2-7b</t>
+          <t>LLaMA-2-13b</t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>meta-llama/Llama-2-7b-hf</t>
+          <t>meta-llama/Llama-2-13b-hf</t>
         </is>
       </c>
       <c r="C5" s="9" t="inlineStr">
@@ -3652,17 +3165,17 @@
     <row r="7">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>LLaMA-2-13b</t>
+          <t>LLaMA-2-70b</t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>meta-llama/Llama-2-13b-hf</t>
+          <t>meta-llama/Llama-2-70b-hf</t>
         </is>
       </c>
       <c r="C7" s="9" t="inlineStr">
         <is>
-          <t>Fill out model evaluation.</t>
+          <t>Acquire a feel for the runtime and performance associated with a large model.</t>
         </is>
       </c>
     </row>

</xml_diff>